<commit_message>
Parameter "5" added for the transformGold powerup.
Former-commit-id: a4b8c50bfc7ad9332a115977191aa8f60dd76b6b
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Powerups.xlsx
+++ b/Docs/Content/HungryDragonContent_Powerups.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\dragon\client\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -323,9 +323,6 @@
     <t>transform_gold</t>
   </si>
   <si>
-    <t>tranformGold</t>
-  </si>
-  <si>
     <t>hp_down_drain_down</t>
   </si>
   <si>
@@ -1422,6 +1419,9 @@
   </si>
   <si>
     <t>TID_POWERUP_LOVEATTRACTION_DESC_SHORT</t>
+  </si>
+  <si>
+    <t>transformGold</t>
   </si>
 </sst>
 </file>
@@ -3157,8 +3157,8 @@
   </sheetPr>
   <dimension ref="A1:L118"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="E56" sqref="E56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3191,10 +3191,10 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F2" s="101" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="114" x14ac:dyDescent="0.25">
@@ -3232,7 +3232,7 @@
         <v>25</v>
       </c>
       <c r="L3" s="11" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -3246,26 +3246,26 @@
         <v>32</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E4" s="17">
         <v>10</v>
       </c>
       <c r="F4" s="17"/>
       <c r="G4" s="18" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H4" s="18" t="s">
         <v>33</v>
       </c>
       <c r="I4" s="19" t="s">
+        <v>312</v>
+      </c>
+      <c r="J4" s="20" t="s">
+        <v>180</v>
+      </c>
+      <c r="K4" s="20" t="s">
         <v>313</v>
-      </c>
-      <c r="J4" s="20" t="s">
-        <v>181</v>
-      </c>
-      <c r="K4" s="20" t="s">
-        <v>314</v>
       </c>
       <c r="L4" s="18">
         <v>0</v>
@@ -3282,26 +3282,26 @@
         <v>34</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E5" s="17">
         <v>5</v>
       </c>
       <c r="F5" s="17"/>
       <c r="G5" s="18" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H5" s="18" t="s">
         <v>5</v>
       </c>
       <c r="I5" s="19" t="s">
+        <v>314</v>
+      </c>
+      <c r="J5" s="20" t="s">
+        <v>194</v>
+      </c>
+      <c r="K5" s="20" t="s">
         <v>315</v>
-      </c>
-      <c r="J5" s="20" t="s">
-        <v>195</v>
-      </c>
-      <c r="K5" s="20" t="s">
-        <v>316</v>
       </c>
       <c r="L5" s="18">
         <v>0</v>
@@ -3318,26 +3318,26 @@
         <v>45</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E6" s="17">
         <v>10</v>
       </c>
       <c r="F6" s="17"/>
       <c r="G6" s="18" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H6" s="18" t="s">
         <v>46</v>
       </c>
       <c r="I6" s="19" t="s">
+        <v>316</v>
+      </c>
+      <c r="J6" s="20" t="s">
         <v>317</v>
       </c>
-      <c r="J6" s="20" t="s">
+      <c r="K6" s="20" t="s">
         <v>318</v>
-      </c>
-      <c r="K6" s="20" t="s">
-        <v>319</v>
       </c>
       <c r="L6" s="18">
         <v>0</v>
@@ -3354,26 +3354,26 @@
         <v>16</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E7" s="17">
         <v>10</v>
       </c>
       <c r="F7" s="17"/>
       <c r="G7" s="18" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H7" s="18" t="s">
         <v>44</v>
       </c>
       <c r="I7" s="19" t="s">
+        <v>319</v>
+      </c>
+      <c r="J7" s="20" t="s">
+        <v>171</v>
+      </c>
+      <c r="K7" s="20" t="s">
         <v>320</v>
-      </c>
-      <c r="J7" s="20" t="s">
-        <v>172</v>
-      </c>
-      <c r="K7" s="20" t="s">
-        <v>321</v>
       </c>
       <c r="L7" s="18">
         <v>0</v>
@@ -3384,32 +3384,32 @@
         <v>3</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>16</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E8" s="17">
         <v>50</v>
       </c>
       <c r="F8" s="17"/>
       <c r="G8" s="18" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H8" s="18" t="s">
         <v>44</v>
       </c>
       <c r="I8" s="19" t="s">
+        <v>321</v>
+      </c>
+      <c r="J8" s="20" t="s">
         <v>322</v>
       </c>
-      <c r="J8" s="20" t="s">
+      <c r="K8" s="20" t="s">
         <v>323</v>
-      </c>
-      <c r="K8" s="20" t="s">
-        <v>324</v>
       </c>
       <c r="L8" s="18">
         <v>0</v>
@@ -3426,26 +3426,26 @@
         <v>50</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E9" s="17">
         <v>10</v>
       </c>
       <c r="F9" s="17"/>
       <c r="G9" s="18" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H9" s="18" t="s">
         <v>44</v>
       </c>
       <c r="I9" s="19" t="s">
+        <v>324</v>
+      </c>
+      <c r="J9" s="20" t="s">
+        <v>168</v>
+      </c>
+      <c r="K9" s="20" t="s">
         <v>325</v>
-      </c>
-      <c r="J9" s="20" t="s">
-        <v>169</v>
-      </c>
-      <c r="K9" s="20" t="s">
-        <v>326</v>
       </c>
       <c r="L9" s="18">
         <v>0</v>
@@ -3462,26 +3462,26 @@
         <v>51</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E10" s="17">
         <v>10</v>
       </c>
       <c r="F10" s="17"/>
       <c r="G10" s="18" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H10" s="18" t="s">
         <v>46</v>
       </c>
       <c r="I10" s="19" t="s">
+        <v>326</v>
+      </c>
+      <c r="J10" s="20" t="s">
+        <v>191</v>
+      </c>
+      <c r="K10" s="20" t="s">
         <v>327</v>
-      </c>
-      <c r="J10" s="20" t="s">
-        <v>192</v>
-      </c>
-      <c r="K10" s="20" t="s">
-        <v>328</v>
       </c>
       <c r="L10" s="18">
         <v>0</v>
@@ -3498,7 +3498,7 @@
         <v>53</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E11" s="17" t="s">
         <v>54</v>
@@ -3507,19 +3507,19 @@
         <v>10</v>
       </c>
       <c r="G11" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H11" s="18" t="s">
         <v>29</v>
       </c>
       <c r="I11" s="19" t="s">
+        <v>328</v>
+      </c>
+      <c r="J11" s="20" t="s">
         <v>329</v>
       </c>
-      <c r="J11" s="20" t="s">
+      <c r="K11" s="20" t="s">
         <v>330</v>
-      </c>
-      <c r="K11" s="20" t="s">
-        <v>331</v>
       </c>
       <c r="L11" s="18">
         <v>0</v>
@@ -3536,7 +3536,7 @@
         <v>53</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E12" s="17" t="s">
         <v>28</v>
@@ -3545,19 +3545,19 @@
         <v>10</v>
       </c>
       <c r="G12" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H12" s="18" t="s">
         <v>29</v>
       </c>
       <c r="I12" s="19" t="s">
+        <v>331</v>
+      </c>
+      <c r="J12" s="20" t="s">
+        <v>186</v>
+      </c>
+      <c r="K12" s="20" t="s">
         <v>332</v>
-      </c>
-      <c r="J12" s="20" t="s">
-        <v>187</v>
-      </c>
-      <c r="K12" s="20" t="s">
-        <v>333</v>
       </c>
       <c r="L12" s="18">
         <v>0</v>
@@ -3574,7 +3574,7 @@
         <v>53</v>
       </c>
       <c r="D13" s="22" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E13" s="23" t="s">
         <v>31</v>
@@ -3583,19 +3583,19 @@
         <v>10</v>
       </c>
       <c r="G13" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H13" s="18" t="s">
         <v>29</v>
       </c>
       <c r="I13" s="19" t="s">
+        <v>333</v>
+      </c>
+      <c r="J13" s="20" t="s">
         <v>334</v>
       </c>
-      <c r="J13" s="20" t="s">
+      <c r="K13" s="20" t="s">
         <v>335</v>
-      </c>
-      <c r="K13" s="20" t="s">
-        <v>336</v>
       </c>
       <c r="L13" s="18">
         <v>0</v>
@@ -3612,26 +3612,26 @@
         <v>12</v>
       </c>
       <c r="D14" s="26" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E14" s="27">
         <v>5</v>
       </c>
       <c r="F14" s="27"/>
       <c r="G14" s="28" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H14" s="18" t="s">
         <v>5</v>
       </c>
       <c r="I14" s="19" t="s">
+        <v>336</v>
+      </c>
+      <c r="J14" s="20" t="s">
+        <v>189</v>
+      </c>
+      <c r="K14" s="29" t="s">
         <v>337</v>
-      </c>
-      <c r="J14" s="20" t="s">
-        <v>190</v>
-      </c>
-      <c r="K14" s="29" t="s">
-        <v>338</v>
       </c>
       <c r="L14" s="18">
         <v>0</v>
@@ -3648,26 +3648,26 @@
         <v>18</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E15" s="17">
         <v>-50</v>
       </c>
       <c r="F15" s="17"/>
       <c r="G15" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H15" s="18" t="s">
         <v>29</v>
       </c>
       <c r="I15" s="19" t="s">
+        <v>338</v>
+      </c>
+      <c r="J15" s="20" t="s">
         <v>339</v>
       </c>
-      <c r="J15" s="20" t="s">
+      <c r="K15" s="20" t="s">
         <v>340</v>
-      </c>
-      <c r="K15" s="20" t="s">
-        <v>341</v>
       </c>
       <c r="L15" s="18">
         <v>0</v>
@@ -3684,26 +3684,26 @@
         <v>57</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E16" s="17">
         <v>20</v>
       </c>
       <c r="F16" s="17"/>
       <c r="G16" s="18" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H16" s="18" t="s">
         <v>5</v>
       </c>
       <c r="I16" s="19" t="s">
+        <v>341</v>
+      </c>
+      <c r="J16" s="20" t="s">
         <v>342</v>
       </c>
-      <c r="J16" s="20" t="s">
+      <c r="K16" s="20" t="s">
         <v>343</v>
-      </c>
-      <c r="K16" s="20" t="s">
-        <v>344</v>
       </c>
       <c r="L16" s="18">
         <v>0</v>
@@ -3714,32 +3714,32 @@
         <v>3</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>57</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E17" s="17">
         <v>-10</v>
       </c>
       <c r="F17" s="17"/>
       <c r="G17" s="18" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H17" s="18" t="s">
         <v>5</v>
       </c>
       <c r="I17" s="19" t="s">
+        <v>344</v>
+      </c>
+      <c r="J17" s="20" t="s">
         <v>345</v>
       </c>
-      <c r="J17" s="20" t="s">
+      <c r="K17" s="20" t="s">
         <v>346</v>
-      </c>
-      <c r="K17" s="20" t="s">
-        <v>347</v>
       </c>
       <c r="L17" s="18">
         <v>0</v>
@@ -3756,26 +3756,26 @@
         <v>58</v>
       </c>
       <c r="D18" s="22" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E18" s="23">
         <v>10</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="18" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H18" s="18" t="s">
         <v>33</v>
       </c>
       <c r="I18" s="19" t="s">
+        <v>347</v>
+      </c>
+      <c r="J18" s="20" t="s">
+        <v>174</v>
+      </c>
+      <c r="K18" s="20" t="s">
         <v>348</v>
-      </c>
-      <c r="J18" s="20" t="s">
-        <v>175</v>
-      </c>
-      <c r="K18" s="20" t="s">
-        <v>349</v>
       </c>
       <c r="L18" s="18">
         <v>0</v>
@@ -3792,28 +3792,28 @@
         <v>65</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E19" s="39" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F19" s="39">
         <v>30</v>
       </c>
       <c r="G19" s="40" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H19" s="41" t="s">
         <v>39</v>
       </c>
       <c r="I19" s="42" t="s">
+        <v>349</v>
+      </c>
+      <c r="J19" s="43" t="s">
         <v>350</v>
       </c>
-      <c r="J19" s="43" t="s">
+      <c r="K19" s="44" t="s">
         <v>351</v>
-      </c>
-      <c r="K19" s="44" t="s">
-        <v>352</v>
       </c>
       <c r="L19" s="41">
         <v>0</v>
@@ -3830,28 +3830,28 @@
         <v>65</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E20" s="39" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F20" s="39">
         <v>30</v>
       </c>
       <c r="G20" s="40" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H20" s="18" t="s">
         <v>39</v>
       </c>
       <c r="I20" s="19" t="s">
+        <v>352</v>
+      </c>
+      <c r="J20" s="20" t="s">
         <v>353</v>
       </c>
-      <c r="J20" s="20" t="s">
+      <c r="K20" s="29" t="s">
         <v>354</v>
-      </c>
-      <c r="K20" s="29" t="s">
-        <v>355</v>
       </c>
       <c r="L20" s="18">
         <v>0</v>
@@ -3868,7 +3868,7 @@
         <v>65</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E21" s="39" t="s">
         <v>68</v>
@@ -3877,19 +3877,19 @@
         <v>30</v>
       </c>
       <c r="G21" s="40" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H21" s="18" t="s">
         <v>39</v>
       </c>
       <c r="I21" s="19" t="s">
+        <v>355</v>
+      </c>
+      <c r="J21" s="20" t="s">
         <v>356</v>
       </c>
-      <c r="J21" s="20" t="s">
+      <c r="K21" s="29" t="s">
         <v>357</v>
-      </c>
-      <c r="K21" s="29" t="s">
-        <v>358</v>
       </c>
       <c r="L21" s="18">
         <v>0</v>
@@ -3906,7 +3906,7 @@
         <v>65</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E22" s="17" t="s">
         <v>70</v>
@@ -3915,19 +3915,19 @@
         <v>30</v>
       </c>
       <c r="G22" s="40" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H22" s="18" t="s">
         <v>39</v>
       </c>
       <c r="I22" s="19" t="s">
+        <v>358</v>
+      </c>
+      <c r="J22" s="20" t="s">
         <v>359</v>
       </c>
-      <c r="J22" s="20" t="s">
+      <c r="K22" s="29" t="s">
         <v>360</v>
-      </c>
-      <c r="K22" s="29" t="s">
-        <v>361</v>
       </c>
       <c r="L22" s="18">
         <v>0</v>
@@ -3944,26 +3944,26 @@
         <v>75</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E23" s="17">
         <v>100</v>
       </c>
       <c r="F23" s="17"/>
       <c r="G23" s="28" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H23" s="28" t="s">
         <v>33</v>
       </c>
       <c r="I23" s="19" t="s">
+        <v>361</v>
+      </c>
+      <c r="J23" s="20" t="s">
         <v>362</v>
       </c>
-      <c r="J23" s="20" t="s">
+      <c r="K23" s="29" t="s">
         <v>363</v>
-      </c>
-      <c r="K23" s="29" t="s">
-        <v>364</v>
       </c>
       <c r="L23" s="28">
         <v>0</v>
@@ -3980,28 +3980,28 @@
         <v>82</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E24" s="17" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F24" s="17">
         <v>10</v>
       </c>
       <c r="G24" s="28" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H24" s="28" t="s">
         <v>29</v>
       </c>
       <c r="I24" s="19" t="s">
+        <v>364</v>
+      </c>
+      <c r="J24" s="20" t="s">
         <v>365</v>
       </c>
-      <c r="J24" s="20" t="s">
+      <c r="K24" s="29" t="s">
         <v>366</v>
-      </c>
-      <c r="K24" s="29" t="s">
-        <v>367</v>
       </c>
       <c r="L24" s="28">
         <v>0</v>
@@ -4018,26 +4018,26 @@
         <v>18</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E25" s="56">
         <v>-50</v>
       </c>
       <c r="F25" s="56"/>
       <c r="G25" s="28" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H25" s="57" t="s">
         <v>39</v>
       </c>
       <c r="I25" s="58" t="s">
+        <v>367</v>
+      </c>
+      <c r="J25" s="59" t="s">
         <v>368</v>
       </c>
-      <c r="J25" s="59" t="s">
+      <c r="K25" s="60" t="s">
         <v>369</v>
-      </c>
-      <c r="K25" s="60" t="s">
-        <v>370</v>
       </c>
       <c r="L25" s="57">
         <v>0</v>
@@ -4054,26 +4054,26 @@
         <v>51</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E26" s="56">
         <v>-30</v>
       </c>
       <c r="F26" s="56"/>
       <c r="G26" s="28" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H26" s="57" t="s">
         <v>39</v>
       </c>
       <c r="I26" s="58" t="s">
+        <v>370</v>
+      </c>
+      <c r="J26" s="59" t="s">
         <v>371</v>
       </c>
-      <c r="J26" s="59" t="s">
+      <c r="K26" s="60" t="s">
         <v>372</v>
-      </c>
-      <c r="K26" s="60" t="s">
-        <v>373</v>
       </c>
       <c r="L26" s="57">
         <v>0</v>
@@ -4084,13 +4084,13 @@
         <v>3</v>
       </c>
       <c r="B27" s="54" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C27" s="55" t="s">
         <v>97</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E27" s="56" t="s">
         <v>95</v>
@@ -4099,19 +4099,19 @@
         <v>96</v>
       </c>
       <c r="G27" s="28" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H27" s="57" t="s">
         <v>29</v>
       </c>
       <c r="I27" s="58" t="s">
+        <v>373</v>
+      </c>
+      <c r="J27" s="59" t="s">
         <v>374</v>
       </c>
-      <c r="J27" s="59" t="s">
+      <c r="K27" s="60" t="s">
         <v>375</v>
-      </c>
-      <c r="K27" s="60" t="s">
-        <v>376</v>
       </c>
       <c r="L27" s="57">
         <v>0</v>
@@ -4122,34 +4122,34 @@
         <v>3</v>
       </c>
       <c r="B28" s="16" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C28" s="6" t="s">
         <v>97</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E28" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="F28" s="17" t="s">
         <v>134</v>
       </c>
-      <c r="F28" s="17" t="s">
-        <v>135</v>
-      </c>
       <c r="G28" s="28" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H28" s="28" t="s">
         <v>35</v>
       </c>
       <c r="I28" s="19" t="s">
+        <v>376</v>
+      </c>
+      <c r="J28" s="20" t="s">
         <v>377</v>
       </c>
-      <c r="J28" s="20" t="s">
+      <c r="K28" s="29" t="s">
         <v>378</v>
-      </c>
-      <c r="K28" s="29" t="s">
-        <v>379</v>
       </c>
       <c r="L28" s="28">
         <v>0</v>
@@ -4166,7 +4166,7 @@
         <v>27</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E29" s="17" t="s">
         <v>28</v>
@@ -4175,19 +4175,19 @@
         <v>1</v>
       </c>
       <c r="G29" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H29" s="18" t="s">
         <v>29</v>
       </c>
       <c r="I29" s="19" t="s">
+        <v>379</v>
+      </c>
+      <c r="J29" s="20" t="s">
         <v>380</v>
       </c>
-      <c r="J29" s="20" t="s">
+      <c r="K29" s="20" t="s">
         <v>381</v>
-      </c>
-      <c r="K29" s="20" t="s">
-        <v>382</v>
       </c>
       <c r="L29" s="18">
         <v>0</v>
@@ -4204,7 +4204,7 @@
         <v>27</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E30" s="17" t="s">
         <v>31</v>
@@ -4213,19 +4213,19 @@
         <v>1</v>
       </c>
       <c r="G30" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H30" s="18" t="s">
         <v>29</v>
       </c>
       <c r="I30" s="19" t="s">
+        <v>382</v>
+      </c>
+      <c r="J30" s="20" t="s">
         <v>383</v>
       </c>
-      <c r="J30" s="20" t="s">
+      <c r="K30" s="20" t="s">
         <v>384</v>
-      </c>
-      <c r="K30" s="20" t="s">
-        <v>385</v>
       </c>
       <c r="L30" s="18">
         <v>0</v>
@@ -4242,24 +4242,24 @@
         <v>7</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E31" s="17"/>
       <c r="F31" s="17"/>
       <c r="G31" s="18" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H31" s="18" t="s">
         <v>35</v>
       </c>
       <c r="I31" s="19" t="s">
+        <v>385</v>
+      </c>
+      <c r="J31" s="20" t="s">
+        <v>178</v>
+      </c>
+      <c r="K31" s="20" t="s">
         <v>386</v>
-      </c>
-      <c r="J31" s="20" t="s">
-        <v>179</v>
-      </c>
-      <c r="K31" s="20" t="s">
-        <v>387</v>
       </c>
       <c r="L31" s="18">
         <v>0</v>
@@ -4276,26 +4276,26 @@
         <v>36</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E32" s="17">
         <v>1</v>
       </c>
       <c r="F32" s="17"/>
       <c r="G32" s="18" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H32" s="18" t="s">
         <v>35</v>
       </c>
       <c r="I32" s="19" t="s">
+        <v>387</v>
+      </c>
+      <c r="J32" s="20" t="s">
         <v>388</v>
       </c>
-      <c r="J32" s="20" t="s">
+      <c r="K32" s="20" t="s">
         <v>389</v>
-      </c>
-      <c r="K32" s="20" t="s">
-        <v>390</v>
       </c>
       <c r="L32" s="18">
         <v>0</v>
@@ -4312,26 +4312,26 @@
         <v>38</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E33" s="17">
         <v>11</v>
       </c>
       <c r="F33" s="17"/>
       <c r="G33" s="18" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H33" s="18" t="s">
         <v>39</v>
       </c>
       <c r="I33" s="19" t="s">
+        <v>390</v>
+      </c>
+      <c r="J33" s="20" t="s">
         <v>391</v>
       </c>
-      <c r="J33" s="20" t="s">
+      <c r="K33" s="20" t="s">
         <v>392</v>
-      </c>
-      <c r="K33" s="20" t="s">
-        <v>393</v>
       </c>
       <c r="L33" s="18">
         <v>0</v>
@@ -4348,26 +4348,26 @@
         <v>38</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E34" s="17">
         <v>12</v>
       </c>
       <c r="F34" s="17"/>
       <c r="G34" s="18" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H34" s="18" t="s">
         <v>39</v>
       </c>
       <c r="I34" s="19" t="s">
+        <v>393</v>
+      </c>
+      <c r="J34" s="20" t="s">
         <v>394</v>
       </c>
-      <c r="J34" s="20" t="s">
+      <c r="K34" s="20" t="s">
         <v>395</v>
-      </c>
-      <c r="K34" s="20" t="s">
-        <v>396</v>
       </c>
       <c r="L34" s="18">
         <v>0</v>
@@ -4384,7 +4384,7 @@
         <v>38</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E35" s="17">
         <v>1</v>
@@ -4393,19 +4393,19 @@
         <v>1</v>
       </c>
       <c r="G35" s="18" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H35" s="18" t="s">
         <v>39</v>
       </c>
       <c r="I35" s="19" t="s">
+        <v>396</v>
+      </c>
+      <c r="J35" s="20" t="s">
         <v>397</v>
       </c>
-      <c r="J35" s="20" t="s">
+      <c r="K35" s="20" t="s">
         <v>398</v>
-      </c>
-      <c r="K35" s="20" t="s">
-        <v>399</v>
       </c>
       <c r="L35" s="18">
         <v>0</v>
@@ -4422,26 +4422,26 @@
         <v>42</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E36" s="17">
         <v>1</v>
       </c>
       <c r="F36" s="17"/>
       <c r="G36" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H36" s="18" t="s">
         <v>29</v>
       </c>
       <c r="I36" s="19" t="s">
+        <v>399</v>
+      </c>
+      <c r="J36" s="20" t="s">
         <v>400</v>
       </c>
-      <c r="J36" s="20" t="s">
+      <c r="K36" s="20" t="s">
         <v>401</v>
-      </c>
-      <c r="K36" s="20" t="s">
-        <v>402</v>
       </c>
       <c r="L36" s="18">
         <v>0</v>
@@ -4458,26 +4458,26 @@
         <v>43</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E37" s="17">
         <v>1</v>
       </c>
       <c r="F37" s="17"/>
       <c r="G37" s="28" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H37" s="28" t="s">
         <v>44</v>
       </c>
       <c r="I37" s="19" t="s">
+        <v>402</v>
+      </c>
+      <c r="J37" s="20" t="s">
         <v>403</v>
       </c>
-      <c r="J37" s="20" t="s">
+      <c r="K37" s="20" t="s">
         <v>404</v>
-      </c>
-      <c r="K37" s="20" t="s">
-        <v>405</v>
       </c>
       <c r="L37" s="28">
         <v>0</v>
@@ -4494,26 +4494,26 @@
         <v>48</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E38" s="17">
         <v>1</v>
       </c>
       <c r="F38" s="17"/>
       <c r="G38" s="18" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H38" s="18" t="s">
         <v>35</v>
       </c>
       <c r="I38" s="19" t="s">
+        <v>405</v>
+      </c>
+      <c r="J38" s="20" t="s">
         <v>406</v>
       </c>
-      <c r="J38" s="20" t="s">
+      <c r="K38" s="20" t="s">
         <v>407</v>
-      </c>
-      <c r="K38" s="20" t="s">
-        <v>408</v>
       </c>
       <c r="L38" s="18">
         <v>0</v>
@@ -4530,26 +4530,26 @@
         <v>49</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E39" s="17">
         <v>1</v>
       </c>
       <c r="F39" s="17"/>
       <c r="G39" s="18" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H39" s="28" t="s">
         <v>35</v>
       </c>
       <c r="I39" s="19" t="s">
+        <v>408</v>
+      </c>
+      <c r="J39" s="20" t="s">
         <v>409</v>
       </c>
-      <c r="J39" s="20" t="s">
+      <c r="K39" s="29" t="s">
         <v>410</v>
-      </c>
-      <c r="K39" s="29" t="s">
-        <v>411</v>
       </c>
       <c r="L39" s="28">
         <v>0</v>
@@ -4566,26 +4566,26 @@
         <v>55</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E40" s="30">
         <v>1</v>
       </c>
       <c r="F40" s="30"/>
       <c r="G40" s="18" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H40" s="28" t="s">
         <v>35</v>
       </c>
       <c r="I40" s="31" t="s">
+        <v>411</v>
+      </c>
+      <c r="J40" s="32" t="s">
         <v>412</v>
       </c>
-      <c r="J40" s="32" t="s">
+      <c r="K40" s="33" t="s">
         <v>413</v>
-      </c>
-      <c r="K40" s="33" t="s">
-        <v>414</v>
       </c>
       <c r="L40" s="28">
         <v>0</v>
@@ -4602,26 +4602,26 @@
         <v>56</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E41" s="17">
         <v>1</v>
       </c>
       <c r="F41" s="17"/>
       <c r="G41" s="18" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H41" s="18" t="s">
         <v>35</v>
       </c>
       <c r="I41" s="19" t="s">
+        <v>414</v>
+      </c>
+      <c r="J41" s="20" t="s">
         <v>415</v>
       </c>
-      <c r="J41" s="20" t="s">
+      <c r="K41" s="20" t="s">
         <v>416</v>
-      </c>
-      <c r="K41" s="20" t="s">
-        <v>417</v>
       </c>
       <c r="L41" s="18">
         <v>0</v>
@@ -4638,26 +4638,26 @@
         <v>59</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E42" s="30">
         <v>100</v>
       </c>
       <c r="F42" s="30"/>
       <c r="G42" s="28" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H42" s="28" t="s">
         <v>39</v>
       </c>
       <c r="I42" s="31" t="s">
+        <v>417</v>
+      </c>
+      <c r="J42" s="32" t="s">
         <v>418</v>
       </c>
-      <c r="J42" s="32" t="s">
+      <c r="K42" s="33" t="s">
         <v>419</v>
-      </c>
-      <c r="K42" s="33" t="s">
-        <v>420</v>
       </c>
       <c r="L42" s="28">
         <v>0</v>
@@ -4674,26 +4674,26 @@
         <v>60</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E43" s="30">
         <v>0</v>
       </c>
       <c r="F43" s="30"/>
       <c r="G43" s="28" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H43" s="28" t="s">
         <v>35</v>
       </c>
       <c r="I43" s="31" t="s">
+        <v>420</v>
+      </c>
+      <c r="J43" s="32" t="s">
         <v>421</v>
       </c>
-      <c r="J43" s="32" t="s">
+      <c r="K43" s="33" t="s">
         <v>422</v>
-      </c>
-      <c r="K43" s="33" t="s">
-        <v>423</v>
       </c>
       <c r="L43" s="28">
         <v>0</v>
@@ -4710,26 +4710,26 @@
         <v>61</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E44" s="17">
         <v>0</v>
       </c>
       <c r="F44" s="17"/>
       <c r="G44" s="28" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H44" s="18" t="s">
         <v>35</v>
       </c>
       <c r="I44" s="19" t="s">
+        <v>423</v>
+      </c>
+      <c r="J44" s="20" t="s">
         <v>424</v>
       </c>
-      <c r="J44" s="20" t="s">
+      <c r="K44" s="29" t="s">
         <v>425</v>
-      </c>
-      <c r="K44" s="29" t="s">
-        <v>426</v>
       </c>
       <c r="L44" s="18">
         <v>0</v>
@@ -4746,26 +4746,26 @@
         <v>62</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E45" s="17" t="s">
         <v>63</v>
       </c>
       <c r="F45" s="17"/>
       <c r="G45" s="28" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H45" s="18" t="s">
         <v>29</v>
       </c>
       <c r="I45" s="19" t="s">
+        <v>426</v>
+      </c>
+      <c r="J45" s="20" t="s">
         <v>427</v>
       </c>
-      <c r="J45" s="20" t="s">
+      <c r="K45" s="29" t="s">
         <v>428</v>
-      </c>
-      <c r="K45" s="29" t="s">
-        <v>429</v>
       </c>
       <c r="L45" s="18">
         <v>0</v>
@@ -4782,24 +4782,24 @@
         <v>72</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E46" s="17"/>
       <c r="F46" s="17"/>
       <c r="G46" s="28" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H46" s="18" t="s">
         <v>29</v>
       </c>
       <c r="I46" s="19" t="s">
+        <v>429</v>
+      </c>
+      <c r="J46" s="20" t="s">
         <v>430</v>
       </c>
-      <c r="J46" s="20" t="s">
+      <c r="K46" s="29" t="s">
         <v>431</v>
-      </c>
-      <c r="K46" s="29" t="s">
-        <v>432</v>
       </c>
       <c r="L46" s="18">
         <v>0</v>
@@ -4816,24 +4816,24 @@
         <v>73</v>
       </c>
       <c r="D47" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E47" s="17"/>
       <c r="F47" s="17"/>
       <c r="G47" s="28" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H47" s="18" t="s">
         <v>29</v>
       </c>
       <c r="I47" s="19" t="s">
+        <v>432</v>
+      </c>
+      <c r="J47" s="20" t="s">
         <v>433</v>
       </c>
-      <c r="J47" s="20" t="s">
+      <c r="K47" s="29" t="s">
         <v>434</v>
-      </c>
-      <c r="K47" s="29" t="s">
-        <v>435</v>
       </c>
       <c r="L47" s="18">
         <v>0</v>
@@ -4850,24 +4850,24 @@
         <v>74</v>
       </c>
       <c r="D48" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E48" s="17"/>
       <c r="F48" s="17"/>
       <c r="G48" s="28" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H48" s="28" t="s">
         <v>35</v>
       </c>
       <c r="I48" s="19" t="s">
+        <v>435</v>
+      </c>
+      <c r="J48" s="20" t="s">
         <v>436</v>
       </c>
-      <c r="J48" s="20" t="s">
+      <c r="K48" s="29" t="s">
         <v>437</v>
-      </c>
-      <c r="K48" s="29" t="s">
-        <v>438</v>
       </c>
       <c r="L48" s="28">
         <v>0</v>
@@ -4884,24 +4884,24 @@
         <v>76</v>
       </c>
       <c r="D49" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E49" s="23"/>
       <c r="F49" s="23"/>
       <c r="G49" s="46" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H49" s="46" t="s">
         <v>33</v>
       </c>
       <c r="I49" s="47" t="s">
+        <v>438</v>
+      </c>
+      <c r="J49" s="48" t="s">
         <v>439</v>
       </c>
-      <c r="J49" s="48" t="s">
+      <c r="K49" s="49" t="s">
         <v>440</v>
-      </c>
-      <c r="K49" s="49" t="s">
-        <v>441</v>
       </c>
       <c r="L49" s="46">
         <v>0</v>
@@ -4918,24 +4918,24 @@
         <v>78</v>
       </c>
       <c r="D50" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E50" s="23"/>
       <c r="F50" s="23"/>
       <c r="G50" s="46" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H50" s="46" t="s">
         <v>35</v>
       </c>
       <c r="I50" s="47" t="s">
+        <v>441</v>
+      </c>
+      <c r="J50" s="48" t="s">
         <v>442</v>
       </c>
-      <c r="J50" s="48" t="s">
+      <c r="K50" s="49" t="s">
         <v>443</v>
-      </c>
-      <c r="K50" s="49" t="s">
-        <v>444</v>
       </c>
       <c r="L50" s="46">
         <v>0</v>
@@ -4952,24 +4952,24 @@
         <v>78</v>
       </c>
       <c r="D51" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E51" s="23"/>
       <c r="F51" s="23"/>
       <c r="G51" s="46" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H51" s="46" t="s">
         <v>35</v>
       </c>
       <c r="I51" s="47" t="s">
+        <v>444</v>
+      </c>
+      <c r="J51" s="48" t="s">
         <v>445</v>
       </c>
-      <c r="J51" s="48" t="s">
+      <c r="K51" s="49" t="s">
         <v>446</v>
-      </c>
-      <c r="K51" s="49" t="s">
-        <v>447</v>
       </c>
       <c r="L51" s="46">
         <v>0</v>
@@ -4986,24 +4986,24 @@
         <v>78</v>
       </c>
       <c r="D52" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E52" s="17"/>
       <c r="F52" s="17"/>
       <c r="G52" s="46" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H52" s="28" t="s">
         <v>35</v>
       </c>
       <c r="I52" s="19" t="s">
+        <v>447</v>
+      </c>
+      <c r="J52" s="20" t="s">
         <v>448</v>
       </c>
-      <c r="J52" s="20" t="s">
+      <c r="K52" s="29" t="s">
         <v>449</v>
-      </c>
-      <c r="K52" s="29" t="s">
-        <v>450</v>
       </c>
       <c r="L52" s="28">
         <v>0</v>
@@ -5020,7 +5020,7 @@
         <v>83</v>
       </c>
       <c r="D53" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E53" s="17"/>
       <c r="F53" s="17"/>
@@ -5054,7 +5054,7 @@
         <v>86</v>
       </c>
       <c r="D54" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E54" s="17">
         <v>1</v>
@@ -5063,19 +5063,19 @@
         <v>1</v>
       </c>
       <c r="G54" s="61" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H54" s="28" t="s">
         <v>39</v>
       </c>
       <c r="I54" s="19" t="s">
+        <v>450</v>
+      </c>
+      <c r="J54" s="20" t="s">
         <v>451</v>
       </c>
-      <c r="J54" s="20" t="s">
+      <c r="K54" s="29" t="s">
         <v>452</v>
-      </c>
-      <c r="K54" s="29" t="s">
-        <v>453</v>
       </c>
       <c r="L54" s="28">
         <v>0</v>
@@ -5092,7 +5092,7 @@
         <v>87</v>
       </c>
       <c r="D55" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E55" s="17">
         <v>1</v>
@@ -5101,19 +5101,19 @@
         <v>1</v>
       </c>
       <c r="G55" s="28" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H55" s="28" t="s">
         <v>39</v>
       </c>
       <c r="I55" s="19" t="s">
+        <v>453</v>
+      </c>
+      <c r="J55" s="20" t="s">
         <v>454</v>
       </c>
-      <c r="J55" s="20" t="s">
+      <c r="K55" s="29" t="s">
         <v>455</v>
-      </c>
-      <c r="K55" s="29" t="s">
-        <v>456</v>
       </c>
       <c r="L55" s="28">
         <v>0</v>
@@ -5126,28 +5126,30 @@
       <c r="B56" s="54" t="s">
         <v>98</v>
       </c>
-      <c r="C56" s="55" t="s">
-        <v>99</v>
+      <c r="C56" s="6" t="s">
+        <v>465</v>
       </c>
       <c r="D56" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="E56" s="56"/>
+        <v>101</v>
+      </c>
+      <c r="E56" s="56">
+        <v>5</v>
+      </c>
       <c r="F56" s="56"/>
       <c r="G56" s="28" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H56" s="57" t="s">
         <v>35</v>
       </c>
       <c r="I56" s="58" t="s">
+        <v>456</v>
+      </c>
+      <c r="J56" s="59" t="s">
         <v>457</v>
       </c>
-      <c r="J56" s="59" t="s">
+      <c r="K56" s="60" t="s">
         <v>458</v>
-      </c>
-      <c r="K56" s="60" t="s">
-        <v>459</v>
       </c>
       <c r="L56" s="57">
         <v>0</v>
@@ -5158,30 +5160,30 @@
         <v>3</v>
       </c>
       <c r="B57" s="63" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C57" s="64" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D57" s="147" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E57" s="67"/>
       <c r="F57" s="67"/>
       <c r="G57" s="28" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H57" s="68" t="s">
         <v>35</v>
       </c>
       <c r="I57" s="69" t="s">
+        <v>105</v>
+      </c>
+      <c r="J57" s="70" t="s">
         <v>106</v>
       </c>
-      <c r="J57" s="70" t="s">
+      <c r="K57" s="71" t="s">
         <v>107</v>
-      </c>
-      <c r="K57" s="71" t="s">
-        <v>108</v>
       </c>
       <c r="L57" s="68">
         <v>0</v>
@@ -5192,30 +5194,30 @@
         <v>3</v>
       </c>
       <c r="B58" s="63" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C58" s="64" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D58" s="147" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E58" s="67"/>
       <c r="F58" s="67"/>
       <c r="G58" s="28" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H58" s="68" t="s">
         <v>35</v>
       </c>
       <c r="I58" s="69" t="s">
+        <v>108</v>
+      </c>
+      <c r="J58" s="70" t="s">
         <v>109</v>
       </c>
-      <c r="J58" s="70" t="s">
+      <c r="K58" s="71" t="s">
         <v>110</v>
-      </c>
-      <c r="K58" s="71" t="s">
-        <v>111</v>
       </c>
       <c r="L58" s="68">
         <v>0</v>
@@ -5226,30 +5228,30 @@
         <v>3</v>
       </c>
       <c r="B59" s="73" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C59" s="65" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D59" s="66" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E59" s="74"/>
       <c r="F59" s="74"/>
       <c r="G59" s="28" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H59" s="75" t="s">
         <v>35</v>
       </c>
       <c r="I59" s="76" t="s">
+        <v>111</v>
+      </c>
+      <c r="J59" s="77" t="s">
         <v>112</v>
       </c>
-      <c r="J59" s="77" t="s">
+      <c r="K59" s="78" t="s">
         <v>113</v>
-      </c>
-      <c r="K59" s="78" t="s">
-        <v>114</v>
       </c>
       <c r="L59" s="75">
         <v>0</v>
@@ -5260,30 +5262,30 @@
         <v>3</v>
       </c>
       <c r="B60" s="81" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C60" s="82" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D60" s="82" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E60" s="83"/>
       <c r="F60" s="83"/>
       <c r="G60" s="28" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H60" s="84" t="s">
         <v>35</v>
       </c>
       <c r="I60" s="85" t="s">
+        <v>115</v>
+      </c>
+      <c r="J60" s="86" t="s">
         <v>116</v>
       </c>
-      <c r="J60" s="86" t="s">
+      <c r="K60" s="86" t="s">
         <v>117</v>
-      </c>
-      <c r="K60" s="86" t="s">
-        <v>118</v>
       </c>
       <c r="L60" s="84">
         <v>0</v>
@@ -5294,30 +5296,30 @@
         <v>3</v>
       </c>
       <c r="B61" s="88" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C61" s="89" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D61" s="89" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E61" s="90"/>
       <c r="F61" s="90"/>
       <c r="G61" s="28" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H61" s="91" t="s">
         <v>35</v>
       </c>
       <c r="I61" s="92" t="s">
+        <v>122</v>
+      </c>
+      <c r="J61" s="92" t="s">
         <v>123</v>
       </c>
-      <c r="J61" s="92" t="s">
+      <c r="K61" s="92" t="s">
         <v>124</v>
-      </c>
-      <c r="K61" s="92" t="s">
-        <v>125</v>
       </c>
       <c r="L61" s="91">
         <v>0</v>
@@ -5328,30 +5330,30 @@
         <v>3</v>
       </c>
       <c r="B62" s="88" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C62" s="89" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D62" s="89" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E62" s="90"/>
       <c r="F62" s="90"/>
       <c r="G62" s="28" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H62" s="91" t="s">
         <v>35</v>
       </c>
       <c r="I62" s="92" t="s">
+        <v>125</v>
+      </c>
+      <c r="J62" s="92" t="s">
         <v>126</v>
       </c>
-      <c r="J62" s="92" t="s">
+      <c r="K62" s="92" t="s">
         <v>127</v>
-      </c>
-      <c r="K62" s="92" t="s">
-        <v>128</v>
       </c>
       <c r="L62" s="91">
         <v>0</v>
@@ -5362,30 +5364,30 @@
         <v>3</v>
       </c>
       <c r="B63" s="88" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C63" s="89" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D63" s="89" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E63" s="93"/>
       <c r="F63" s="93"/>
       <c r="G63" s="28" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H63" s="91" t="s">
         <v>35</v>
       </c>
       <c r="I63" s="92" t="s">
+        <v>459</v>
+      </c>
+      <c r="J63" s="94" t="s">
         <v>460</v>
       </c>
-      <c r="J63" s="94" t="s">
+      <c r="K63" s="95" t="s">
         <v>461</v>
-      </c>
-      <c r="K63" s="95" t="s">
-        <v>462</v>
       </c>
       <c r="L63" s="91">
         <v>0</v>
@@ -5396,30 +5398,30 @@
         <v>3</v>
       </c>
       <c r="B64" s="88" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C64" s="89" t="s">
         <v>74</v>
       </c>
       <c r="D64" s="89" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E64" s="96"/>
       <c r="F64" s="96"/>
       <c r="G64" s="28" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H64" s="91" t="s">
         <v>35</v>
       </c>
       <c r="I64" s="97" t="s">
+        <v>462</v>
+      </c>
+      <c r="J64" s="98" t="s">
         <v>463</v>
       </c>
-      <c r="J64" s="98" t="s">
+      <c r="K64" s="99" t="s">
         <v>464</v>
-      </c>
-      <c r="K64" s="99" t="s">
-        <v>465</v>
       </c>
       <c r="L64" s="91">
         <v>0</v>
@@ -5430,32 +5432,32 @@
         <v>3</v>
       </c>
       <c r="B65" s="102" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C65" s="103" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D65" s="103" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E65" s="104">
         <v>1</v>
       </c>
       <c r="F65" s="104"/>
       <c r="G65" s="105" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H65" s="105" t="s">
         <v>35</v>
       </c>
       <c r="I65" s="106" t="s">
+        <v>128</v>
+      </c>
+      <c r="J65" s="106" t="s">
         <v>129</v>
       </c>
-      <c r="J65" s="106" t="s">
+      <c r="K65" s="106" t="s">
         <v>130</v>
-      </c>
-      <c r="K65" s="106" t="s">
-        <v>131</v>
       </c>
       <c r="L65" s="105">
         <v>0</v>
@@ -5466,32 +5468,32 @@
         <v>3</v>
       </c>
       <c r="B66" s="107" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C66" s="118" t="s">
         <v>50</v>
       </c>
       <c r="D66" s="118" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E66" s="119">
         <v>150</v>
       </c>
       <c r="F66" s="119"/>
       <c r="G66" s="108" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H66" s="120" t="s">
         <v>44</v>
       </c>
       <c r="I66" s="121" t="s">
+        <v>167</v>
+      </c>
+      <c r="J66" s="122" t="s">
         <v>168</v>
       </c>
-      <c r="J66" s="122" t="s">
-        <v>169</v>
-      </c>
       <c r="K66" s="122" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="L66" s="120">
         <v>1</v>
@@ -5502,32 +5504,32 @@
         <v>3</v>
       </c>
       <c r="B67" s="107" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C67" s="118" t="s">
         <v>50</v>
       </c>
       <c r="D67" s="118" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E67" s="119">
         <v>70</v>
       </c>
       <c r="F67" s="119"/>
       <c r="G67" s="108" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H67" s="120" t="s">
         <v>44</v>
       </c>
       <c r="I67" s="121" t="s">
+        <v>167</v>
+      </c>
+      <c r="J67" s="122" t="s">
         <v>168</v>
       </c>
-      <c r="J67" s="122" t="s">
-        <v>169</v>
-      </c>
       <c r="K67" s="122" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="L67" s="120">
         <v>1</v>
@@ -5538,32 +5540,32 @@
         <v>3</v>
       </c>
       <c r="B68" s="107" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C68" s="118" t="s">
         <v>16</v>
       </c>
       <c r="D68" s="118" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E68" s="119">
         <v>100</v>
       </c>
       <c r="F68" s="119"/>
       <c r="G68" s="108" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H68" s="120" t="s">
         <v>44</v>
       </c>
       <c r="I68" s="121" t="s">
+        <v>170</v>
+      </c>
+      <c r="J68" s="122" t="s">
         <v>171</v>
       </c>
-      <c r="J68" s="122" t="s">
-        <v>172</v>
-      </c>
       <c r="K68" s="122" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="L68" s="120">
         <v>1</v>
@@ -5574,32 +5576,32 @@
         <v>3</v>
       </c>
       <c r="B69" s="123" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C69" s="118" t="s">
         <v>16</v>
       </c>
       <c r="D69" s="118" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E69" s="119">
         <v>75</v>
       </c>
       <c r="F69" s="119"/>
       <c r="G69" s="108" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H69" s="120" t="s">
         <v>44</v>
       </c>
       <c r="I69" s="121" t="s">
+        <v>170</v>
+      </c>
+      <c r="J69" s="122" t="s">
         <v>171</v>
       </c>
-      <c r="J69" s="122" t="s">
-        <v>172</v>
-      </c>
       <c r="K69" s="122" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="L69" s="120">
         <v>1</v>
@@ -5610,32 +5612,32 @@
         <v>3</v>
       </c>
       <c r="B70" s="123" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C70" s="118" t="s">
         <v>58</v>
       </c>
       <c r="D70" s="118" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E70" s="119">
         <v>50</v>
       </c>
       <c r="F70" s="119"/>
       <c r="G70" s="108" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H70" s="120" t="s">
         <v>33</v>
       </c>
       <c r="I70" s="121" t="s">
+        <v>173</v>
+      </c>
+      <c r="J70" s="122" t="s">
         <v>174</v>
       </c>
-      <c r="J70" s="122" t="s">
-        <v>175</v>
-      </c>
       <c r="K70" s="122" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="L70" s="120">
         <v>1</v>
@@ -5646,32 +5648,32 @@
         <v>3</v>
       </c>
       <c r="B71" s="123" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C71" s="118" t="s">
         <v>58</v>
       </c>
       <c r="D71" s="118" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E71" s="119">
         <v>30</v>
       </c>
       <c r="F71" s="119"/>
       <c r="G71" s="108" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H71" s="120" t="s">
         <v>33</v>
       </c>
       <c r="I71" s="121" t="s">
+        <v>173</v>
+      </c>
+      <c r="J71" s="122" t="s">
         <v>174</v>
       </c>
-      <c r="J71" s="122" t="s">
-        <v>175</v>
-      </c>
       <c r="K71" s="122" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="L71" s="120">
         <v>1</v>
@@ -5682,30 +5684,30 @@
         <v>3</v>
       </c>
       <c r="B72" s="123" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C72" s="118" t="s">
         <v>7</v>
       </c>
       <c r="D72" s="118" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E72" s="119"/>
       <c r="F72" s="119"/>
       <c r="G72" s="108" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H72" s="120" t="s">
         <v>33</v>
       </c>
       <c r="I72" s="121" t="s">
+        <v>177</v>
+      </c>
+      <c r="J72" s="122" t="s">
         <v>178</v>
       </c>
-      <c r="J72" s="122" t="s">
-        <v>179</v>
-      </c>
       <c r="K72" s="122" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="L72" s="120">
         <v>1</v>
@@ -5716,32 +5718,32 @@
         <v>3</v>
       </c>
       <c r="B73" s="107" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C73" s="118" t="s">
         <v>32</v>
       </c>
       <c r="D73" s="118" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E73" s="119">
         <v>25</v>
       </c>
       <c r="F73" s="119"/>
       <c r="G73" s="108" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H73" s="120" t="s">
         <v>33</v>
       </c>
       <c r="I73" s="121" t="s">
+        <v>179</v>
+      </c>
+      <c r="J73" s="122" t="s">
         <v>180</v>
       </c>
-      <c r="J73" s="122" t="s">
-        <v>181</v>
-      </c>
       <c r="K73" s="122" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="L73" s="120">
         <v>1</v>
@@ -5752,32 +5754,32 @@
         <v>3</v>
       </c>
       <c r="B74" s="123" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C74" s="118" t="s">
         <v>32</v>
       </c>
       <c r="D74" s="118" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E74" s="119">
         <v>15</v>
       </c>
       <c r="F74" s="119"/>
       <c r="G74" s="108" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H74" s="120" t="s">
         <v>33</v>
       </c>
       <c r="I74" s="121" t="s">
+        <v>179</v>
+      </c>
+      <c r="J74" s="122" t="s">
         <v>180</v>
       </c>
-      <c r="J74" s="122" t="s">
-        <v>181</v>
-      </c>
       <c r="K74" s="122" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="L74" s="120">
         <v>1</v>
@@ -5788,13 +5790,13 @@
         <v>3</v>
       </c>
       <c r="B75" s="123" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C75" s="118" t="s">
         <v>53</v>
       </c>
       <c r="D75" s="118" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E75" s="119" t="s">
         <v>31</v>
@@ -5803,19 +5805,19 @@
         <v>100</v>
       </c>
       <c r="G75" s="108" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H75" s="120" t="s">
         <v>29</v>
       </c>
       <c r="I75" s="121" t="s">
+        <v>182</v>
+      </c>
+      <c r="J75" s="122" t="s">
         <v>183</v>
       </c>
-      <c r="J75" s="122" t="s">
+      <c r="K75" s="122" t="s">
         <v>184</v>
-      </c>
-      <c r="K75" s="122" t="s">
-        <v>185</v>
       </c>
       <c r="L75" s="120">
         <v>1</v>
@@ -5826,13 +5828,13 @@
         <v>3</v>
       </c>
       <c r="B76" s="123" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C76" s="118" t="s">
         <v>53</v>
       </c>
       <c r="D76" s="118" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E76" s="119" t="s">
         <v>28</v>
@@ -5841,19 +5843,19 @@
         <v>50</v>
       </c>
       <c r="G76" s="108" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H76" s="120" t="s">
         <v>29</v>
       </c>
       <c r="I76" s="121" t="s">
+        <v>185</v>
+      </c>
+      <c r="J76" s="122" t="s">
         <v>186</v>
       </c>
-      <c r="J76" s="122" t="s">
-        <v>187</v>
-      </c>
       <c r="K76" s="122" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="L76" s="120">
         <v>1</v>
@@ -5864,13 +5866,13 @@
         <v>3</v>
       </c>
       <c r="B77" s="123" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C77" s="118" t="s">
         <v>53</v>
       </c>
       <c r="D77" s="118" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E77" s="119" t="s">
         <v>28</v>
@@ -5879,19 +5881,19 @@
         <v>35</v>
       </c>
       <c r="G77" s="108" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H77" s="120" t="s">
         <v>29</v>
       </c>
       <c r="I77" s="121" t="s">
+        <v>185</v>
+      </c>
+      <c r="J77" s="122" t="s">
         <v>186</v>
       </c>
-      <c r="J77" s="122" t="s">
-        <v>187</v>
-      </c>
       <c r="K77" s="122" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="L77" s="120">
         <v>1</v>
@@ -5902,32 +5904,32 @@
         <v>3</v>
       </c>
       <c r="B78" s="125" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C78" s="126" t="s">
         <v>12</v>
       </c>
       <c r="D78" s="126" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E78" s="127">
         <v>50</v>
       </c>
       <c r="F78" s="127"/>
       <c r="G78" s="108" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H78" s="120" t="s">
         <v>5</v>
       </c>
       <c r="I78" s="121" t="s">
+        <v>188</v>
+      </c>
+      <c r="J78" s="122" t="s">
         <v>189</v>
       </c>
-      <c r="J78" s="122" t="s">
-        <v>190</v>
-      </c>
       <c r="K78" s="122" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="L78" s="120">
         <v>1</v>
@@ -5938,32 +5940,32 @@
         <v>3</v>
       </c>
       <c r="B79" s="123" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C79" s="118" t="s">
         <v>51</v>
       </c>
       <c r="D79" s="118" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E79" s="119">
         <v>25</v>
       </c>
       <c r="F79" s="119"/>
       <c r="G79" s="108" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H79" s="120" t="s">
         <v>46</v>
       </c>
       <c r="I79" s="121" t="s">
+        <v>190</v>
+      </c>
+      <c r="J79" s="122" t="s">
         <v>191</v>
       </c>
-      <c r="J79" s="122" t="s">
-        <v>192</v>
-      </c>
       <c r="K79" s="122" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="L79" s="120">
         <v>1</v>
@@ -5974,32 +5976,32 @@
         <v>3</v>
       </c>
       <c r="B80" s="123" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C80" s="118" t="s">
         <v>51</v>
       </c>
       <c r="D80" s="118" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E80" s="119">
         <v>15</v>
       </c>
       <c r="F80" s="119"/>
       <c r="G80" s="108" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H80" s="120" t="s">
         <v>46</v>
       </c>
       <c r="I80" s="121" t="s">
+        <v>190</v>
+      </c>
+      <c r="J80" s="122" t="s">
         <v>191</v>
       </c>
-      <c r="J80" s="122" t="s">
-        <v>192</v>
-      </c>
       <c r="K80" s="122" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="L80" s="120">
         <v>1</v>
@@ -6010,32 +6012,32 @@
         <v>3</v>
       </c>
       <c r="B81" s="129" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C81" s="130" t="s">
         <v>34</v>
       </c>
       <c r="D81" s="130" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E81" s="131">
         <v>20</v>
       </c>
       <c r="F81" s="131"/>
       <c r="G81" s="132" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H81" s="133" t="s">
         <v>5</v>
       </c>
       <c r="I81" s="121" t="s">
+        <v>193</v>
+      </c>
+      <c r="J81" s="122" t="s">
         <v>194</v>
       </c>
-      <c r="J81" s="122" t="s">
-        <v>195</v>
-      </c>
       <c r="K81" s="122" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="L81" s="133">
         <v>1</v>
@@ -6046,34 +6048,34 @@
         <v>3</v>
       </c>
       <c r="B82" s="109" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C82" s="111" t="s">
         <v>97</v>
       </c>
       <c r="D82" s="111" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E82" s="112" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F82" s="112" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G82" s="46" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H82" s="113" t="s">
         <v>35</v>
       </c>
       <c r="I82" s="114" t="s">
+        <v>196</v>
+      </c>
+      <c r="J82" s="115" t="s">
         <v>197</v>
       </c>
-      <c r="J82" s="115" t="s">
+      <c r="K82" s="115" t="s">
         <v>198</v>
-      </c>
-      <c r="K82" s="115" t="s">
-        <v>199</v>
       </c>
       <c r="L82" s="113">
         <v>2</v>
@@ -6084,34 +6086,34 @@
         <v>3</v>
       </c>
       <c r="B83" s="109" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C83" s="111" t="s">
         <v>97</v>
       </c>
       <c r="D83" s="111" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E83" s="112" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F83" s="112" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G83" s="113" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H83" s="113" t="s">
         <v>35</v>
       </c>
       <c r="I83" s="114" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="J83" s="115" t="s">
+        <v>200</v>
+      </c>
+      <c r="K83" s="115" t="s">
         <v>201</v>
-      </c>
-      <c r="K83" s="115" t="s">
-        <v>202</v>
       </c>
       <c r="L83" s="113">
         <v>2</v>
@@ -6122,34 +6124,34 @@
         <v>3</v>
       </c>
       <c r="B84" s="109" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C84" s="111" t="s">
         <v>97</v>
       </c>
       <c r="D84" s="111" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E84" s="112" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F84" s="112" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G84" s="113" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H84" s="113" t="s">
         <v>35</v>
       </c>
       <c r="I84" s="114" t="s">
+        <v>203</v>
+      </c>
+      <c r="J84" s="115" t="s">
         <v>204</v>
       </c>
-      <c r="J84" s="115" t="s">
+      <c r="K84" s="115" t="s">
         <v>205</v>
-      </c>
-      <c r="K84" s="115" t="s">
-        <v>206</v>
       </c>
       <c r="L84" s="113">
         <v>2</v>
@@ -6160,34 +6162,34 @@
         <v>3</v>
       </c>
       <c r="B85" s="109" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C85" s="111" t="s">
         <v>97</v>
       </c>
       <c r="D85" s="110" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E85" s="112" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F85" s="112" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G85" s="113" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H85" s="113" t="s">
         <v>35</v>
       </c>
       <c r="I85" s="114" t="s">
+        <v>206</v>
+      </c>
+      <c r="J85" s="115" t="s">
         <v>207</v>
       </c>
-      <c r="J85" s="115" t="s">
+      <c r="K85" s="115" t="s">
         <v>208</v>
-      </c>
-      <c r="K85" s="115" t="s">
-        <v>209</v>
       </c>
       <c r="L85" s="113">
         <v>2</v>
@@ -6198,34 +6200,34 @@
         <v>3</v>
       </c>
       <c r="B86" s="109" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C86" s="111" t="s">
         <v>97</v>
       </c>
       <c r="D86" s="111" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E86" s="112" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F86" s="112" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G86" s="113" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H86" s="113" t="s">
         <v>35</v>
       </c>
       <c r="I86" s="114" t="s">
+        <v>210</v>
+      </c>
+      <c r="J86" s="115" t="s">
         <v>211</v>
       </c>
-      <c r="J86" s="115" t="s">
+      <c r="K86" s="115" t="s">
         <v>212</v>
-      </c>
-      <c r="K86" s="115" t="s">
-        <v>213</v>
       </c>
       <c r="L86" s="113">
         <v>2</v>
@@ -6236,34 +6238,34 @@
         <v>3</v>
       </c>
       <c r="B87" s="109" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C87" s="111" t="s">
         <v>97</v>
       </c>
       <c r="D87" s="111" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E87" s="112" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F87" s="112" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G87" s="113" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H87" s="113" t="s">
         <v>35</v>
       </c>
       <c r="I87" s="114" t="s">
+        <v>213</v>
+      </c>
+      <c r="J87" s="115" t="s">
         <v>214</v>
       </c>
-      <c r="J87" s="115" t="s">
+      <c r="K87" s="115" t="s">
         <v>215</v>
-      </c>
-      <c r="K87" s="115" t="s">
-        <v>216</v>
       </c>
       <c r="L87" s="113">
         <v>2</v>
@@ -6274,34 +6276,34 @@
         <v>3</v>
       </c>
       <c r="B88" s="109" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C88" s="111" t="s">
         <v>97</v>
       </c>
       <c r="D88" s="111" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E88" s="112" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F88" s="112" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G88" s="113" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H88" s="113" t="s">
         <v>35</v>
       </c>
       <c r="I88" s="114" t="s">
+        <v>217</v>
+      </c>
+      <c r="J88" s="115" t="s">
         <v>218</v>
       </c>
-      <c r="J88" s="115" t="s">
+      <c r="K88" s="115" t="s">
         <v>219</v>
-      </c>
-      <c r="K88" s="115" t="s">
-        <v>220</v>
       </c>
       <c r="L88" s="113">
         <v>2</v>
@@ -6312,34 +6314,34 @@
         <v>3</v>
       </c>
       <c r="B89" s="109" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C89" s="111" t="s">
         <v>97</v>
       </c>
       <c r="D89" s="111" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E89" s="112" t="s">
+        <v>153</v>
+      </c>
+      <c r="F89" s="112" t="s">
         <v>154</v>
       </c>
-      <c r="F89" s="112" t="s">
-        <v>155</v>
-      </c>
       <c r="G89" s="113" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H89" s="113" t="s">
         <v>35</v>
       </c>
       <c r="I89" s="114" t="s">
+        <v>220</v>
+      </c>
+      <c r="J89" s="115" t="s">
         <v>221</v>
       </c>
-      <c r="J89" s="115" t="s">
+      <c r="K89" s="115" t="s">
         <v>222</v>
-      </c>
-      <c r="K89" s="115" t="s">
-        <v>223</v>
       </c>
       <c r="L89" s="113">
         <v>2</v>
@@ -6350,34 +6352,34 @@
         <v>3</v>
       </c>
       <c r="B90" s="21" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C90" s="111" t="s">
         <v>97</v>
       </c>
       <c r="D90" s="111" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E90" s="112" t="s">
+        <v>144</v>
+      </c>
+      <c r="F90" s="112" t="s">
         <v>145</v>
       </c>
-      <c r="F90" s="112" t="s">
-        <v>146</v>
-      </c>
       <c r="G90" s="113" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H90" s="113" t="s">
         <v>35</v>
       </c>
       <c r="I90" s="114" t="s">
+        <v>223</v>
+      </c>
+      <c r="J90" s="115" t="s">
         <v>224</v>
       </c>
-      <c r="J90" s="115" t="s">
+      <c r="K90" s="115" t="s">
         <v>225</v>
-      </c>
-      <c r="K90" s="115" t="s">
-        <v>226</v>
       </c>
       <c r="L90" s="113">
         <v>2</v>
@@ -6388,34 +6390,34 @@
         <v>3</v>
       </c>
       <c r="B91" s="21" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C91" s="111" t="s">
         <v>97</v>
       </c>
       <c r="D91" s="111" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E91" s="23" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F91" s="112" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G91" s="113" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H91" s="113" t="s">
         <v>35</v>
       </c>
       <c r="I91" s="114" t="s">
+        <v>223</v>
+      </c>
+      <c r="J91" s="115" t="s">
         <v>224</v>
       </c>
-      <c r="J91" s="115" t="s">
+      <c r="K91" s="115" t="s">
         <v>225</v>
-      </c>
-      <c r="K91" s="115" t="s">
-        <v>226</v>
       </c>
       <c r="L91" s="113">
         <v>2</v>
@@ -6426,34 +6428,34 @@
         <v>3</v>
       </c>
       <c r="B92" s="109" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C92" s="111" t="s">
         <v>97</v>
       </c>
       <c r="D92" s="110" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E92" s="112" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F92" s="112" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G92" s="113" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H92" s="113" t="s">
         <v>35</v>
       </c>
       <c r="I92" s="114" t="s">
+        <v>226</v>
+      </c>
+      <c r="J92" s="115" t="s">
         <v>227</v>
       </c>
-      <c r="J92" s="115" t="s">
+      <c r="K92" s="115" t="s">
         <v>228</v>
-      </c>
-      <c r="K92" s="115" t="s">
-        <v>229</v>
       </c>
       <c r="L92" s="113">
         <v>2</v>
@@ -6464,34 +6466,34 @@
         <v>3</v>
       </c>
       <c r="B93" s="109" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C93" s="111" t="s">
         <v>97</v>
       </c>
       <c r="D93" s="111" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E93" s="112" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F93" s="112" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G93" s="113" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H93" s="113" t="s">
         <v>35</v>
       </c>
       <c r="I93" s="114" t="s">
+        <v>230</v>
+      </c>
+      <c r="J93" s="115" t="s">
         <v>231</v>
       </c>
-      <c r="J93" s="115" t="s">
+      <c r="K93" s="115" t="s">
         <v>232</v>
-      </c>
-      <c r="K93" s="115" t="s">
-        <v>233</v>
       </c>
       <c r="L93" s="113">
         <v>2</v>
@@ -6502,34 +6504,34 @@
         <v>3</v>
       </c>
       <c r="B94" s="109" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C94" s="111" t="s">
         <v>97</v>
       </c>
       <c r="D94" s="111" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E94" s="112" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F94" s="112" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G94" s="113" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H94" s="113" t="s">
         <v>35</v>
       </c>
       <c r="I94" s="114" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="J94" s="115" t="s">
+        <v>234</v>
+      </c>
+      <c r="K94" s="115" t="s">
         <v>235</v>
-      </c>
-      <c r="K94" s="115" t="s">
-        <v>236</v>
       </c>
       <c r="L94" s="113">
         <v>2</v>
@@ -6540,34 +6542,34 @@
         <v>3</v>
       </c>
       <c r="B95" s="109" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C95" s="111" t="s">
         <v>97</v>
       </c>
       <c r="D95" s="111" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E95" s="112" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F95" s="112" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G95" s="113" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H95" s="113" t="s">
         <v>35</v>
       </c>
       <c r="I95" s="114" t="s">
+        <v>237</v>
+      </c>
+      <c r="J95" s="115" t="s">
         <v>238</v>
       </c>
-      <c r="J95" s="115" t="s">
+      <c r="K95" s="115" t="s">
         <v>239</v>
-      </c>
-      <c r="K95" s="115" t="s">
-        <v>240</v>
       </c>
       <c r="L95" s="113">
         <v>2</v>
@@ -6578,34 +6580,34 @@
         <v>3</v>
       </c>
       <c r="B96" s="109" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C96" s="111" t="s">
         <v>97</v>
       </c>
       <c r="D96" s="111" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E96" s="112" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F96" s="112" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G96" s="113" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H96" s="113" t="s">
         <v>35</v>
       </c>
       <c r="I96" s="114" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J96" s="115" t="s">
+        <v>241</v>
+      </c>
+      <c r="K96" s="115" t="s">
         <v>242</v>
-      </c>
-      <c r="K96" s="115" t="s">
-        <v>243</v>
       </c>
       <c r="L96" s="113">
         <v>2</v>
@@ -6616,34 +6618,34 @@
         <v>3</v>
       </c>
       <c r="B97" s="109" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C97" s="111" t="s">
         <v>97</v>
       </c>
       <c r="D97" s="111" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E97" s="112" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F97" s="112" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G97" s="113" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H97" s="113" t="s">
         <v>35</v>
       </c>
       <c r="I97" s="114" t="s">
+        <v>244</v>
+      </c>
+      <c r="J97" s="115" t="s">
         <v>245</v>
       </c>
-      <c r="J97" s="115" t="s">
+      <c r="K97" s="115" t="s">
         <v>246</v>
-      </c>
-      <c r="K97" s="115" t="s">
-        <v>247</v>
       </c>
       <c r="L97" s="113">
         <v>2</v>
@@ -6654,34 +6656,34 @@
         <v>3</v>
       </c>
       <c r="B98" s="109" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C98" s="111" t="s">
         <v>97</v>
       </c>
       <c r="D98" s="111" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E98" s="112" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F98" s="112" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G98" s="113" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H98" s="113" t="s">
         <v>35</v>
       </c>
       <c r="I98" s="114" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="J98" s="115" t="s">
+        <v>248</v>
+      </c>
+      <c r="K98" s="115" t="s">
         <v>249</v>
-      </c>
-      <c r="K98" s="115" t="s">
-        <v>250</v>
       </c>
       <c r="L98" s="113">
         <v>2</v>
@@ -6692,34 +6694,34 @@
         <v>3</v>
       </c>
       <c r="B99" s="109" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C99" s="111" t="s">
         <v>97</v>
       </c>
       <c r="D99" s="111" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E99" s="112" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F99" s="112" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G99" s="113" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H99" s="113" t="s">
         <v>35</v>
       </c>
       <c r="I99" s="114" t="s">
+        <v>251</v>
+      </c>
+      <c r="J99" s="115" t="s">
         <v>252</v>
       </c>
-      <c r="J99" s="115" t="s">
+      <c r="K99" s="115" t="s">
         <v>253</v>
-      </c>
-      <c r="K99" s="115" t="s">
-        <v>254</v>
       </c>
       <c r="L99" s="113">
         <v>2</v>
@@ -6730,34 +6732,34 @@
         <v>3</v>
       </c>
       <c r="B100" s="109" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C100" s="111" t="s">
         <v>97</v>
       </c>
       <c r="D100" s="111" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E100" s="112" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F100" s="112" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G100" s="113" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H100" s="113" t="s">
         <v>35</v>
       </c>
       <c r="I100" s="114" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="J100" s="115" t="s">
+        <v>255</v>
+      </c>
+      <c r="K100" s="115" t="s">
         <v>256</v>
-      </c>
-      <c r="K100" s="115" t="s">
-        <v>257</v>
       </c>
       <c r="L100" s="113">
         <v>2</v>
@@ -6768,34 +6770,34 @@
         <v>3</v>
       </c>
       <c r="B101" s="109" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C101" s="111" t="s">
         <v>97</v>
       </c>
       <c r="D101" s="111" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E101" s="112" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F101" s="112" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G101" s="113" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H101" s="113" t="s">
         <v>35</v>
       </c>
       <c r="I101" s="114" t="s">
+        <v>258</v>
+      </c>
+      <c r="J101" s="115" t="s">
         <v>259</v>
       </c>
-      <c r="J101" s="115" t="s">
+      <c r="K101" s="115" t="s">
         <v>260</v>
-      </c>
-      <c r="K101" s="115" t="s">
-        <v>261</v>
       </c>
       <c r="L101" s="113">
         <v>2</v>
@@ -6806,34 +6808,34 @@
         <v>3</v>
       </c>
       <c r="B102" s="109" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C102" s="111" t="s">
         <v>97</v>
       </c>
       <c r="D102" s="111" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E102" s="112" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F102" s="112" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G102" s="113" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H102" s="113" t="s">
         <v>35</v>
       </c>
       <c r="I102" s="114" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="J102" s="115" t="s">
+        <v>262</v>
+      </c>
+      <c r="K102" s="115" t="s">
         <v>263</v>
-      </c>
-      <c r="K102" s="115" t="s">
-        <v>264</v>
       </c>
       <c r="L102" s="113">
         <v>2</v>
@@ -6844,34 +6846,34 @@
         <v>3</v>
       </c>
       <c r="B103" s="109" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C103" s="140" t="s">
         <v>97</v>
       </c>
       <c r="D103" s="140" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E103" s="141" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F103" s="141" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G103" s="142" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H103" s="142" t="s">
         <v>35</v>
       </c>
       <c r="I103" s="47" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="J103" s="20" t="s">
+        <v>309</v>
+      </c>
+      <c r="K103" s="20" t="s">
         <v>310</v>
-      </c>
-      <c r="K103" s="20" t="s">
-        <v>311</v>
       </c>
       <c r="L103" s="142">
         <v>2</v>
@@ -6882,34 +6884,34 @@
         <v>3</v>
       </c>
       <c r="B104" s="134" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C104" s="130" t="s">
         <v>97</v>
       </c>
       <c r="D104" s="130" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E104" s="131" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F104" s="131" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G104" s="132" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H104" s="133" t="s">
         <v>35</v>
       </c>
       <c r="I104" s="135" t="s">
+        <v>264</v>
+      </c>
+      <c r="J104" s="122" t="s">
         <v>265</v>
       </c>
-      <c r="J104" s="122" t="s">
+      <c r="K104" s="122" t="s">
         <v>266</v>
-      </c>
-      <c r="K104" s="122" t="s">
-        <v>267</v>
       </c>
       <c r="L104" s="133">
         <v>3</v>
@@ -6920,34 +6922,34 @@
         <v>3</v>
       </c>
       <c r="B105" s="134" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C105" s="130" t="s">
         <v>97</v>
       </c>
       <c r="D105" s="130" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E105" s="131" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F105" s="131" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G105" s="133" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H105" s="133" t="s">
         <v>35</v>
       </c>
       <c r="I105" s="135" t="s">
+        <v>267</v>
+      </c>
+      <c r="J105" s="122" t="s">
         <v>268</v>
       </c>
-      <c r="J105" s="122" t="s">
+      <c r="K105" s="122" t="s">
         <v>269</v>
-      </c>
-      <c r="K105" s="122" t="s">
-        <v>270</v>
       </c>
       <c r="L105" s="133">
         <v>3</v>
@@ -6958,34 +6960,34 @@
         <v>3</v>
       </c>
       <c r="B106" s="134" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C106" s="130" t="s">
         <v>97</v>
       </c>
       <c r="D106" s="130" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E106" s="131" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F106" s="131" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G106" s="133" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H106" s="133" t="s">
         <v>35</v>
       </c>
       <c r="I106" s="135" t="s">
+        <v>270</v>
+      </c>
+      <c r="J106" s="122" t="s">
         <v>271</v>
       </c>
-      <c r="J106" s="122" t="s">
+      <c r="K106" s="122" t="s">
         <v>272</v>
-      </c>
-      <c r="K106" s="122" t="s">
-        <v>273</v>
       </c>
       <c r="L106" s="133">
         <v>3</v>
@@ -6996,34 +6998,34 @@
         <v>3</v>
       </c>
       <c r="B107" s="134" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C107" s="130" t="s">
         <v>97</v>
       </c>
       <c r="D107" s="130" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E107" s="131" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F107" s="131" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G107" s="133" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H107" s="133" t="s">
         <v>35</v>
       </c>
       <c r="I107" s="135" t="s">
+        <v>273</v>
+      </c>
+      <c r="J107" s="122" t="s">
         <v>274</v>
       </c>
-      <c r="J107" s="122" t="s">
+      <c r="K107" s="122" t="s">
         <v>275</v>
-      </c>
-      <c r="K107" s="122" t="s">
-        <v>276</v>
       </c>
       <c r="L107" s="133">
         <v>3</v>
@@ -7034,34 +7036,34 @@
         <v>3</v>
       </c>
       <c r="B108" s="134" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C108" s="130" t="s">
         <v>97</v>
       </c>
       <c r="D108" s="130" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E108" s="131" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F108" s="131" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G108" s="133" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H108" s="133" t="s">
         <v>35</v>
       </c>
       <c r="I108" s="135" t="s">
+        <v>276</v>
+      </c>
+      <c r="J108" s="122" t="s">
         <v>277</v>
       </c>
-      <c r="J108" s="122" t="s">
+      <c r="K108" s="122" t="s">
         <v>278</v>
-      </c>
-      <c r="K108" s="122" t="s">
-        <v>279</v>
       </c>
       <c r="L108" s="133">
         <v>3</v>
@@ -7072,34 +7074,34 @@
         <v>3</v>
       </c>
       <c r="B109" s="134" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C109" s="130" t="s">
         <v>97</v>
       </c>
       <c r="D109" s="130" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E109" s="131" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F109" s="131" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G109" s="133" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H109" s="133" t="s">
         <v>35</v>
       </c>
       <c r="I109" s="135" t="s">
+        <v>279</v>
+      </c>
+      <c r="J109" s="136" t="s">
         <v>280</v>
       </c>
-      <c r="J109" s="136" t="s">
+      <c r="K109" s="136" t="s">
         <v>281</v>
-      </c>
-      <c r="K109" s="136" t="s">
-        <v>282</v>
       </c>
       <c r="L109" s="133">
         <v>3</v>
@@ -7110,34 +7112,34 @@
         <v>3</v>
       </c>
       <c r="B110" s="129" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C110" s="130" t="s">
         <v>97</v>
       </c>
       <c r="D110" s="130" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E110" s="137" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="F110" s="137" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G110" s="133" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H110" s="133" t="s">
         <v>35</v>
       </c>
       <c r="I110" s="138" t="s">
+        <v>282</v>
+      </c>
+      <c r="J110" s="139" t="s">
         <v>283</v>
       </c>
-      <c r="J110" s="139" t="s">
+      <c r="K110" s="139" t="s">
         <v>284</v>
-      </c>
-      <c r="K110" s="139" t="s">
-        <v>285</v>
       </c>
       <c r="L110" s="133">
         <v>3</v>
@@ -7148,34 +7150,34 @@
         <v>3</v>
       </c>
       <c r="B111" s="134" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C111" s="130" t="s">
         <v>97</v>
       </c>
       <c r="D111" s="130" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E111" s="131" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="F111" s="131" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G111" s="133" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H111" s="133" t="s">
         <v>35</v>
       </c>
       <c r="I111" s="135" t="s">
+        <v>298</v>
+      </c>
+      <c r="J111" s="122" t="s">
         <v>299</v>
       </c>
-      <c r="J111" s="122" t="s">
+      <c r="K111" s="122" t="s">
         <v>300</v>
-      </c>
-      <c r="K111" s="122" t="s">
-        <v>301</v>
       </c>
       <c r="L111" s="133">
         <v>3</v>
@@ -7186,34 +7188,34 @@
         <v>3</v>
       </c>
       <c r="B112" s="134" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C112" s="130" t="s">
         <v>97</v>
       </c>
       <c r="D112" s="130" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E112" s="131" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F112" s="131" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G112" s="133" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H112" s="133" t="s">
         <v>35</v>
       </c>
       <c r="I112" s="135" t="s">
+        <v>302</v>
+      </c>
+      <c r="J112" s="136" t="s">
         <v>303</v>
       </c>
-      <c r="J112" s="136" t="s">
+      <c r="K112" s="136" t="s">
         <v>304</v>
-      </c>
-      <c r="K112" s="136" t="s">
-        <v>305</v>
       </c>
       <c r="L112" s="133">
         <v>3</v>
@@ -7224,34 +7226,34 @@
         <v>3</v>
       </c>
       <c r="B113" s="143" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C113" s="126" t="s">
         <v>97</v>
       </c>
       <c r="D113" s="126" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E113" s="144" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F113" s="144" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G113" s="120" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H113" s="120" t="s">
         <v>35</v>
       </c>
       <c r="I113" s="145" t="s">
+        <v>306</v>
+      </c>
+      <c r="J113" s="145" t="s">
         <v>307</v>
       </c>
-      <c r="J113" s="145" t="s">
+      <c r="K113" s="145" t="s">
         <v>308</v>
-      </c>
-      <c r="K113" s="145" t="s">
-        <v>309</v>
       </c>
       <c r="L113" s="120">
         <v>3</v>

</xml_diff>

<commit_message>
Tweaked a bit the transformGold power.
Former-commit-id: 28d58215ab75177afe0f89064107c0b6bfa9707a
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Powerups.xlsx
+++ b/Docs/Content/HungryDragonContent_Powerups.xlsx
@@ -3158,7 +3158,7 @@
   <dimension ref="A1:L118"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="E56" sqref="E56"/>
+      <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5133,7 +5133,7 @@
         <v>101</v>
       </c>
       <c r="E56" s="56">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F56" s="56"/>
       <c r="G56" s="28" t="s">

</xml_diff>

<commit_message>
coin_throw powerup added in content!
Former-commit-id: 83cb6cc99935f3e492051da82639c91f02ea0709
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Powerups.xlsx
+++ b/Docs/Content/HungryDragonContent_Powerups.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1095" uniqueCount="466">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1104" uniqueCount="471">
   <si>
     <t>[sku]</t>
   </si>
@@ -1422,13 +1422,28 @@
   </si>
   <si>
     <t>transformGold</t>
+  </si>
+  <si>
+    <t>coin_throw</t>
+  </si>
+  <si>
+    <t>coin_reward</t>
+  </si>
+  <si>
+    <t>TID_POWERUP_COIN_THROW_NAME</t>
+  </si>
+  <si>
+    <t>TID_POWERUP_COIN_THROW_DESC</t>
+  </si>
+  <si>
+    <t>TID_POWERUP_COIN_THROW_DESC_SHORT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1557,6 +1572,12 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1814,7 +1835,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="148">
+  <cellXfs count="152">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2237,6 +2258,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2858,8 +2891,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="powerUpsDefinitions" displayName="powerUpsDefinitions" ref="A3:L113" totalsRowShown="0" headerRowDxfId="28" dataDxfId="26" headerRowBorderDxfId="27" tableBorderDxfId="25" totalsRowBorderDxfId="24">
-  <autoFilter ref="A3:L113"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="powerUpsDefinitions" displayName="powerUpsDefinitions" ref="A3:L114" totalsRowShown="0" headerRowDxfId="28" dataDxfId="26" headerRowBorderDxfId="27" tableBorderDxfId="25" totalsRowBorderDxfId="24">
+  <autoFilter ref="A3:L114"/>
   <sortState ref="A4:K53">
     <sortCondition ref="D3:D53"/>
   </sortState>
@@ -3155,10 +3188,10 @@
   <sheetPr>
     <tabColor theme="7"/>
   </sheetPr>
-  <dimension ref="A1:L118"/>
+  <dimension ref="A1:L119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="E47" sqref="E47"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="C62" sqref="C62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5464,39 +5497,39 @@
       </c>
     </row>
     <row r="66" spans="1:12" s="87" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="117" t="s">
-        <v>3</v>
-      </c>
-      <c r="B66" s="107" t="s">
-        <v>144</v>
-      </c>
-      <c r="C66" s="118" t="s">
-        <v>50</v>
-      </c>
-      <c r="D66" s="118" t="s">
-        <v>100</v>
-      </c>
-      <c r="E66" s="119">
-        <v>150</v>
-      </c>
-      <c r="F66" s="119"/>
-      <c r="G66" s="108" t="s">
-        <v>140</v>
-      </c>
-      <c r="H66" s="120" t="s">
-        <v>44</v>
-      </c>
-      <c r="I66" s="121" t="s">
-        <v>167</v>
-      </c>
-      <c r="J66" s="122" t="s">
-        <v>168</v>
-      </c>
-      <c r="K66" s="122" t="s">
-        <v>285</v>
-      </c>
-      <c r="L66" s="120">
-        <v>1</v>
+      <c r="A66" s="88" t="s">
+        <v>3</v>
+      </c>
+      <c r="B66" s="148" t="s">
+        <v>466</v>
+      </c>
+      <c r="C66" s="149" t="s">
+        <v>467</v>
+      </c>
+      <c r="D66" s="89" t="s">
+        <v>101</v>
+      </c>
+      <c r="E66" s="150">
+        <v>5</v>
+      </c>
+      <c r="F66" s="150"/>
+      <c r="G66" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="H66" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="I66" s="92" t="s">
+        <v>468</v>
+      </c>
+      <c r="J66" s="92" t="s">
+        <v>469</v>
+      </c>
+      <c r="K66" s="92" t="s">
+        <v>470</v>
+      </c>
+      <c r="L66" s="151">
+        <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.25">
@@ -5504,7 +5537,7 @@
         <v>3</v>
       </c>
       <c r="B67" s="107" t="s">
-        <v>169</v>
+        <v>144</v>
       </c>
       <c r="C67" s="118" t="s">
         <v>50</v>
@@ -5513,7 +5546,7 @@
         <v>100</v>
       </c>
       <c r="E67" s="119">
-        <v>70</v>
+        <v>150</v>
       </c>
       <c r="F67" s="119"/>
       <c r="G67" s="108" t="s">
@@ -5540,16 +5573,16 @@
         <v>3</v>
       </c>
       <c r="B68" s="107" t="s">
-        <v>153</v>
+        <v>169</v>
       </c>
       <c r="C68" s="118" t="s">
-        <v>16</v>
+        <v>50</v>
       </c>
       <c r="D68" s="118" t="s">
         <v>100</v>
       </c>
       <c r="E68" s="119">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="F68" s="119"/>
       <c r="G68" s="108" t="s">
@@ -5559,13 +5592,13 @@
         <v>44</v>
       </c>
       <c r="I68" s="121" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="J68" s="122" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="K68" s="122" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="L68" s="120">
         <v>1</v>
@@ -5575,8 +5608,8 @@
       <c r="A69" s="117" t="s">
         <v>3</v>
       </c>
-      <c r="B69" s="123" t="s">
-        <v>172</v>
+      <c r="B69" s="107" t="s">
+        <v>153</v>
       </c>
       <c r="C69" s="118" t="s">
         <v>16</v>
@@ -5585,7 +5618,7 @@
         <v>100</v>
       </c>
       <c r="E69" s="119">
-        <v>75</v>
+        <v>100</v>
       </c>
       <c r="F69" s="119"/>
       <c r="G69" s="108" t="s">
@@ -5612,32 +5645,32 @@
         <v>3</v>
       </c>
       <c r="B70" s="123" t="s">
-        <v>151</v>
+        <v>172</v>
       </c>
       <c r="C70" s="118" t="s">
-        <v>58</v>
+        <v>16</v>
       </c>
       <c r="D70" s="118" t="s">
         <v>100</v>
       </c>
       <c r="E70" s="119">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="F70" s="119"/>
       <c r="G70" s="108" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="H70" s="120" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="I70" s="121" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="J70" s="122" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="K70" s="122" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="L70" s="120">
         <v>1</v>
@@ -5648,7 +5681,7 @@
         <v>3</v>
       </c>
       <c r="B71" s="123" t="s">
-        <v>175</v>
+        <v>151</v>
       </c>
       <c r="C71" s="118" t="s">
         <v>58</v>
@@ -5657,7 +5690,7 @@
         <v>100</v>
       </c>
       <c r="E71" s="119">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="F71" s="119"/>
       <c r="G71" s="108" t="s">
@@ -5684,15 +5717,17 @@
         <v>3</v>
       </c>
       <c r="B72" s="123" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C72" s="118" t="s">
-        <v>7</v>
+        <v>58</v>
       </c>
       <c r="D72" s="118" t="s">
-        <v>101</v>
-      </c>
-      <c r="E72" s="119"/>
+        <v>100</v>
+      </c>
+      <c r="E72" s="119">
+        <v>30</v>
+      </c>
       <c r="F72" s="119"/>
       <c r="G72" s="108" t="s">
         <v>137</v>
@@ -5701,13 +5736,13 @@
         <v>33</v>
       </c>
       <c r="I72" s="121" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="J72" s="122" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="K72" s="122" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="L72" s="120">
         <v>1</v>
@@ -5717,18 +5752,16 @@
       <c r="A73" s="117" t="s">
         <v>3</v>
       </c>
-      <c r="B73" s="107" t="s">
-        <v>145</v>
+      <c r="B73" s="123" t="s">
+        <v>176</v>
       </c>
       <c r="C73" s="118" t="s">
-        <v>32</v>
+        <v>7</v>
       </c>
       <c r="D73" s="118" t="s">
-        <v>100</v>
-      </c>
-      <c r="E73" s="119">
-        <v>25</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="E73" s="119"/>
       <c r="F73" s="119"/>
       <c r="G73" s="108" t="s">
         <v>137</v>
@@ -5737,13 +5770,13 @@
         <v>33</v>
       </c>
       <c r="I73" s="121" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="J73" s="122" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="K73" s="122" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="L73" s="120">
         <v>1</v>
@@ -5753,8 +5786,8 @@
       <c r="A74" s="117" t="s">
         <v>3</v>
       </c>
-      <c r="B74" s="123" t="s">
-        <v>181</v>
+      <c r="B74" s="107" t="s">
+        <v>145</v>
       </c>
       <c r="C74" s="118" t="s">
         <v>32</v>
@@ -5763,7 +5796,7 @@
         <v>100</v>
       </c>
       <c r="E74" s="119">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="F74" s="119"/>
       <c r="G74" s="108" t="s">
@@ -5790,34 +5823,32 @@
         <v>3</v>
       </c>
       <c r="B75" s="123" t="s">
-        <v>148</v>
+        <v>181</v>
       </c>
       <c r="C75" s="118" t="s">
-        <v>53</v>
+        <v>32</v>
       </c>
       <c r="D75" s="118" t="s">
         <v>100</v>
       </c>
-      <c r="E75" s="119" t="s">
-        <v>31</v>
-      </c>
-      <c r="F75" s="119">
-        <v>100</v>
-      </c>
+      <c r="E75" s="119">
+        <v>15</v>
+      </c>
+      <c r="F75" s="119"/>
       <c r="G75" s="108" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="H75" s="120" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="I75" s="121" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="J75" s="122" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="K75" s="122" t="s">
-        <v>184</v>
+        <v>289</v>
       </c>
       <c r="L75" s="120">
         <v>1</v>
@@ -5828,7 +5859,7 @@
         <v>3</v>
       </c>
       <c r="B76" s="123" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="C76" s="118" t="s">
         <v>53</v>
@@ -5837,10 +5868,10 @@
         <v>100</v>
       </c>
       <c r="E76" s="119" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="F76" s="119">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="G76" s="108" t="s">
         <v>142</v>
@@ -5849,13 +5880,13 @@
         <v>29</v>
       </c>
       <c r="I76" s="121" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="J76" s="122" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="K76" s="122" t="s">
-        <v>290</v>
+        <v>184</v>
       </c>
       <c r="L76" s="120">
         <v>1</v>
@@ -5866,7 +5897,7 @@
         <v>3</v>
       </c>
       <c r="B77" s="123" t="s">
-        <v>187</v>
+        <v>157</v>
       </c>
       <c r="C77" s="118" t="s">
         <v>53</v>
@@ -5878,7 +5909,7 @@
         <v>28</v>
       </c>
       <c r="F77" s="119">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="G77" s="108" t="s">
         <v>142</v>
@@ -5900,72 +5931,74 @@
       </c>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A78" s="124" t="s">
-        <v>3</v>
-      </c>
-      <c r="B78" s="125" t="s">
-        <v>159</v>
-      </c>
-      <c r="C78" s="126" t="s">
-        <v>12</v>
-      </c>
-      <c r="D78" s="126" t="s">
-        <v>100</v>
-      </c>
-      <c r="E78" s="127">
-        <v>50</v>
-      </c>
-      <c r="F78" s="127"/>
+      <c r="A78" s="117" t="s">
+        <v>3</v>
+      </c>
+      <c r="B78" s="123" t="s">
+        <v>187</v>
+      </c>
+      <c r="C78" s="118" t="s">
+        <v>53</v>
+      </c>
+      <c r="D78" s="118" t="s">
+        <v>100</v>
+      </c>
+      <c r="E78" s="119" t="s">
+        <v>28</v>
+      </c>
+      <c r="F78" s="119">
+        <v>35</v>
+      </c>
       <c r="G78" s="108" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="H78" s="120" t="s">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="I78" s="121" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="J78" s="122" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="K78" s="122" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="L78" s="120">
         <v>1</v>
       </c>
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A79" s="117" t="s">
-        <v>3</v>
-      </c>
-      <c r="B79" s="123" t="s">
-        <v>154</v>
-      </c>
-      <c r="C79" s="118" t="s">
-        <v>51</v>
-      </c>
-      <c r="D79" s="118" t="s">
-        <v>100</v>
-      </c>
-      <c r="E79" s="119">
-        <v>25</v>
-      </c>
-      <c r="F79" s="119"/>
+      <c r="A79" s="124" t="s">
+        <v>3</v>
+      </c>
+      <c r="B79" s="125" t="s">
+        <v>159</v>
+      </c>
+      <c r="C79" s="126" t="s">
+        <v>12</v>
+      </c>
+      <c r="D79" s="126" t="s">
+        <v>100</v>
+      </c>
+      <c r="E79" s="127">
+        <v>50</v>
+      </c>
+      <c r="F79" s="127"/>
       <c r="G79" s="108" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="H79" s="120" t="s">
-        <v>46</v>
+        <v>5</v>
       </c>
       <c r="I79" s="121" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="J79" s="122" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="K79" s="122" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="L79" s="120">
         <v>1</v>
@@ -5976,7 +6009,7 @@
         <v>3</v>
       </c>
       <c r="B80" s="123" t="s">
-        <v>192</v>
+        <v>154</v>
       </c>
       <c r="C80" s="118" t="s">
         <v>51</v>
@@ -5985,7 +6018,7 @@
         <v>100</v>
       </c>
       <c r="E80" s="119">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="F80" s="119"/>
       <c r="G80" s="108" t="s">
@@ -6008,77 +6041,75 @@
       </c>
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A81" s="128" t="s">
-        <v>3</v>
-      </c>
-      <c r="B81" s="129" t="s">
+      <c r="A81" s="117" t="s">
+        <v>3</v>
+      </c>
+      <c r="B81" s="123" t="s">
+        <v>192</v>
+      </c>
+      <c r="C81" s="118" t="s">
+        <v>51</v>
+      </c>
+      <c r="D81" s="118" t="s">
+        <v>100</v>
+      </c>
+      <c r="E81" s="119">
+        <v>15</v>
+      </c>
+      <c r="F81" s="119"/>
+      <c r="G81" s="108" t="s">
+        <v>141</v>
+      </c>
+      <c r="H81" s="120" t="s">
+        <v>46</v>
+      </c>
+      <c r="I81" s="121" t="s">
+        <v>190</v>
+      </c>
+      <c r="J81" s="122" t="s">
+        <v>191</v>
+      </c>
+      <c r="K81" s="122" t="s">
+        <v>292</v>
+      </c>
+      <c r="L81" s="120">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A82" s="128" t="s">
+        <v>3</v>
+      </c>
+      <c r="B82" s="129" t="s">
         <v>146</v>
       </c>
-      <c r="C81" s="130" t="s">
+      <c r="C82" s="130" t="s">
         <v>34</v>
       </c>
-      <c r="D81" s="130" t="s">
-        <v>100</v>
-      </c>
-      <c r="E81" s="131">
+      <c r="D82" s="130" t="s">
+        <v>100</v>
+      </c>
+      <c r="E82" s="131">
         <v>20</v>
       </c>
-      <c r="F81" s="131"/>
-      <c r="G81" s="132" t="s">
+      <c r="F82" s="131"/>
+      <c r="G82" s="132" t="s">
         <v>138</v>
       </c>
-      <c r="H81" s="133" t="s">
+      <c r="H82" s="133" t="s">
         <v>5</v>
       </c>
-      <c r="I81" s="121" t="s">
+      <c r="I82" s="121" t="s">
         <v>193</v>
       </c>
-      <c r="J81" s="122" t="s">
+      <c r="J82" s="122" t="s">
         <v>194</v>
       </c>
-      <c r="K81" s="122" t="s">
+      <c r="K82" s="122" t="s">
         <v>293</v>
       </c>
-      <c r="L81" s="133">
+      <c r="L82" s="133">
         <v>1</v>
-      </c>
-    </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A82" s="116" t="s">
-        <v>3</v>
-      </c>
-      <c r="B82" s="109" t="s">
-        <v>195</v>
-      </c>
-      <c r="C82" s="111" t="s">
-        <v>97</v>
-      </c>
-      <c r="D82" s="111" t="s">
-        <v>100</v>
-      </c>
-      <c r="E82" s="112" t="s">
-        <v>151</v>
-      </c>
-      <c r="F82" s="112" t="s">
-        <v>153</v>
-      </c>
-      <c r="G82" s="46" t="s">
-        <v>143</v>
-      </c>
-      <c r="H82" s="113" t="s">
-        <v>35</v>
-      </c>
-      <c r="I82" s="114" t="s">
-        <v>196</v>
-      </c>
-      <c r="J82" s="115" t="s">
-        <v>197</v>
-      </c>
-      <c r="K82" s="115" t="s">
-        <v>198</v>
-      </c>
-      <c r="L82" s="113">
-        <v>2</v>
       </c>
     </row>
     <row r="83" spans="1:12" x14ac:dyDescent="0.25">
@@ -6086,7 +6117,7 @@
         <v>3</v>
       </c>
       <c r="B83" s="109" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="C83" s="111" t="s">
         <v>97</v>
@@ -6095,12 +6126,12 @@
         <v>100</v>
       </c>
       <c r="E83" s="112" t="s">
-        <v>175</v>
+        <v>151</v>
       </c>
       <c r="F83" s="112" t="s">
-        <v>172</v>
-      </c>
-      <c r="G83" s="113" t="s">
+        <v>153</v>
+      </c>
+      <c r="G83" s="46" t="s">
         <v>143</v>
       </c>
       <c r="H83" s="113" t="s">
@@ -6110,10 +6141,10 @@
         <v>196</v>
       </c>
       <c r="J83" s="115" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="K83" s="115" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="L83" s="113">
         <v>2</v>
@@ -6124,7 +6155,7 @@
         <v>3</v>
       </c>
       <c r="B84" s="109" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="C84" s="111" t="s">
         <v>97</v>
@@ -6133,10 +6164,10 @@
         <v>100</v>
       </c>
       <c r="E84" s="112" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F84" s="112" t="s">
-        <v>146</v>
+        <v>172</v>
       </c>
       <c r="G84" s="113" t="s">
         <v>143</v>
@@ -6145,13 +6176,13 @@
         <v>35</v>
       </c>
       <c r="I84" s="114" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="J84" s="115" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="K84" s="115" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="L84" s="113">
         <v>2</v>
@@ -6162,19 +6193,19 @@
         <v>3</v>
       </c>
       <c r="B85" s="109" t="s">
-        <v>150</v>
+        <v>202</v>
       </c>
       <c r="C85" s="111" t="s">
         <v>97</v>
       </c>
-      <c r="D85" s="110" t="s">
+      <c r="D85" s="111" t="s">
         <v>100</v>
       </c>
       <c r="E85" s="112" t="s">
         <v>176</v>
       </c>
       <c r="F85" s="112" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="G85" s="113" t="s">
         <v>143</v>
@@ -6183,13 +6214,13 @@
         <v>35</v>
       </c>
       <c r="I85" s="114" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="J85" s="115" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="K85" s="115" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="L85" s="113">
         <v>2</v>
@@ -6200,19 +6231,19 @@
         <v>3</v>
       </c>
       <c r="B86" s="109" t="s">
-        <v>209</v>
+        <v>150</v>
       </c>
       <c r="C86" s="111" t="s">
         <v>97</v>
       </c>
-      <c r="D86" s="111" t="s">
+      <c r="D86" s="110" t="s">
         <v>100</v>
       </c>
       <c r="E86" s="112" t="s">
-        <v>151</v>
+        <v>176</v>
       </c>
       <c r="F86" s="112" t="s">
-        <v>159</v>
+        <v>144</v>
       </c>
       <c r="G86" s="113" t="s">
         <v>143</v>
@@ -6221,13 +6252,13 @@
         <v>35</v>
       </c>
       <c r="I86" s="114" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="J86" s="115" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="K86" s="115" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="L86" s="113">
         <v>2</v>
@@ -6238,7 +6269,7 @@
         <v>3</v>
       </c>
       <c r="B87" s="109" t="s">
-        <v>149</v>
+        <v>209</v>
       </c>
       <c r="C87" s="111" t="s">
         <v>97</v>
@@ -6247,10 +6278,10 @@
         <v>100</v>
       </c>
       <c r="E87" s="112" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="F87" s="112" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="G87" s="113" t="s">
         <v>143</v>
@@ -6259,13 +6290,13 @@
         <v>35</v>
       </c>
       <c r="I87" s="114" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="J87" s="115" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="K87" s="115" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="L87" s="113">
         <v>2</v>
@@ -6276,7 +6307,7 @@
         <v>3</v>
       </c>
       <c r="B88" s="109" t="s">
-        <v>216</v>
+        <v>149</v>
       </c>
       <c r="C88" s="111" t="s">
         <v>97</v>
@@ -6285,10 +6316,10 @@
         <v>100</v>
       </c>
       <c r="E88" s="112" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="F88" s="112" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="G88" s="113" t="s">
         <v>143</v>
@@ -6297,13 +6328,13 @@
         <v>35</v>
       </c>
       <c r="I88" s="114" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="J88" s="115" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="K88" s="115" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="L88" s="113">
         <v>2</v>
@@ -6314,7 +6345,7 @@
         <v>3</v>
       </c>
       <c r="B89" s="109" t="s">
-        <v>155</v>
+        <v>216</v>
       </c>
       <c r="C89" s="111" t="s">
         <v>97</v>
@@ -6323,10 +6354,10 @@
         <v>100</v>
       </c>
       <c r="E89" s="112" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="F89" s="112" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="G89" s="113" t="s">
         <v>143</v>
@@ -6335,13 +6366,13 @@
         <v>35</v>
       </c>
       <c r="I89" s="114" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="J89" s="115" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="K89" s="115" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="L89" s="113">
         <v>2</v>
@@ -6351,8 +6382,8 @@
       <c r="A90" s="116" t="s">
         <v>3</v>
       </c>
-      <c r="B90" s="21" t="s">
-        <v>156</v>
+      <c r="B90" s="109" t="s">
+        <v>155</v>
       </c>
       <c r="C90" s="111" t="s">
         <v>97</v>
@@ -6361,10 +6392,10 @@
         <v>100</v>
       </c>
       <c r="E90" s="112" t="s">
-        <v>144</v>
+        <v>153</v>
       </c>
       <c r="F90" s="112" t="s">
-        <v>145</v>
+        <v>154</v>
       </c>
       <c r="G90" s="113" t="s">
         <v>143</v>
@@ -6373,13 +6404,13 @@
         <v>35</v>
       </c>
       <c r="I90" s="114" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="J90" s="115" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="K90" s="115" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="L90" s="113">
         <v>2</v>
@@ -6390,7 +6421,7 @@
         <v>3</v>
       </c>
       <c r="B91" s="21" t="s">
-        <v>311</v>
+        <v>156</v>
       </c>
       <c r="C91" s="111" t="s">
         <v>97</v>
@@ -6398,8 +6429,8 @@
       <c r="D91" s="111" t="s">
         <v>100</v>
       </c>
-      <c r="E91" s="23" t="s">
-        <v>169</v>
+      <c r="E91" s="112" t="s">
+        <v>144</v>
       </c>
       <c r="F91" s="112" t="s">
         <v>145</v>
@@ -6427,17 +6458,17 @@
       <c r="A92" s="116" t="s">
         <v>3</v>
       </c>
-      <c r="B92" s="109" t="s">
-        <v>152</v>
+      <c r="B92" s="21" t="s">
+        <v>311</v>
       </c>
       <c r="C92" s="111" t="s">
         <v>97</v>
       </c>
-      <c r="D92" s="110" t="s">
-        <v>100</v>
-      </c>
-      <c r="E92" s="112" t="s">
-        <v>151</v>
+      <c r="D92" s="111" t="s">
+        <v>100</v>
+      </c>
+      <c r="E92" s="23" t="s">
+        <v>169</v>
       </c>
       <c r="F92" s="112" t="s">
         <v>145</v>
@@ -6449,13 +6480,13 @@
         <v>35</v>
       </c>
       <c r="I92" s="114" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="J92" s="115" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="K92" s="115" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="L92" s="113">
         <v>2</v>
@@ -6466,19 +6497,19 @@
         <v>3</v>
       </c>
       <c r="B93" s="109" t="s">
-        <v>229</v>
+        <v>152</v>
       </c>
       <c r="C93" s="111" t="s">
         <v>97</v>
       </c>
-      <c r="D93" s="111" t="s">
+      <c r="D93" s="110" t="s">
         <v>100</v>
       </c>
       <c r="E93" s="112" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="F93" s="112" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="G93" s="113" t="s">
         <v>143</v>
@@ -6487,13 +6518,13 @@
         <v>35</v>
       </c>
       <c r="I93" s="114" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="J93" s="115" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="K93" s="115" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="L93" s="113">
         <v>2</v>
@@ -6504,7 +6535,7 @@
         <v>3</v>
       </c>
       <c r="B94" s="109" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="C94" s="111" t="s">
         <v>97</v>
@@ -6516,7 +6547,7 @@
         <v>148</v>
       </c>
       <c r="F94" s="112" t="s">
-        <v>192</v>
+        <v>154</v>
       </c>
       <c r="G94" s="113" t="s">
         <v>143</v>
@@ -6528,10 +6559,10 @@
         <v>230</v>
       </c>
       <c r="J94" s="115" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="K94" s="115" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="L94" s="113">
         <v>2</v>
@@ -6542,7 +6573,7 @@
         <v>3</v>
       </c>
       <c r="B95" s="109" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="C95" s="111" t="s">
         <v>97</v>
@@ -6551,10 +6582,10 @@
         <v>100</v>
       </c>
       <c r="E95" s="112" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="F95" s="112" t="s">
-        <v>159</v>
+        <v>192</v>
       </c>
       <c r="G95" s="113" t="s">
         <v>143</v>
@@ -6563,13 +6594,13 @@
         <v>35</v>
       </c>
       <c r="I95" s="114" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="J95" s="115" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="K95" s="115" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="L95" s="113">
         <v>2</v>
@@ -6580,7 +6611,7 @@
         <v>3</v>
       </c>
       <c r="B96" s="109" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="C96" s="111" t="s">
         <v>97</v>
@@ -6589,7 +6620,7 @@
         <v>100</v>
       </c>
       <c r="E96" s="112" t="s">
-        <v>187</v>
+        <v>157</v>
       </c>
       <c r="F96" s="112" t="s">
         <v>159</v>
@@ -6604,10 +6635,10 @@
         <v>237</v>
       </c>
       <c r="J96" s="115" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="K96" s="115" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="L96" s="113">
         <v>2</v>
@@ -6618,7 +6649,7 @@
         <v>3</v>
       </c>
       <c r="B97" s="109" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="C97" s="111" t="s">
         <v>97</v>
@@ -6627,10 +6658,10 @@
         <v>100</v>
       </c>
       <c r="E97" s="112" t="s">
-        <v>157</v>
+        <v>187</v>
       </c>
       <c r="F97" s="112" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="G97" s="113" t="s">
         <v>143</v>
@@ -6639,13 +6670,13 @@
         <v>35</v>
       </c>
       <c r="I97" s="114" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="J97" s="115" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="K97" s="115" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="L97" s="113">
         <v>2</v>
@@ -6656,7 +6687,7 @@
         <v>3</v>
       </c>
       <c r="B98" s="109" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="C98" s="111" t="s">
         <v>97</v>
@@ -6665,10 +6696,10 @@
         <v>100</v>
       </c>
       <c r="E98" s="112" t="s">
-        <v>187</v>
+        <v>157</v>
       </c>
       <c r="F98" s="112" t="s">
-        <v>172</v>
+        <v>153</v>
       </c>
       <c r="G98" s="113" t="s">
         <v>143</v>
@@ -6680,10 +6711,10 @@
         <v>244</v>
       </c>
       <c r="J98" s="115" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="K98" s="115" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="L98" s="113">
         <v>2</v>
@@ -6694,7 +6725,7 @@
         <v>3</v>
       </c>
       <c r="B99" s="109" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="C99" s="111" t="s">
         <v>97</v>
@@ -6703,10 +6734,10 @@
         <v>100</v>
       </c>
       <c r="E99" s="112" t="s">
-        <v>144</v>
+        <v>187</v>
       </c>
       <c r="F99" s="112" t="s">
-        <v>157</v>
+        <v>172</v>
       </c>
       <c r="G99" s="113" t="s">
         <v>143</v>
@@ -6715,13 +6746,13 @@
         <v>35</v>
       </c>
       <c r="I99" s="114" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="J99" s="115" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="K99" s="115" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="L99" s="113">
         <v>2</v>
@@ -6732,7 +6763,7 @@
         <v>3</v>
       </c>
       <c r="B100" s="109" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="C100" s="111" t="s">
         <v>97</v>
@@ -6741,10 +6772,10 @@
         <v>100</v>
       </c>
       <c r="E100" s="112" t="s">
-        <v>169</v>
+        <v>144</v>
       </c>
       <c r="F100" s="112" t="s">
-        <v>187</v>
+        <v>157</v>
       </c>
       <c r="G100" s="113" t="s">
         <v>143</v>
@@ -6756,10 +6787,10 @@
         <v>251</v>
       </c>
       <c r="J100" s="115" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="K100" s="115" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="L100" s="113">
         <v>2</v>
@@ -6770,7 +6801,7 @@
         <v>3</v>
       </c>
       <c r="B101" s="109" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="C101" s="111" t="s">
         <v>97</v>
@@ -6779,10 +6810,10 @@
         <v>100</v>
       </c>
       <c r="E101" s="112" t="s">
-        <v>148</v>
+        <v>169</v>
       </c>
       <c r="F101" s="112" t="s">
-        <v>157</v>
+        <v>187</v>
       </c>
       <c r="G101" s="113" t="s">
         <v>143</v>
@@ -6791,13 +6822,13 @@
         <v>35</v>
       </c>
       <c r="I101" s="114" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="J101" s="115" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="K101" s="115" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="L101" s="113">
         <v>2</v>
@@ -6808,7 +6839,7 @@
         <v>3</v>
       </c>
       <c r="B102" s="109" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="C102" s="111" t="s">
         <v>97</v>
@@ -6820,7 +6851,7 @@
         <v>148</v>
       </c>
       <c r="F102" s="112" t="s">
-        <v>187</v>
+        <v>157</v>
       </c>
       <c r="G102" s="113" t="s">
         <v>143</v>
@@ -6832,89 +6863,89 @@
         <v>258</v>
       </c>
       <c r="J102" s="115" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="K102" s="115" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="L102" s="113">
         <v>2</v>
       </c>
     </row>
     <row r="103" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A103" s="45" t="s">
+      <c r="A103" s="116" t="s">
         <v>3</v>
       </c>
       <c r="B103" s="109" t="s">
+        <v>261</v>
+      </c>
+      <c r="C103" s="111" t="s">
+        <v>97</v>
+      </c>
+      <c r="D103" s="111" t="s">
+        <v>100</v>
+      </c>
+      <c r="E103" s="112" t="s">
+        <v>148</v>
+      </c>
+      <c r="F103" s="112" t="s">
+        <v>187</v>
+      </c>
+      <c r="G103" s="113" t="s">
+        <v>143</v>
+      </c>
+      <c r="H103" s="113" t="s">
+        <v>35</v>
+      </c>
+      <c r="I103" s="114" t="s">
+        <v>258</v>
+      </c>
+      <c r="J103" s="115" t="s">
+        <v>262</v>
+      </c>
+      <c r="K103" s="115" t="s">
+        <v>263</v>
+      </c>
+      <c r="L103" s="113">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A104" s="45" t="s">
+        <v>3</v>
+      </c>
+      <c r="B104" s="109" t="s">
         <v>297</v>
       </c>
-      <c r="C103" s="140" t="s">
+      <c r="C104" s="140" t="s">
         <v>97</v>
       </c>
-      <c r="D103" s="140" t="s">
-        <v>100</v>
-      </c>
-      <c r="E103" s="141" t="s">
+      <c r="D104" s="140" t="s">
+        <v>100</v>
+      </c>
+      <c r="E104" s="141" t="s">
         <v>151</v>
       </c>
-      <c r="F103" s="141" t="s">
+      <c r="F104" s="141" t="s">
         <v>154</v>
       </c>
-      <c r="G103" s="142" t="s">
+      <c r="G104" s="142" t="s">
         <v>143</v>
       </c>
-      <c r="H103" s="142" t="s">
+      <c r="H104" s="142" t="s">
         <v>35</v>
       </c>
-      <c r="I103" s="47" t="s">
+      <c r="I104" s="47" t="s">
         <v>282</v>
       </c>
-      <c r="J103" s="20" t="s">
+      <c r="J104" s="20" t="s">
         <v>309</v>
       </c>
-      <c r="K103" s="20" t="s">
+      <c r="K104" s="20" t="s">
         <v>310</v>
       </c>
-      <c r="L103" s="142">
+      <c r="L104" s="142">
         <v>2</v>
-      </c>
-    </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A104" s="128" t="s">
-        <v>3</v>
-      </c>
-      <c r="B104" s="134" t="s">
-        <v>158</v>
-      </c>
-      <c r="C104" s="130" t="s">
-        <v>97</v>
-      </c>
-      <c r="D104" s="130" t="s">
-        <v>100</v>
-      </c>
-      <c r="E104" s="131" t="s">
-        <v>247</v>
-      </c>
-      <c r="F104" s="131" t="s">
-        <v>146</v>
-      </c>
-      <c r="G104" s="132" t="s">
-        <v>143</v>
-      </c>
-      <c r="H104" s="133" t="s">
-        <v>35</v>
-      </c>
-      <c r="I104" s="135" t="s">
-        <v>264</v>
-      </c>
-      <c r="J104" s="122" t="s">
-        <v>265</v>
-      </c>
-      <c r="K104" s="122" t="s">
-        <v>266</v>
-      </c>
-      <c r="L104" s="133">
-        <v>3</v>
       </c>
     </row>
     <row r="105" spans="1:12" x14ac:dyDescent="0.25">
@@ -6922,7 +6953,7 @@
         <v>3</v>
       </c>
       <c r="B105" s="134" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C105" s="130" t="s">
         <v>97</v>
@@ -6931,25 +6962,25 @@
         <v>100</v>
       </c>
       <c r="E105" s="131" t="s">
-        <v>261</v>
+        <v>247</v>
       </c>
       <c r="F105" s="131" t="s">
-        <v>159</v>
-      </c>
-      <c r="G105" s="133" t="s">
+        <v>146</v>
+      </c>
+      <c r="G105" s="132" t="s">
         <v>143</v>
       </c>
       <c r="H105" s="133" t="s">
         <v>35</v>
       </c>
       <c r="I105" s="135" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="J105" s="122" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="K105" s="122" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="L105" s="133">
         <v>3</v>
@@ -6960,7 +6991,7 @@
         <v>3</v>
       </c>
       <c r="B106" s="134" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C106" s="130" t="s">
         <v>97</v>
@@ -6969,10 +7000,10 @@
         <v>100</v>
       </c>
       <c r="E106" s="131" t="s">
-        <v>199</v>
+        <v>261</v>
       </c>
       <c r="F106" s="131" t="s">
-        <v>187</v>
+        <v>159</v>
       </c>
       <c r="G106" s="133" t="s">
         <v>143</v>
@@ -6981,13 +7012,13 @@
         <v>35</v>
       </c>
       <c r="I106" s="135" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="J106" s="122" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="K106" s="122" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="L106" s="133">
         <v>3</v>
@@ -6998,7 +7029,7 @@
         <v>3</v>
       </c>
       <c r="B107" s="134" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C107" s="130" t="s">
         <v>97</v>
@@ -7007,10 +7038,10 @@
         <v>100</v>
       </c>
       <c r="E107" s="131" t="s">
-        <v>254</v>
+        <v>199</v>
       </c>
       <c r="F107" s="131" t="s">
-        <v>159</v>
+        <v>187</v>
       </c>
       <c r="G107" s="133" t="s">
         <v>143</v>
@@ -7019,13 +7050,13 @@
         <v>35</v>
       </c>
       <c r="I107" s="135" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="J107" s="122" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="K107" s="122" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="L107" s="133">
         <v>3</v>
@@ -7036,7 +7067,7 @@
         <v>3</v>
       </c>
       <c r="B108" s="134" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C108" s="130" t="s">
         <v>97</v>
@@ -7045,10 +7076,10 @@
         <v>100</v>
       </c>
       <c r="E108" s="131" t="s">
-        <v>240</v>
+        <v>254</v>
       </c>
       <c r="F108" s="131" t="s">
-        <v>192</v>
+        <v>159</v>
       </c>
       <c r="G108" s="133" t="s">
         <v>143</v>
@@ -7057,13 +7088,13 @@
         <v>35</v>
       </c>
       <c r="I108" s="135" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="J108" s="122" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="K108" s="122" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="L108" s="133">
         <v>3</v>
@@ -7074,7 +7105,7 @@
         <v>3</v>
       </c>
       <c r="B109" s="134" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C109" s="130" t="s">
         <v>97</v>
@@ -7083,10 +7114,10 @@
         <v>100</v>
       </c>
       <c r="E109" s="131" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="F109" s="131" t="s">
-        <v>181</v>
+        <v>192</v>
       </c>
       <c r="G109" s="133" t="s">
         <v>143</v>
@@ -7095,13 +7126,13 @@
         <v>35</v>
       </c>
       <c r="I109" s="135" t="s">
-        <v>279</v>
-      </c>
-      <c r="J109" s="136" t="s">
-        <v>280</v>
-      </c>
-      <c r="K109" s="136" t="s">
-        <v>281</v>
+        <v>276</v>
+      </c>
+      <c r="J109" s="122" t="s">
+        <v>277</v>
+      </c>
+      <c r="K109" s="122" t="s">
+        <v>278</v>
       </c>
       <c r="L109" s="133">
         <v>3</v>
@@ -7111,8 +7142,8 @@
       <c r="A110" s="128" t="s">
         <v>3</v>
       </c>
-      <c r="B110" s="129" t="s">
-        <v>147</v>
+      <c r="B110" s="134" t="s">
+        <v>164</v>
       </c>
       <c r="C110" s="130" t="s">
         <v>97</v>
@@ -7120,11 +7151,11 @@
       <c r="D110" s="130" t="s">
         <v>100</v>
       </c>
-      <c r="E110" s="137" t="s">
-        <v>311</v>
-      </c>
-      <c r="F110" s="137" t="s">
-        <v>146</v>
+      <c r="E110" s="131" t="s">
+        <v>233</v>
+      </c>
+      <c r="F110" s="131" t="s">
+        <v>181</v>
       </c>
       <c r="G110" s="133" t="s">
         <v>143</v>
@@ -7132,14 +7163,14 @@
       <c r="H110" s="133" t="s">
         <v>35</v>
       </c>
-      <c r="I110" s="138" t="s">
-        <v>282</v>
-      </c>
-      <c r="J110" s="139" t="s">
-        <v>283</v>
-      </c>
-      <c r="K110" s="139" t="s">
-        <v>284</v>
+      <c r="I110" s="135" t="s">
+        <v>279</v>
+      </c>
+      <c r="J110" s="136" t="s">
+        <v>280</v>
+      </c>
+      <c r="K110" s="136" t="s">
+        <v>281</v>
       </c>
       <c r="L110" s="133">
         <v>3</v>
@@ -7149,8 +7180,8 @@
       <c r="A111" s="128" t="s">
         <v>3</v>
       </c>
-      <c r="B111" s="134" t="s">
-        <v>296</v>
+      <c r="B111" s="129" t="s">
+        <v>147</v>
       </c>
       <c r="C111" s="130" t="s">
         <v>97</v>
@@ -7158,11 +7189,11 @@
       <c r="D111" s="130" t="s">
         <v>100</v>
       </c>
-      <c r="E111" s="131" t="s">
-        <v>297</v>
-      </c>
-      <c r="F111" s="131" t="s">
-        <v>157</v>
+      <c r="E111" s="137" t="s">
+        <v>311</v>
+      </c>
+      <c r="F111" s="137" t="s">
+        <v>146</v>
       </c>
       <c r="G111" s="133" t="s">
         <v>143</v>
@@ -7170,14 +7201,14 @@
       <c r="H111" s="133" t="s">
         <v>35</v>
       </c>
-      <c r="I111" s="135" t="s">
-        <v>298</v>
-      </c>
-      <c r="J111" s="122" t="s">
-        <v>299</v>
-      </c>
-      <c r="K111" s="122" t="s">
-        <v>300</v>
+      <c r="I111" s="138" t="s">
+        <v>282</v>
+      </c>
+      <c r="J111" s="139" t="s">
+        <v>283</v>
+      </c>
+      <c r="K111" s="139" t="s">
+        <v>284</v>
       </c>
       <c r="L111" s="133">
         <v>3</v>
@@ -7188,7 +7219,7 @@
         <v>3</v>
       </c>
       <c r="B112" s="134" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="C112" s="130" t="s">
         <v>97</v>
@@ -7197,10 +7228,10 @@
         <v>100</v>
       </c>
       <c r="E112" s="131" t="s">
-        <v>156</v>
+        <v>297</v>
       </c>
       <c r="F112" s="131" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="G112" s="133" t="s">
         <v>143</v>
@@ -7209,100 +7240,138 @@
         <v>35</v>
       </c>
       <c r="I112" s="135" t="s">
+        <v>298</v>
+      </c>
+      <c r="J112" s="122" t="s">
+        <v>299</v>
+      </c>
+      <c r="K112" s="122" t="s">
+        <v>300</v>
+      </c>
+      <c r="L112" s="133">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="113" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A113" s="128" t="s">
+        <v>3</v>
+      </c>
+      <c r="B113" s="134" t="s">
+        <v>301</v>
+      </c>
+      <c r="C113" s="130" t="s">
+        <v>97</v>
+      </c>
+      <c r="D113" s="130" t="s">
+        <v>100</v>
+      </c>
+      <c r="E113" s="131" t="s">
+        <v>156</v>
+      </c>
+      <c r="F113" s="131" t="s">
+        <v>151</v>
+      </c>
+      <c r="G113" s="133" t="s">
+        <v>143</v>
+      </c>
+      <c r="H113" s="133" t="s">
+        <v>35</v>
+      </c>
+      <c r="I113" s="135" t="s">
         <v>302</v>
       </c>
-      <c r="J112" s="136" t="s">
+      <c r="J113" s="136" t="s">
         <v>303</v>
       </c>
-      <c r="K112" s="136" t="s">
+      <c r="K113" s="136" t="s">
         <v>304</v>
       </c>
-      <c r="L112" s="133">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A113" s="146" t="s">
-        <v>3</v>
-      </c>
-      <c r="B113" s="143" t="s">
+      <c r="L113" s="133">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A114" s="146" t="s">
+        <v>3</v>
+      </c>
+      <c r="B114" s="143" t="s">
         <v>305</v>
       </c>
-      <c r="C113" s="126" t="s">
+      <c r="C114" s="126" t="s">
         <v>97</v>
       </c>
-      <c r="D113" s="126" t="s">
-        <v>100</v>
-      </c>
-      <c r="E113" s="144" t="s">
+      <c r="D114" s="126" t="s">
+        <v>100</v>
+      </c>
+      <c r="E114" s="144" t="s">
         <v>155</v>
       </c>
-      <c r="F113" s="144" t="s">
+      <c r="F114" s="144" t="s">
         <v>146</v>
       </c>
-      <c r="G113" s="120" t="s">
+      <c r="G114" s="120" t="s">
         <v>143</v>
       </c>
-      <c r="H113" s="120" t="s">
+      <c r="H114" s="120" t="s">
         <v>35</v>
       </c>
-      <c r="I113" s="145" t="s">
+      <c r="I114" s="145" t="s">
         <v>306</v>
       </c>
-      <c r="J113" s="145" t="s">
+      <c r="J114" s="145" t="s">
         <v>307</v>
       </c>
-      <c r="K113" s="145" t="s">
+      <c r="K114" s="145" t="s">
         <v>308</v>
       </c>
-      <c r="L113" s="120">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="114" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="115" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A115" s="1" t="s">
+      <c r="L114" s="120">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="115" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="116" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A116" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B115" s="1"/>
-      <c r="C115" s="1"/>
-      <c r="D115" s="1"/>
-      <c r="E115" s="1"/>
-      <c r="F115" s="1"/>
-      <c r="G115" s="1"/>
-      <c r="H115" s="1"/>
-    </row>
-    <row r="117" spans="1:12" ht="136.5" x14ac:dyDescent="0.25">
-      <c r="A117" s="2" t="s">
+      <c r="B116" s="1"/>
+      <c r="C116" s="1"/>
+      <c r="D116" s="1"/>
+      <c r="E116" s="1"/>
+      <c r="F116" s="1"/>
+      <c r="G116" s="1"/>
+      <c r="H116" s="1"/>
+    </row>
+    <row r="118" spans="1:12" ht="136.5" x14ac:dyDescent="0.25">
+      <c r="A118" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="B117" s="2" t="s">
+      <c r="B118" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C117" s="50" t="s">
+      <c r="C118" s="50" t="s">
         <v>90</v>
       </c>
-      <c r="D117" s="51" t="s">
+      <c r="D118" s="51" t="s">
         <v>91</v>
       </c>
-      <c r="E117" s="51" t="s">
+      <c r="E118" s="51" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A118" s="52" t="s">
-        <v>3</v>
-      </c>
-      <c r="B118" s="4" t="s">
+    <row r="119" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A119" s="52" t="s">
+        <v>3</v>
+      </c>
+      <c r="B119" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="C118" s="3">
+      <c r="C119" s="3">
         <v>11</v>
       </c>
-      <c r="D118" s="5">
+      <c r="D119" s="5">
         <v>2.2999999999999998</v>
       </c>
-      <c r="E118" s="5">
+      <c r="E119" s="5">
         <v>0.25</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixing color and icon for pet Shu
Former-commit-id: 49eabed67abf4257dd6adcbf69ad29c6d8be443e
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Powerups.xlsx
+++ b/Docs/Content/HungryDragonContent_Powerups.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\dragon\client\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\client\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="powerups" sheetId="6" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" calcOnSave="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1578,6 +1578,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1835,7 +1836,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="152">
+  <cellXfs count="150">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2258,12 +2259,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3190,8 +3185,8 @@
   </sheetPr>
   <dimension ref="A1:L119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="C62" sqref="C62"/>
+    <sheetView tabSelected="1" topLeftCell="C37" workbookViewId="0">
+      <selection activeCell="G65" sqref="G65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5477,7 +5472,7 @@
         <v>1</v>
       </c>
       <c r="F65" s="104"/>
-      <c r="G65" s="105" t="s">
+      <c r="G65" s="91" t="s">
         <v>143</v>
       </c>
       <c r="H65" s="105" t="s">
@@ -5500,21 +5495,21 @@
       <c r="A66" s="88" t="s">
         <v>3</v>
       </c>
-      <c r="B66" s="148" t="s">
+      <c r="B66" s="21" t="s">
         <v>466</v>
       </c>
-      <c r="C66" s="149" t="s">
+      <c r="C66" s="22" t="s">
         <v>467</v>
       </c>
       <c r="D66" s="89" t="s">
         <v>101</v>
       </c>
-      <c r="E66" s="150">
+      <c r="E66" s="148">
         <v>5</v>
       </c>
-      <c r="F66" s="150"/>
+      <c r="F66" s="148"/>
       <c r="G66" s="18" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="H66" s="18" t="s">
         <v>5</v>
@@ -5528,7 +5523,7 @@
       <c r="K66" s="92" t="s">
         <v>470</v>
       </c>
-      <c r="L66" s="151">
+      <c r="L66" s="149">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixing Scully last disguise power up name
Former-commit-id: dcf002c5f1e5954513563014fc64e6308c4e61be
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Powerups.xlsx
+++ b/Docs/Content/HungryDragonContent_Powerups.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\dragon\client\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\client\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1126" uniqueCount="476">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1126" uniqueCount="478">
   <si>
     <t>[sku]</t>
   </si>
@@ -1452,6 +1452,12 @@
   </si>
   <si>
     <t>trash_eater_better</t>
+  </si>
+  <si>
+    <t>TID_POWERUP_DISGUISE_35_DESC</t>
+  </si>
+  <si>
+    <t>TID_POWERUP_DISGUISE_35_DESC_SHORT</t>
   </si>
 </sst>
 </file>
@@ -1778,7 +1784,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="109">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1988,15 +1994,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="11" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2091,6 +2088,16 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="29">
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
@@ -2116,7 +2123,7 @@
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
         <top style="thin">
@@ -2649,27 +2656,10 @@
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
       <border outline="0">
         <top style="thin">
           <color auto="1"/>
         </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -2689,6 +2679,13 @@
       <alignment horizontal="center" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
@@ -2705,32 +2702,32 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="powerUpsDefinitions2" displayName="powerUpsDefinitions2" ref="A3:L115" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27" headerRowBorderDxfId="25" tableBorderDxfId="26" totalsRowBorderDxfId="24">
-  <autoFilter ref="A3:L115"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="powerUpsDefinitions2" displayName="powerUpsDefinitions2" ref="A3:L116" totalsRowShown="0" headerRowDxfId="28" dataDxfId="26" headerRowBorderDxfId="27" tableBorderDxfId="25" totalsRowBorderDxfId="24">
+  <autoFilter ref="A3:L116"/>
   <sortState ref="A4:K53">
     <sortCondition ref="D3:D53"/>
   </sortState>
   <tableColumns count="12">
-    <tableColumn id="1" name="{powerUpsDefinitions}" dataDxfId="22" totalsRowDxfId="23"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="20" totalsRowDxfId="21"/>
-    <tableColumn id="3" name="[type]" dataDxfId="18" totalsRowDxfId="19"/>
-    <tableColumn id="11" name="[category]" dataDxfId="16" totalsRowDxfId="17"/>
-    <tableColumn id="4" name="[param1]" dataDxfId="14" totalsRowDxfId="15"/>
-    <tableColumn id="5" name="[param2]" dataDxfId="12" totalsRowDxfId="13"/>
-    <tableColumn id="6" name="[icon]" dataDxfId="10" totalsRowDxfId="11">
+    <tableColumn id="1" name="{powerUpsDefinitions}" dataDxfId="23" totalsRowDxfId="22"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="21" totalsRowDxfId="20"/>
+    <tableColumn id="3" name="[type]" dataDxfId="19" totalsRowDxfId="18"/>
+    <tableColumn id="11" name="[category]" dataDxfId="17" totalsRowDxfId="16"/>
+    <tableColumn id="4" name="[param1]" dataDxfId="15" totalsRowDxfId="14"/>
+    <tableColumn id="5" name="[param2]" dataDxfId="13" totalsRowDxfId="12"/>
+    <tableColumn id="6" name="[icon]" dataDxfId="11" totalsRowDxfId="10">
       <calculatedColumnFormula>CONCATENATE("icon_",powerUpsDefinitions2[[#This Row],['[sku']]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="[miniIcon]" dataDxfId="8" totalsRowDxfId="9"/>
-    <tableColumn id="7" name="[tidName]" dataDxfId="6" totalsRowDxfId="7">
+    <tableColumn id="10" name="[miniIcon]" dataDxfId="9" totalsRowDxfId="8"/>
+    <tableColumn id="7" name="[tidName]" dataDxfId="7" totalsRowDxfId="6">
       <calculatedColumnFormula>CONCATENATE("TID_POWERUP_",UPPER(powerUpsDefinitions2[[#This Row],['[sku']]]),"_NAME")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="[tidDesc]" dataDxfId="4" totalsRowDxfId="5">
+    <tableColumn id="8" name="[tidDesc]" dataDxfId="5" totalsRowDxfId="4">
       <calculatedColumnFormula>CONCATENATE("TID_POWERUP_",UPPER(powerUpsDefinitions2[[#This Row],['[sku']]]),"_DESC")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="[tidDescShort]" dataDxfId="2" totalsRowDxfId="3">
+    <tableColumn id="9" name="[tidDescShort]" dataDxfId="3" totalsRowDxfId="2">
       <calculatedColumnFormula>CONCATENATE(powerUpsDefinitions2[[#This Row],['[tidDesc']]],"_SHORT")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="[level]" dataDxfId="0" totalsRowDxfId="1"/>
+    <tableColumn id="12" name="[level]" dataDxfId="1" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3004,8 +3001,8 @@
   </sheetPr>
   <dimension ref="A1:L121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="B103" sqref="B103"/>
+    <sheetView tabSelected="1" topLeftCell="H85" workbookViewId="0">
+      <selection activeCell="J116" sqref="J116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3874,7 +3871,7 @@
       <c r="G25" s="28" t="s">
         <v>139</v>
       </c>
-      <c r="H25" s="81" t="s">
+      <c r="H25" s="78" t="s">
         <v>37</v>
       </c>
       <c r="I25" s="31" t="s">
@@ -3886,7 +3883,7 @@
       <c r="K25" s="33" t="s">
         <v>367</v>
       </c>
-      <c r="L25" s="81">
+      <c r="L25" s="78">
         <v>0</v>
       </c>
     </row>
@@ -3910,7 +3907,7 @@
       <c r="G26" s="28" t="s">
         <v>139</v>
       </c>
-      <c r="H26" s="81" t="s">
+      <c r="H26" s="78" t="s">
         <v>37</v>
       </c>
       <c r="I26" s="31" t="s">
@@ -3922,7 +3919,7 @@
       <c r="K26" s="33" t="s">
         <v>370</v>
       </c>
-      <c r="L26" s="81">
+      <c r="L26" s="78">
         <v>0</v>
       </c>
     </row>
@@ -3948,7 +3945,7 @@
       <c r="G27" s="28" t="s">
         <v>141</v>
       </c>
-      <c r="H27" s="81" t="s">
+      <c r="H27" s="78" t="s">
         <v>27</v>
       </c>
       <c r="I27" s="31" t="s">
@@ -3960,7 +3957,7 @@
       <c r="K27" s="33" t="s">
         <v>373</v>
       </c>
-      <c r="L27" s="81">
+      <c r="L27" s="78">
         <v>0</v>
       </c>
     </row>
@@ -4986,7 +4983,7 @@
       <c r="G56" s="28" t="s">
         <v>141</v>
       </c>
-      <c r="H56" s="81" t="s">
+      <c r="H56" s="78" t="s">
         <v>33</v>
       </c>
       <c r="I56" s="31" t="s">
@@ -4998,7 +4995,7 @@
       <c r="K56" s="33" t="s">
         <v>456</v>
       </c>
-      <c r="L56" s="81">
+      <c r="L56" s="78">
         <v>0</v>
       </c>
     </row>
@@ -5012,7 +5009,7 @@
       <c r="C57" s="35" t="s">
         <v>100</v>
       </c>
-      <c r="D57" s="82" t="s">
+      <c r="D57" s="79" t="s">
         <v>99</v>
       </c>
       <c r="E57" s="30"/>
@@ -5020,7 +5017,7 @@
       <c r="G57" s="28" t="s">
         <v>141</v>
       </c>
-      <c r="H57" s="81" t="s">
+      <c r="H57" s="78" t="s">
         <v>33</v>
       </c>
       <c r="I57" s="31" t="s">
@@ -5032,7 +5029,7 @@
       <c r="K57" s="33" t="s">
         <v>105</v>
       </c>
-      <c r="L57" s="81">
+      <c r="L57" s="78">
         <v>0</v>
       </c>
     </row>
@@ -5046,7 +5043,7 @@
       <c r="C58" s="35" t="s">
         <v>101</v>
       </c>
-      <c r="D58" s="82" t="s">
+      <c r="D58" s="79" t="s">
         <v>99</v>
       </c>
       <c r="E58" s="30"/>
@@ -5054,7 +5051,7 @@
       <c r="G58" s="28" t="s">
         <v>141</v>
       </c>
-      <c r="H58" s="81" t="s">
+      <c r="H58" s="78" t="s">
         <v>33</v>
       </c>
       <c r="I58" s="31" t="s">
@@ -5066,7 +5063,7 @@
       <c r="K58" s="33" t="s">
         <v>108</v>
       </c>
-      <c r="L58" s="81">
+      <c r="L58" s="78">
         <v>0</v>
       </c>
     </row>
@@ -5074,13 +5071,13 @@
       <c r="A59" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="B59" s="83" t="s">
+      <c r="B59" s="80" t="s">
         <v>102</v>
       </c>
       <c r="C59" s="70" t="s">
         <v>102</v>
       </c>
-      <c r="D59" s="84" t="s">
+      <c r="D59" s="81" t="s">
         <v>99</v>
       </c>
       <c r="E59" s="71"/>
@@ -5091,13 +5088,13 @@
       <c r="H59" s="72" t="s">
         <v>33</v>
       </c>
-      <c r="I59" s="85" t="s">
+      <c r="I59" s="82" t="s">
         <v>109</v>
       </c>
-      <c r="J59" s="86" t="s">
+      <c r="J59" s="83" t="s">
         <v>110</v>
       </c>
-      <c r="K59" s="87" t="s">
+      <c r="K59" s="84" t="s">
         <v>111</v>
       </c>
       <c r="L59" s="72">
@@ -5105,10 +5102,10 @@
       </c>
     </row>
     <row r="60" spans="1:12" s="54" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="88" t="s">
-        <v>3</v>
-      </c>
-      <c r="B60" s="83" t="s">
+      <c r="A60" s="85" t="s">
+        <v>3</v>
+      </c>
+      <c r="B60" s="80" t="s">
         <v>112</v>
       </c>
       <c r="C60" s="70" t="s">
@@ -5125,7 +5122,7 @@
       <c r="H60" s="72" t="s">
         <v>33</v>
       </c>
-      <c r="I60" s="85" t="s">
+      <c r="I60" s="82" t="s">
         <v>113</v>
       </c>
       <c r="J60" s="32" t="s">
@@ -5253,21 +5250,21 @@
       <c r="D64" s="57" t="s">
         <v>99</v>
       </c>
-      <c r="E64" s="89"/>
-      <c r="F64" s="89"/>
+      <c r="E64" s="86"/>
+      <c r="F64" s="86"/>
       <c r="G64" s="28" t="s">
         <v>141</v>
       </c>
       <c r="H64" s="59" t="s">
         <v>33</v>
       </c>
-      <c r="I64" s="90" t="s">
+      <c r="I64" s="87" t="s">
         <v>460</v>
       </c>
-      <c r="J64" s="86" t="s">
+      <c r="J64" s="83" t="s">
         <v>461</v>
       </c>
-      <c r="K64" s="87" t="s">
+      <c r="K64" s="84" t="s">
         <v>462</v>
       </c>
       <c r="L64" s="59">
@@ -5347,582 +5344,582 @@
       </c>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A67" s="91" t="s">
+      <c r="A67" s="88" t="s">
         <v>3</v>
       </c>
       <c r="B67" s="63" t="s">
         <v>142</v>
       </c>
-      <c r="C67" s="92" t="s">
+      <c r="C67" s="89" t="s">
         <v>48</v>
       </c>
-      <c r="D67" s="92" t="s">
-        <v>98</v>
-      </c>
-      <c r="E67" s="93">
+      <c r="D67" s="89" t="s">
+        <v>98</v>
+      </c>
+      <c r="E67" s="90">
         <v>150</v>
       </c>
-      <c r="F67" s="93"/>
+      <c r="F67" s="90"/>
       <c r="G67" s="64" t="s">
         <v>138</v>
       </c>
-      <c r="H67" s="94" t="s">
+      <c r="H67" s="91" t="s">
         <v>42</v>
       </c>
-      <c r="I67" s="95" t="s">
+      <c r="I67" s="92" t="s">
         <v>165</v>
       </c>
-      <c r="J67" s="96" t="s">
+      <c r="J67" s="93" t="s">
         <v>166</v>
       </c>
-      <c r="K67" s="96" t="s">
+      <c r="K67" s="93" t="s">
         <v>283</v>
       </c>
-      <c r="L67" s="94">
+      <c r="L67" s="91">
         <v>1</v>
       </c>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A68" s="91" t="s">
+      <c r="A68" s="88" t="s">
         <v>3</v>
       </c>
       <c r="B68" s="63" t="s">
         <v>167</v>
       </c>
-      <c r="C68" s="92" t="s">
+      <c r="C68" s="89" t="s">
         <v>48</v>
       </c>
-      <c r="D68" s="92" t="s">
-        <v>98</v>
-      </c>
-      <c r="E68" s="93">
+      <c r="D68" s="89" t="s">
+        <v>98</v>
+      </c>
+      <c r="E68" s="90">
         <v>70</v>
       </c>
-      <c r="F68" s="93"/>
+      <c r="F68" s="90"/>
       <c r="G68" s="64" t="s">
         <v>138</v>
       </c>
-      <c r="H68" s="94" t="s">
+      <c r="H68" s="91" t="s">
         <v>42</v>
       </c>
-      <c r="I68" s="95" t="s">
+      <c r="I68" s="92" t="s">
         <v>165</v>
       </c>
-      <c r="J68" s="96" t="s">
+      <c r="J68" s="93" t="s">
         <v>166</v>
       </c>
-      <c r="K68" s="96" t="s">
+      <c r="K68" s="93" t="s">
         <v>283</v>
       </c>
-      <c r="L68" s="94">
+      <c r="L68" s="91">
         <v>1</v>
       </c>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A69" s="91" t="s">
+      <c r="A69" s="88" t="s">
         <v>3</v>
       </c>
       <c r="B69" s="63" t="s">
         <v>151</v>
       </c>
-      <c r="C69" s="92" t="s">
+      <c r="C69" s="89" t="s">
         <v>14</v>
       </c>
-      <c r="D69" s="92" t="s">
-        <v>98</v>
-      </c>
-      <c r="E69" s="93">
+      <c r="D69" s="89" t="s">
+        <v>98</v>
+      </c>
+      <c r="E69" s="90">
         <v>100</v>
       </c>
-      <c r="F69" s="93"/>
+      <c r="F69" s="90"/>
       <c r="G69" s="64" t="s">
         <v>138</v>
       </c>
-      <c r="H69" s="94" t="s">
+      <c r="H69" s="91" t="s">
         <v>42</v>
       </c>
-      <c r="I69" s="95" t="s">
+      <c r="I69" s="92" t="s">
         <v>168</v>
       </c>
-      <c r="J69" s="96" t="s">
+      <c r="J69" s="93" t="s">
         <v>169</v>
       </c>
-      <c r="K69" s="96" t="s">
+      <c r="K69" s="93" t="s">
         <v>284</v>
       </c>
-      <c r="L69" s="94">
+      <c r="L69" s="91">
         <v>1</v>
       </c>
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A70" s="91" t="s">
-        <v>3</v>
-      </c>
-      <c r="B70" s="97" t="s">
+      <c r="A70" s="88" t="s">
+        <v>3</v>
+      </c>
+      <c r="B70" s="94" t="s">
         <v>170</v>
       </c>
-      <c r="C70" s="92" t="s">
+      <c r="C70" s="89" t="s">
         <v>14</v>
       </c>
-      <c r="D70" s="92" t="s">
-        <v>98</v>
-      </c>
-      <c r="E70" s="93">
+      <c r="D70" s="89" t="s">
+        <v>98</v>
+      </c>
+      <c r="E70" s="90">
         <v>75</v>
       </c>
-      <c r="F70" s="93"/>
+      <c r="F70" s="90"/>
       <c r="G70" s="64" t="s">
         <v>138</v>
       </c>
-      <c r="H70" s="94" t="s">
+      <c r="H70" s="91" t="s">
         <v>42</v>
       </c>
-      <c r="I70" s="95" t="s">
+      <c r="I70" s="92" t="s">
         <v>168</v>
       </c>
-      <c r="J70" s="96" t="s">
+      <c r="J70" s="93" t="s">
         <v>169</v>
       </c>
-      <c r="K70" s="96" t="s">
+      <c r="K70" s="93" t="s">
         <v>284</v>
       </c>
-      <c r="L70" s="94">
+      <c r="L70" s="91">
         <v>1</v>
       </c>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A71" s="91" t="s">
-        <v>3</v>
-      </c>
-      <c r="B71" s="97" t="s">
+      <c r="A71" s="88" t="s">
+        <v>3</v>
+      </c>
+      <c r="B71" s="94" t="s">
         <v>149</v>
       </c>
-      <c r="C71" s="92" t="s">
+      <c r="C71" s="89" t="s">
         <v>56</v>
       </c>
-      <c r="D71" s="92" t="s">
-        <v>98</v>
-      </c>
-      <c r="E71" s="93">
+      <c r="D71" s="89" t="s">
+        <v>98</v>
+      </c>
+      <c r="E71" s="90">
         <v>50</v>
       </c>
-      <c r="F71" s="93"/>
+      <c r="F71" s="90"/>
       <c r="G71" s="64" t="s">
         <v>135</v>
       </c>
-      <c r="H71" s="94" t="s">
+      <c r="H71" s="91" t="s">
         <v>31</v>
       </c>
-      <c r="I71" s="95" t="s">
+      <c r="I71" s="92" t="s">
         <v>171</v>
       </c>
-      <c r="J71" s="96" t="s">
+      <c r="J71" s="93" t="s">
         <v>172</v>
       </c>
-      <c r="K71" s="96" t="s">
+      <c r="K71" s="93" t="s">
         <v>285</v>
       </c>
-      <c r="L71" s="94">
+      <c r="L71" s="91">
         <v>1</v>
       </c>
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A72" s="91" t="s">
-        <v>3</v>
-      </c>
-      <c r="B72" s="97" t="s">
+      <c r="A72" s="88" t="s">
+        <v>3</v>
+      </c>
+      <c r="B72" s="94" t="s">
         <v>173</v>
       </c>
-      <c r="C72" s="92" t="s">
+      <c r="C72" s="89" t="s">
         <v>56</v>
       </c>
-      <c r="D72" s="92" t="s">
-        <v>98</v>
-      </c>
-      <c r="E72" s="93">
+      <c r="D72" s="89" t="s">
+        <v>98</v>
+      </c>
+      <c r="E72" s="90">
         <v>30</v>
       </c>
-      <c r="F72" s="93"/>
+      <c r="F72" s="90"/>
       <c r="G72" s="64" t="s">
         <v>135</v>
       </c>
-      <c r="H72" s="94" t="s">
+      <c r="H72" s="91" t="s">
         <v>31</v>
       </c>
-      <c r="I72" s="95" t="s">
+      <c r="I72" s="92" t="s">
         <v>171</v>
       </c>
-      <c r="J72" s="96" t="s">
+      <c r="J72" s="93" t="s">
         <v>172</v>
       </c>
-      <c r="K72" s="96" t="s">
+      <c r="K72" s="93" t="s">
         <v>285</v>
       </c>
-      <c r="L72" s="94">
+      <c r="L72" s="91">
         <v>1</v>
       </c>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A73" s="91" t="s">
-        <v>3</v>
-      </c>
-      <c r="B73" s="97" t="s">
+      <c r="A73" s="88" t="s">
+        <v>3</v>
+      </c>
+      <c r="B73" s="94" t="s">
         <v>174</v>
       </c>
-      <c r="C73" s="92" t="s">
+      <c r="C73" s="89" t="s">
         <v>5</v>
       </c>
-      <c r="D73" s="92" t="s">
+      <c r="D73" s="89" t="s">
         <v>99</v>
       </c>
-      <c r="E73" s="93"/>
-      <c r="F73" s="93"/>
+      <c r="E73" s="90"/>
+      <c r="F73" s="90"/>
       <c r="G73" s="64" t="s">
         <v>135</v>
       </c>
-      <c r="H73" s="94" t="s">
+      <c r="H73" s="91" t="s">
         <v>31</v>
       </c>
-      <c r="I73" s="95" t="s">
+      <c r="I73" s="92" t="s">
         <v>175</v>
       </c>
-      <c r="J73" s="96" t="s">
+      <c r="J73" s="93" t="s">
         <v>176</v>
       </c>
-      <c r="K73" s="96" t="s">
+      <c r="K73" s="93" t="s">
         <v>286</v>
       </c>
-      <c r="L73" s="94">
+      <c r="L73" s="91">
         <v>1</v>
       </c>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A74" s="91" t="s">
+      <c r="A74" s="88" t="s">
         <v>3</v>
       </c>
       <c r="B74" s="63" t="s">
         <v>143</v>
       </c>
-      <c r="C74" s="92" t="s">
+      <c r="C74" s="89" t="s">
         <v>30</v>
       </c>
-      <c r="D74" s="92" t="s">
-        <v>98</v>
-      </c>
-      <c r="E74" s="93">
+      <c r="D74" s="89" t="s">
+        <v>98</v>
+      </c>
+      <c r="E74" s="90">
         <v>25</v>
       </c>
-      <c r="F74" s="93"/>
+      <c r="F74" s="90"/>
       <c r="G74" s="64" t="s">
         <v>135</v>
       </c>
-      <c r="H74" s="94" t="s">
+      <c r="H74" s="91" t="s">
         <v>31</v>
       </c>
-      <c r="I74" s="95" t="s">
+      <c r="I74" s="92" t="s">
         <v>177</v>
       </c>
-      <c r="J74" s="96" t="s">
+      <c r="J74" s="93" t="s">
         <v>178</v>
       </c>
-      <c r="K74" s="96" t="s">
+      <c r="K74" s="93" t="s">
         <v>287</v>
       </c>
-      <c r="L74" s="94">
+      <c r="L74" s="91">
         <v>1</v>
       </c>
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A75" s="91" t="s">
-        <v>3</v>
-      </c>
-      <c r="B75" s="97" t="s">
+      <c r="A75" s="88" t="s">
+        <v>3</v>
+      </c>
+      <c r="B75" s="94" t="s">
         <v>179</v>
       </c>
-      <c r="C75" s="92" t="s">
+      <c r="C75" s="89" t="s">
         <v>30</v>
       </c>
-      <c r="D75" s="92" t="s">
-        <v>98</v>
-      </c>
-      <c r="E75" s="93">
+      <c r="D75" s="89" t="s">
+        <v>98</v>
+      </c>
+      <c r="E75" s="90">
         <v>15</v>
       </c>
-      <c r="F75" s="93"/>
+      <c r="F75" s="90"/>
       <c r="G75" s="64" t="s">
         <v>135</v>
       </c>
-      <c r="H75" s="94" t="s">
+      <c r="H75" s="91" t="s">
         <v>31</v>
       </c>
-      <c r="I75" s="95" t="s">
+      <c r="I75" s="92" t="s">
         <v>177</v>
       </c>
-      <c r="J75" s="96" t="s">
+      <c r="J75" s="93" t="s">
         <v>178</v>
       </c>
-      <c r="K75" s="96" t="s">
+      <c r="K75" s="93" t="s">
         <v>287</v>
       </c>
-      <c r="L75" s="94">
+      <c r="L75" s="91">
         <v>1</v>
       </c>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A76" s="91" t="s">
-        <v>3</v>
-      </c>
-      <c r="B76" s="97" t="s">
+      <c r="A76" s="88" t="s">
+        <v>3</v>
+      </c>
+      <c r="B76" s="94" t="s">
         <v>146</v>
       </c>
-      <c r="C76" s="92" t="s">
+      <c r="C76" s="89" t="s">
         <v>51</v>
       </c>
-      <c r="D76" s="92" t="s">
-        <v>98</v>
-      </c>
-      <c r="E76" s="93" t="s">
+      <c r="D76" s="89" t="s">
+        <v>98</v>
+      </c>
+      <c r="E76" s="90" t="s">
         <v>29</v>
       </c>
-      <c r="F76" s="93">
+      <c r="F76" s="90">
         <v>100</v>
       </c>
       <c r="G76" s="64" t="s">
         <v>140</v>
       </c>
-      <c r="H76" s="94" t="s">
+      <c r="H76" s="91" t="s">
         <v>27</v>
       </c>
-      <c r="I76" s="95" t="s">
+      <c r="I76" s="92" t="s">
         <v>180</v>
       </c>
-      <c r="J76" s="96" t="s">
+      <c r="J76" s="93" t="s">
         <v>181</v>
       </c>
-      <c r="K76" s="96" t="s">
+      <c r="K76" s="93" t="s">
         <v>182</v>
       </c>
-      <c r="L76" s="94">
+      <c r="L76" s="91">
         <v>1</v>
       </c>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A77" s="91" t="s">
-        <v>3</v>
-      </c>
-      <c r="B77" s="97" t="s">
+      <c r="A77" s="88" t="s">
+        <v>3</v>
+      </c>
+      <c r="B77" s="94" t="s">
         <v>155</v>
       </c>
-      <c r="C77" s="92" t="s">
+      <c r="C77" s="89" t="s">
         <v>51</v>
       </c>
-      <c r="D77" s="92" t="s">
-        <v>98</v>
-      </c>
-      <c r="E77" s="93" t="s">
+      <c r="D77" s="89" t="s">
+        <v>98</v>
+      </c>
+      <c r="E77" s="90" t="s">
         <v>26</v>
       </c>
-      <c r="F77" s="93">
+      <c r="F77" s="90">
         <v>50</v>
       </c>
       <c r="G77" s="64" t="s">
         <v>140</v>
       </c>
-      <c r="H77" s="94" t="s">
+      <c r="H77" s="91" t="s">
         <v>27</v>
       </c>
-      <c r="I77" s="95" t="s">
+      <c r="I77" s="92" t="s">
         <v>183</v>
       </c>
-      <c r="J77" s="96" t="s">
+      <c r="J77" s="93" t="s">
         <v>184</v>
       </c>
-      <c r="K77" s="96" t="s">
+      <c r="K77" s="93" t="s">
         <v>288</v>
       </c>
-      <c r="L77" s="94">
+      <c r="L77" s="91">
         <v>1</v>
       </c>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A78" s="91" t="s">
-        <v>3</v>
-      </c>
-      <c r="B78" s="97" t="s">
+      <c r="A78" s="88" t="s">
+        <v>3</v>
+      </c>
+      <c r="B78" s="94" t="s">
         <v>185</v>
       </c>
-      <c r="C78" s="92" t="s">
+      <c r="C78" s="89" t="s">
         <v>51</v>
       </c>
-      <c r="D78" s="92" t="s">
-        <v>98</v>
-      </c>
-      <c r="E78" s="93" t="s">
+      <c r="D78" s="89" t="s">
+        <v>98</v>
+      </c>
+      <c r="E78" s="90" t="s">
         <v>26</v>
       </c>
-      <c r="F78" s="93">
+      <c r="F78" s="90">
         <v>35</v>
       </c>
       <c r="G78" s="64" t="s">
         <v>140</v>
       </c>
-      <c r="H78" s="94" t="s">
+      <c r="H78" s="91" t="s">
         <v>27</v>
       </c>
-      <c r="I78" s="95" t="s">
+      <c r="I78" s="92" t="s">
         <v>183</v>
       </c>
-      <c r="J78" s="96" t="s">
+      <c r="J78" s="93" t="s">
         <v>184</v>
       </c>
-      <c r="K78" s="96" t="s">
+      <c r="K78" s="93" t="s">
         <v>288</v>
       </c>
-      <c r="L78" s="94">
+      <c r="L78" s="91">
         <v>1</v>
       </c>
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A79" s="98" t="s">
-        <v>3</v>
-      </c>
-      <c r="B79" s="99" t="s">
+      <c r="A79" s="95" t="s">
+        <v>3</v>
+      </c>
+      <c r="B79" s="96" t="s">
         <v>157</v>
       </c>
-      <c r="C79" s="100" t="s">
+      <c r="C79" s="97" t="s">
         <v>10</v>
       </c>
-      <c r="D79" s="100" t="s">
-        <v>98</v>
-      </c>
-      <c r="E79" s="101">
+      <c r="D79" s="97" t="s">
+        <v>98</v>
+      </c>
+      <c r="E79" s="98">
         <v>50</v>
       </c>
-      <c r="F79" s="101"/>
+      <c r="F79" s="98"/>
       <c r="G79" s="64" t="s">
         <v>136</v>
       </c>
-      <c r="H79" s="94" t="s">
+      <c r="H79" s="91" t="s">
         <v>4</v>
       </c>
-      <c r="I79" s="95" t="s">
+      <c r="I79" s="92" t="s">
         <v>186</v>
       </c>
-      <c r="J79" s="96" t="s">
+      <c r="J79" s="93" t="s">
         <v>187</v>
       </c>
-      <c r="K79" s="96" t="s">
+      <c r="K79" s="93" t="s">
         <v>289</v>
       </c>
-      <c r="L79" s="94">
+      <c r="L79" s="91">
         <v>1</v>
       </c>
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A80" s="91" t="s">
-        <v>3</v>
-      </c>
-      <c r="B80" s="97" t="s">
+      <c r="A80" s="88" t="s">
+        <v>3</v>
+      </c>
+      <c r="B80" s="94" t="s">
         <v>152</v>
       </c>
-      <c r="C80" s="92" t="s">
+      <c r="C80" s="89" t="s">
         <v>49</v>
       </c>
-      <c r="D80" s="92" t="s">
-        <v>98</v>
-      </c>
-      <c r="E80" s="93">
+      <c r="D80" s="89" t="s">
+        <v>98</v>
+      </c>
+      <c r="E80" s="90">
         <v>25</v>
       </c>
-      <c r="F80" s="93"/>
+      <c r="F80" s="90"/>
       <c r="G80" s="64" t="s">
         <v>139</v>
       </c>
-      <c r="H80" s="94" t="s">
+      <c r="H80" s="91" t="s">
         <v>44</v>
       </c>
-      <c r="I80" s="95" t="s">
+      <c r="I80" s="92" t="s">
         <v>188</v>
       </c>
-      <c r="J80" s="96" t="s">
+      <c r="J80" s="93" t="s">
         <v>189</v>
       </c>
-      <c r="K80" s="96" t="s">
+      <c r="K80" s="93" t="s">
         <v>290</v>
       </c>
-      <c r="L80" s="94">
+      <c r="L80" s="91">
         <v>1</v>
       </c>
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A81" s="91" t="s">
-        <v>3</v>
-      </c>
-      <c r="B81" s="97" t="s">
+      <c r="A81" s="88" t="s">
+        <v>3</v>
+      </c>
+      <c r="B81" s="94" t="s">
         <v>190</v>
       </c>
-      <c r="C81" s="92" t="s">
+      <c r="C81" s="89" t="s">
         <v>49</v>
       </c>
-      <c r="D81" s="92" t="s">
-        <v>98</v>
-      </c>
-      <c r="E81" s="93">
+      <c r="D81" s="89" t="s">
+        <v>98</v>
+      </c>
+      <c r="E81" s="90">
         <v>15</v>
       </c>
-      <c r="F81" s="93"/>
+      <c r="F81" s="90"/>
       <c r="G81" s="64" t="s">
         <v>139</v>
       </c>
-      <c r="H81" s="94" t="s">
+      <c r="H81" s="91" t="s">
         <v>44</v>
       </c>
-      <c r="I81" s="95" t="s">
+      <c r="I81" s="92" t="s">
         <v>188</v>
       </c>
-      <c r="J81" s="96" t="s">
+      <c r="J81" s="93" t="s">
         <v>189</v>
       </c>
-      <c r="K81" s="96" t="s">
+      <c r="K81" s="93" t="s">
         <v>290</v>
       </c>
-      <c r="L81" s="94">
+      <c r="L81" s="91">
         <v>1</v>
       </c>
     </row>
     <row r="82" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A82" s="102" t="s">
+      <c r="A82" s="99" t="s">
         <v>3</v>
       </c>
       <c r="B82" s="65" t="s">
         <v>144</v>
       </c>
-      <c r="C82" s="103" t="s">
+      <c r="C82" s="100" t="s">
         <v>32</v>
       </c>
-      <c r="D82" s="103" t="s">
-        <v>98</v>
-      </c>
-      <c r="E82" s="104">
+      <c r="D82" s="100" t="s">
+        <v>98</v>
+      </c>
+      <c r="E82" s="101">
         <v>20</v>
       </c>
-      <c r="F82" s="104"/>
+      <c r="F82" s="101"/>
       <c r="G82" s="66" t="s">
         <v>136</v>
       </c>
-      <c r="H82" s="105" t="s">
+      <c r="H82" s="102" t="s">
         <v>4</v>
       </c>
-      <c r="I82" s="95" t="s">
+      <c r="I82" s="92" t="s">
         <v>191</v>
       </c>
-      <c r="J82" s="96" t="s">
+      <c r="J82" s="93" t="s">
         <v>192</v>
       </c>
-      <c r="K82" s="96" t="s">
+      <c r="K82" s="93" t="s">
         <v>291</v>
       </c>
-      <c r="L82" s="105">
+      <c r="L82" s="102">
         <v>1</v>
       </c>
     </row>
@@ -5930,7 +5927,7 @@
       <c r="A83" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="B83" s="83" t="s">
+      <c r="B83" s="80" t="s">
         <v>193</v>
       </c>
       <c r="C83" s="70" t="s">
@@ -5951,7 +5948,7 @@
       <c r="H83" s="72" t="s">
         <v>33</v>
       </c>
-      <c r="I83" s="85" t="s">
+      <c r="I83" s="82" t="s">
         <v>194</v>
       </c>
       <c r="J83" s="32" t="s">
@@ -5968,7 +5965,7 @@
       <c r="A84" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="B84" s="83" t="s">
+      <c r="B84" s="80" t="s">
         <v>197</v>
       </c>
       <c r="C84" s="70" t="s">
@@ -5989,7 +5986,7 @@
       <c r="H84" s="72" t="s">
         <v>33</v>
       </c>
-      <c r="I84" s="85" t="s">
+      <c r="I84" s="82" t="s">
         <v>194</v>
       </c>
       <c r="J84" s="32" t="s">
@@ -6006,7 +6003,7 @@
       <c r="A85" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="B85" s="83" t="s">
+      <c r="B85" s="80" t="s">
         <v>200</v>
       </c>
       <c r="C85" s="70" t="s">
@@ -6027,7 +6024,7 @@
       <c r="H85" s="72" t="s">
         <v>33</v>
       </c>
-      <c r="I85" s="85" t="s">
+      <c r="I85" s="82" t="s">
         <v>201</v>
       </c>
       <c r="J85" s="32" t="s">
@@ -6044,7 +6041,7 @@
       <c r="A86" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="B86" s="83" t="s">
+      <c r="B86" s="80" t="s">
         <v>148</v>
       </c>
       <c r="C86" s="70" t="s">
@@ -6065,7 +6062,7 @@
       <c r="H86" s="72" t="s">
         <v>33</v>
       </c>
-      <c r="I86" s="85" t="s">
+      <c r="I86" s="82" t="s">
         <v>204</v>
       </c>
       <c r="J86" s="32" t="s">
@@ -6082,7 +6079,7 @@
       <c r="A87" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="B87" s="83" t="s">
+      <c r="B87" s="80" t="s">
         <v>207</v>
       </c>
       <c r="C87" s="70" t="s">
@@ -6103,7 +6100,7 @@
       <c r="H87" s="72" t="s">
         <v>33</v>
       </c>
-      <c r="I87" s="85" t="s">
+      <c r="I87" s="82" t="s">
         <v>208</v>
       </c>
       <c r="J87" s="32" t="s">
@@ -6120,7 +6117,7 @@
       <c r="A88" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="B88" s="83" t="s">
+      <c r="B88" s="80" t="s">
         <v>147</v>
       </c>
       <c r="C88" s="70" t="s">
@@ -6141,7 +6138,7 @@
       <c r="H88" s="72" t="s">
         <v>33</v>
       </c>
-      <c r="I88" s="85" t="s">
+      <c r="I88" s="82" t="s">
         <v>211</v>
       </c>
       <c r="J88" s="32" t="s">
@@ -6158,7 +6155,7 @@
       <c r="A89" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="B89" s="83" t="s">
+      <c r="B89" s="80" t="s">
         <v>214</v>
       </c>
       <c r="C89" s="70" t="s">
@@ -6179,7 +6176,7 @@
       <c r="H89" s="72" t="s">
         <v>33</v>
       </c>
-      <c r="I89" s="85" t="s">
+      <c r="I89" s="82" t="s">
         <v>215</v>
       </c>
       <c r="J89" s="32" t="s">
@@ -6196,7 +6193,7 @@
       <c r="A90" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="B90" s="83" t="s">
+      <c r="B90" s="80" t="s">
         <v>153</v>
       </c>
       <c r="C90" s="70" t="s">
@@ -6217,7 +6214,7 @@
       <c r="H90" s="72" t="s">
         <v>33</v>
       </c>
-      <c r="I90" s="85" t="s">
+      <c r="I90" s="82" t="s">
         <v>218</v>
       </c>
       <c r="J90" s="32" t="s">
@@ -6255,7 +6252,7 @@
       <c r="H91" s="72" t="s">
         <v>33</v>
       </c>
-      <c r="I91" s="85" t="s">
+      <c r="I91" s="82" t="s">
         <v>221</v>
       </c>
       <c r="J91" s="32" t="s">
@@ -6293,7 +6290,7 @@
       <c r="H92" s="72" t="s">
         <v>33</v>
       </c>
-      <c r="I92" s="85" t="s">
+      <c r="I92" s="82" t="s">
         <v>221</v>
       </c>
       <c r="J92" s="32" t="s">
@@ -6310,7 +6307,7 @@
       <c r="A93" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="B93" s="83" t="s">
+      <c r="B93" s="80" t="s">
         <v>150</v>
       </c>
       <c r="C93" s="70" t="s">
@@ -6331,7 +6328,7 @@
       <c r="H93" s="72" t="s">
         <v>33</v>
       </c>
-      <c r="I93" s="85" t="s">
+      <c r="I93" s="82" t="s">
         <v>224</v>
       </c>
       <c r="J93" s="32" t="s">
@@ -6348,7 +6345,7 @@
       <c r="A94" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="B94" s="83" t="s">
+      <c r="B94" s="80" t="s">
         <v>227</v>
       </c>
       <c r="C94" s="70" t="s">
@@ -6369,7 +6366,7 @@
       <c r="H94" s="72" t="s">
         <v>33</v>
       </c>
-      <c r="I94" s="85" t="s">
+      <c r="I94" s="82" t="s">
         <v>228</v>
       </c>
       <c r="J94" s="32" t="s">
@@ -6386,7 +6383,7 @@
       <c r="A95" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="B95" s="83" t="s">
+      <c r="B95" s="80" t="s">
         <v>231</v>
       </c>
       <c r="C95" s="70" t="s">
@@ -6407,7 +6404,7 @@
       <c r="H95" s="72" t="s">
         <v>33</v>
       </c>
-      <c r="I95" s="85" t="s">
+      <c r="I95" s="82" t="s">
         <v>228</v>
       </c>
       <c r="J95" s="32" t="s">
@@ -6424,7 +6421,7 @@
       <c r="A96" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="B96" s="83" t="s">
+      <c r="B96" s="80" t="s">
         <v>234</v>
       </c>
       <c r="C96" s="70" t="s">
@@ -6445,7 +6442,7 @@
       <c r="H96" s="72" t="s">
         <v>33</v>
       </c>
-      <c r="I96" s="85" t="s">
+      <c r="I96" s="82" t="s">
         <v>235</v>
       </c>
       <c r="J96" s="32" t="s">
@@ -6462,7 +6459,7 @@
       <c r="A97" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="B97" s="83" t="s">
+      <c r="B97" s="80" t="s">
         <v>238</v>
       </c>
       <c r="C97" s="70" t="s">
@@ -6483,7 +6480,7 @@
       <c r="H97" s="72" t="s">
         <v>33</v>
       </c>
-      <c r="I97" s="85" t="s">
+      <c r="I97" s="82" t="s">
         <v>235</v>
       </c>
       <c r="J97" s="32" t="s">
@@ -6500,7 +6497,7 @@
       <c r="A98" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="B98" s="83" t="s">
+      <c r="B98" s="80" t="s">
         <v>241</v>
       </c>
       <c r="C98" s="70" t="s">
@@ -6521,7 +6518,7 @@
       <c r="H98" s="72" t="s">
         <v>33</v>
       </c>
-      <c r="I98" s="85" t="s">
+      <c r="I98" s="82" t="s">
         <v>242</v>
       </c>
       <c r="J98" s="32" t="s">
@@ -6538,7 +6535,7 @@
       <c r="A99" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="B99" s="83" t="s">
+      <c r="B99" s="80" t="s">
         <v>245</v>
       </c>
       <c r="C99" s="70" t="s">
@@ -6559,7 +6556,7 @@
       <c r="H99" s="72" t="s">
         <v>33</v>
       </c>
-      <c r="I99" s="85" t="s">
+      <c r="I99" s="82" t="s">
         <v>242</v>
       </c>
       <c r="J99" s="32" t="s">
@@ -6576,7 +6573,7 @@
       <c r="A100" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="B100" s="83" t="s">
+      <c r="B100" s="80" t="s">
         <v>248</v>
       </c>
       <c r="C100" s="70" t="s">
@@ -6597,7 +6594,7 @@
       <c r="H100" s="72" t="s">
         <v>33</v>
       </c>
-      <c r="I100" s="85" t="s">
+      <c r="I100" s="82" t="s">
         <v>249</v>
       </c>
       <c r="J100" s="32" t="s">
@@ -6614,7 +6611,7 @@
       <c r="A101" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="B101" s="83" t="s">
+      <c r="B101" s="80" t="s">
         <v>252</v>
       </c>
       <c r="C101" s="70" t="s">
@@ -6635,7 +6632,7 @@
       <c r="H101" s="72" t="s">
         <v>33</v>
       </c>
-      <c r="I101" s="85" t="s">
+      <c r="I101" s="82" t="s">
         <v>249</v>
       </c>
       <c r="J101" s="32" t="s">
@@ -6652,7 +6649,7 @@
       <c r="A102" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="B102" s="83" t="s">
+      <c r="B102" s="80" t="s">
         <v>255</v>
       </c>
       <c r="C102" s="70" t="s">
@@ -6673,7 +6670,7 @@
       <c r="H102" s="72" t="s">
         <v>33</v>
       </c>
-      <c r="I102" s="85" t="s">
+      <c r="I102" s="82" t="s">
         <v>256</v>
       </c>
       <c r="J102" s="32" t="s">
@@ -6690,7 +6687,7 @@
       <c r="A103" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="B103" s="83" t="s">
+      <c r="B103" s="80" t="s">
         <v>259</v>
       </c>
       <c r="C103" s="70" t="s">
@@ -6711,7 +6708,7 @@
       <c r="H103" s="72" t="s">
         <v>33</v>
       </c>
-      <c r="I103" s="85" t="s">
+      <c r="I103" s="82" t="s">
         <v>256</v>
       </c>
       <c r="J103" s="32" t="s">
@@ -6728,7 +6725,7 @@
       <c r="A104" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="B104" s="83" t="s">
+      <c r="B104" s="80" t="s">
         <v>295</v>
       </c>
       <c r="C104" s="70" t="s">
@@ -6787,13 +6784,13 @@
       <c r="H105" s="72" t="s">
         <v>33</v>
       </c>
-      <c r="I105" s="77" t="s">
+      <c r="I105" s="47" t="s">
         <v>280</v>
       </c>
-      <c r="J105" s="78" t="s">
+      <c r="J105" s="20" t="s">
         <v>307</v>
       </c>
-      <c r="K105" s="78" t="s">
+      <c r="K105" s="20" t="s">
         <v>308</v>
       </c>
       <c r="L105" s="72">
@@ -6801,244 +6798,244 @@
       </c>
     </row>
     <row r="106" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A106" s="102" t="s">
-        <v>3</v>
-      </c>
-      <c r="B106" s="106" t="s">
+      <c r="A106" s="99" t="s">
+        <v>3</v>
+      </c>
+      <c r="B106" s="103" t="s">
         <v>156</v>
       </c>
-      <c r="C106" s="103" t="s">
+      <c r="C106" s="100" t="s">
         <v>95</v>
       </c>
-      <c r="D106" s="103" t="s">
-        <v>98</v>
-      </c>
-      <c r="E106" s="104" t="s">
+      <c r="D106" s="100" t="s">
+        <v>98</v>
+      </c>
+      <c r="E106" s="101" t="s">
         <v>245</v>
       </c>
-      <c r="F106" s="104" t="s">
+      <c r="F106" s="101" t="s">
         <v>144</v>
       </c>
       <c r="G106" s="66" t="s">
         <v>141</v>
       </c>
-      <c r="H106" s="105" t="s">
+      <c r="H106" s="102" t="s">
         <v>33</v>
       </c>
-      <c r="I106" s="107" t="s">
+      <c r="I106" s="104" t="s">
         <v>262</v>
       </c>
-      <c r="J106" s="96" t="s">
+      <c r="J106" s="93" t="s">
         <v>263</v>
       </c>
-      <c r="K106" s="96" t="s">
+      <c r="K106" s="93" t="s">
         <v>264</v>
       </c>
-      <c r="L106" s="105">
+      <c r="L106" s="102">
         <v>3</v>
       </c>
     </row>
     <row r="107" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A107" s="102" t="s">
-        <v>3</v>
-      </c>
-      <c r="B107" s="106" t="s">
+      <c r="A107" s="99" t="s">
+        <v>3</v>
+      </c>
+      <c r="B107" s="103" t="s">
         <v>158</v>
       </c>
-      <c r="C107" s="103" t="s">
+      <c r="C107" s="100" t="s">
         <v>95</v>
       </c>
-      <c r="D107" s="103" t="s">
-        <v>98</v>
-      </c>
-      <c r="E107" s="104" t="s">
+      <c r="D107" s="100" t="s">
+        <v>98</v>
+      </c>
+      <c r="E107" s="101" t="s">
         <v>259</v>
       </c>
-      <c r="F107" s="104" t="s">
+      <c r="F107" s="101" t="s">
         <v>157</v>
       </c>
-      <c r="G107" s="105" t="s">
+      <c r="G107" s="102" t="s">
         <v>141</v>
       </c>
-      <c r="H107" s="105" t="s">
+      <c r="H107" s="102" t="s">
         <v>33</v>
       </c>
-      <c r="I107" s="107" t="s">
+      <c r="I107" s="104" t="s">
         <v>265</v>
       </c>
-      <c r="J107" s="96" t="s">
+      <c r="J107" s="93" t="s">
         <v>266</v>
       </c>
-      <c r="K107" s="96" t="s">
+      <c r="K107" s="93" t="s">
         <v>267</v>
       </c>
-      <c r="L107" s="105">
+      <c r="L107" s="102">
         <v>3</v>
       </c>
     </row>
     <row r="108" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A108" s="102" t="s">
-        <v>3</v>
-      </c>
-      <c r="B108" s="106" t="s">
+      <c r="A108" s="99" t="s">
+        <v>3</v>
+      </c>
+      <c r="B108" s="103" t="s">
         <v>159</v>
       </c>
-      <c r="C108" s="103" t="s">
+      <c r="C108" s="100" t="s">
         <v>95</v>
       </c>
-      <c r="D108" s="103" t="s">
-        <v>98</v>
-      </c>
-      <c r="E108" s="104" t="s">
+      <c r="D108" s="100" t="s">
+        <v>98</v>
+      </c>
+      <c r="E108" s="101" t="s">
         <v>197</v>
       </c>
-      <c r="F108" s="104" t="s">
+      <c r="F108" s="101" t="s">
         <v>185</v>
       </c>
-      <c r="G108" s="105" t="s">
+      <c r="G108" s="102" t="s">
         <v>141</v>
       </c>
-      <c r="H108" s="105" t="s">
+      <c r="H108" s="102" t="s">
         <v>33</v>
       </c>
-      <c r="I108" s="107" t="s">
+      <c r="I108" s="104" t="s">
         <v>268</v>
       </c>
-      <c r="J108" s="96" t="s">
+      <c r="J108" s="93" t="s">
         <v>269</v>
       </c>
-      <c r="K108" s="96" t="s">
+      <c r="K108" s="93" t="s">
         <v>270</v>
       </c>
-      <c r="L108" s="105">
+      <c r="L108" s="102">
         <v>3</v>
       </c>
     </row>
     <row r="109" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A109" s="102" t="s">
-        <v>3</v>
-      </c>
-      <c r="B109" s="106" t="s">
+      <c r="A109" s="99" t="s">
+        <v>3</v>
+      </c>
+      <c r="B109" s="103" t="s">
         <v>160</v>
       </c>
-      <c r="C109" s="103" t="s">
+      <c r="C109" s="100" t="s">
         <v>95</v>
       </c>
-      <c r="D109" s="103" t="s">
-        <v>98</v>
-      </c>
-      <c r="E109" s="104" t="s">
+      <c r="D109" s="100" t="s">
+        <v>98</v>
+      </c>
+      <c r="E109" s="101" t="s">
         <v>252</v>
       </c>
-      <c r="F109" s="104" t="s">
+      <c r="F109" s="101" t="s">
         <v>157</v>
       </c>
-      <c r="G109" s="105" t="s">
+      <c r="G109" s="102" t="s">
         <v>141</v>
       </c>
-      <c r="H109" s="105" t="s">
+      <c r="H109" s="102" t="s">
         <v>33</v>
       </c>
-      <c r="I109" s="107" t="s">
+      <c r="I109" s="104" t="s">
         <v>271</v>
       </c>
-      <c r="J109" s="96" t="s">
+      <c r="J109" s="93" t="s">
         <v>272</v>
       </c>
-      <c r="K109" s="96" t="s">
+      <c r="K109" s="93" t="s">
         <v>273</v>
       </c>
-      <c r="L109" s="105">
+      <c r="L109" s="102">
         <v>3</v>
       </c>
     </row>
     <row r="110" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A110" s="102" t="s">
-        <v>3</v>
-      </c>
-      <c r="B110" s="106" t="s">
+      <c r="A110" s="99" t="s">
+        <v>3</v>
+      </c>
+      <c r="B110" s="103" t="s">
         <v>161</v>
       </c>
-      <c r="C110" s="103" t="s">
+      <c r="C110" s="100" t="s">
         <v>95</v>
       </c>
-      <c r="D110" s="103" t="s">
-        <v>98</v>
-      </c>
-      <c r="E110" s="104" t="s">
+      <c r="D110" s="100" t="s">
+        <v>98</v>
+      </c>
+      <c r="E110" s="101" t="s">
         <v>238</v>
       </c>
-      <c r="F110" s="104" t="s">
+      <c r="F110" s="101" t="s">
         <v>190</v>
       </c>
-      <c r="G110" s="105" t="s">
+      <c r="G110" s="102" t="s">
         <v>141</v>
       </c>
-      <c r="H110" s="105" t="s">
+      <c r="H110" s="102" t="s">
         <v>33</v>
       </c>
-      <c r="I110" s="107" t="s">
+      <c r="I110" s="104" t="s">
         <v>274</v>
       </c>
-      <c r="J110" s="96" t="s">
+      <c r="J110" s="93" t="s">
         <v>275</v>
       </c>
-      <c r="K110" s="96" t="s">
+      <c r="K110" s="93" t="s">
         <v>276</v>
       </c>
-      <c r="L110" s="105">
+      <c r="L110" s="102">
         <v>3</v>
       </c>
     </row>
     <row r="111" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A111" s="102" t="s">
-        <v>3</v>
-      </c>
-      <c r="B111" s="106" t="s">
+      <c r="A111" s="99" t="s">
+        <v>3</v>
+      </c>
+      <c r="B111" s="103" t="s">
         <v>162</v>
       </c>
-      <c r="C111" s="103" t="s">
+      <c r="C111" s="100" t="s">
         <v>95</v>
       </c>
-      <c r="D111" s="103" t="s">
-        <v>98</v>
-      </c>
-      <c r="E111" s="104" t="s">
+      <c r="D111" s="100" t="s">
+        <v>98</v>
+      </c>
+      <c r="E111" s="101" t="s">
         <v>231</v>
       </c>
-      <c r="F111" s="104" t="s">
+      <c r="F111" s="101" t="s">
         <v>179</v>
       </c>
-      <c r="G111" s="105" t="s">
+      <c r="G111" s="102" t="s">
         <v>141</v>
       </c>
-      <c r="H111" s="105" t="s">
+      <c r="H111" s="102" t="s">
         <v>33</v>
       </c>
-      <c r="I111" s="107" t="s">
+      <c r="I111" s="104" t="s">
         <v>277</v>
       </c>
-      <c r="J111" s="108" t="s">
+      <c r="J111" s="105" t="s">
         <v>278</v>
       </c>
-      <c r="K111" s="108" t="s">
+      <c r="K111" s="105" t="s">
         <v>279</v>
       </c>
-      <c r="L111" s="105">
+      <c r="L111" s="102">
         <v>3</v>
       </c>
     </row>
     <row r="112" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A112" s="102" t="s">
+      <c r="A112" s="99" t="s">
         <v>3</v>
       </c>
       <c r="B112" s="65" t="s">
         <v>145</v>
       </c>
-      <c r="C112" s="103" t="s">
+      <c r="C112" s="100" t="s">
         <v>95</v>
       </c>
-      <c r="D112" s="103" t="s">
+      <c r="D112" s="100" t="s">
         <v>98</v>
       </c>
       <c r="E112" s="67" t="s">
@@ -7047,10 +7044,10 @@
       <c r="F112" s="67" t="s">
         <v>144</v>
       </c>
-      <c r="G112" s="105" t="s">
+      <c r="G112" s="102" t="s">
         <v>141</v>
       </c>
-      <c r="H112" s="105" t="s">
+      <c r="H112" s="102" t="s">
         <v>33</v>
       </c>
       <c r="I112" s="68" t="s">
@@ -7062,97 +7059,97 @@
       <c r="K112" s="69" t="s">
         <v>282</v>
       </c>
-      <c r="L112" s="105">
+      <c r="L112" s="102">
         <v>3</v>
       </c>
     </row>
     <row r="113" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A113" s="102" t="s">
-        <v>3</v>
-      </c>
-      <c r="B113" s="106" t="s">
+      <c r="A113" s="99" t="s">
+        <v>3</v>
+      </c>
+      <c r="B113" s="103" t="s">
         <v>294</v>
       </c>
-      <c r="C113" s="103" t="s">
+      <c r="C113" s="100" t="s">
         <v>95</v>
       </c>
-      <c r="D113" s="103" t="s">
-        <v>98</v>
-      </c>
-      <c r="E113" s="104" t="s">
+      <c r="D113" s="100" t="s">
+        <v>98</v>
+      </c>
+      <c r="E113" s="101" t="s">
         <v>295</v>
       </c>
-      <c r="F113" s="104" t="s">
+      <c r="F113" s="101" t="s">
         <v>155</v>
       </c>
-      <c r="G113" s="105" t="s">
+      <c r="G113" s="102" t="s">
         <v>141</v>
       </c>
-      <c r="H113" s="105" t="s">
+      <c r="H113" s="102" t="s">
         <v>33</v>
       </c>
-      <c r="I113" s="107" t="s">
+      <c r="I113" s="104" t="s">
         <v>296</v>
       </c>
-      <c r="J113" s="96" t="s">
+      <c r="J113" s="93" t="s">
         <v>297</v>
       </c>
-      <c r="K113" s="96" t="s">
+      <c r="K113" s="93" t="s">
         <v>298</v>
       </c>
-      <c r="L113" s="105">
+      <c r="L113" s="102">
         <v>3</v>
       </c>
     </row>
     <row r="114" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A114" s="102" t="s">
-        <v>3</v>
-      </c>
-      <c r="B114" s="106" t="s">
+      <c r="A114" s="99" t="s">
+        <v>3</v>
+      </c>
+      <c r="B114" s="103" t="s">
         <v>299</v>
       </c>
-      <c r="C114" s="103" t="s">
+      <c r="C114" s="100" t="s">
         <v>95</v>
       </c>
-      <c r="D114" s="103" t="s">
-        <v>98</v>
-      </c>
-      <c r="E114" s="104" t="s">
+      <c r="D114" s="100" t="s">
+        <v>98</v>
+      </c>
+      <c r="E114" s="101" t="s">
         <v>154</v>
       </c>
-      <c r="F114" s="104" t="s">
+      <c r="F114" s="101" t="s">
         <v>149</v>
       </c>
-      <c r="G114" s="105" t="s">
+      <c r="G114" s="102" t="s">
         <v>141</v>
       </c>
-      <c r="H114" s="105" t="s">
+      <c r="H114" s="102" t="s">
         <v>33</v>
       </c>
-      <c r="I114" s="107" t="s">
+      <c r="I114" s="68" t="s">
         <v>300</v>
       </c>
-      <c r="J114" s="108" t="s">
+      <c r="J114" s="105" t="s">
         <v>301</v>
       </c>
-      <c r="K114" s="108" t="s">
+      <c r="K114" s="105" t="s">
         <v>302</v>
       </c>
-      <c r="L114" s="105">
+      <c r="L114" s="102">
         <v>3</v>
       </c>
     </row>
     <row r="115" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A115" s="80" t="s">
+      <c r="A115" s="77" t="s">
         <v>3</v>
       </c>
       <c r="B115" s="73" t="s">
         <v>303</v>
       </c>
-      <c r="C115" s="100" t="s">
+      <c r="C115" s="97" t="s">
         <v>95</v>
       </c>
-      <c r="D115" s="100" t="s">
+      <c r="D115" s="97" t="s">
         <v>98</v>
       </c>
       <c r="E115" s="74" t="s">
@@ -7161,10 +7158,10 @@
       <c r="F115" s="74" t="s">
         <v>144</v>
       </c>
-      <c r="G115" s="94" t="s">
+      <c r="G115" s="91" t="s">
         <v>141</v>
       </c>
-      <c r="H115" s="94" t="s">
+      <c r="H115" s="91" t="s">
         <v>33</v>
       </c>
       <c r="I115" s="75" t="s">
@@ -7176,21 +7173,21 @@
       <c r="K115" s="75" t="s">
         <v>306</v>
       </c>
-      <c r="L115" s="94">
+      <c r="L115" s="91">
         <v>3</v>
       </c>
     </row>
     <row r="116" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A116" s="80" t="s">
+      <c r="A116" s="77" t="s">
         <v>3</v>
       </c>
       <c r="B116" s="73" t="s">
         <v>470</v>
       </c>
-      <c r="C116" s="100" t="s">
+      <c r="C116" s="97" t="s">
         <v>95</v>
       </c>
-      <c r="D116" s="100" t="s">
+      <c r="D116" s="97" t="s">
         <v>98</v>
       </c>
       <c r="E116" s="74" t="s">
@@ -7199,22 +7196,22 @@
       <c r="F116" s="74" t="s">
         <v>45</v>
       </c>
-      <c r="G116" s="94" t="s">
+      <c r="G116" s="91" t="s">
         <v>141</v>
       </c>
-      <c r="H116" s="94" t="s">
+      <c r="H116" s="91" t="s">
         <v>33</v>
       </c>
-      <c r="I116" s="79" t="s">
-        <v>304</v>
-      </c>
-      <c r="J116" s="79" t="s">
-        <v>305</v>
-      </c>
-      <c r="K116" s="79" t="s">
-        <v>306</v>
-      </c>
-      <c r="L116" s="94">
+      <c r="I116" s="75" t="s">
+        <v>126</v>
+      </c>
+      <c r="J116" s="75" t="s">
+        <v>476</v>
+      </c>
+      <c r="K116" s="75" t="s">
+        <v>477</v>
+      </c>
+      <c r="L116" s="91">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Texts (WIP) and Baby D. color rarity
Former-commit-id: 52686c7fd272e5dddbe2cdabe21d031a1acd1c48
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Powerups.xlsx
+++ b/Docs/Content/HungryDragonContent_Powerups.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1342" uniqueCount="509">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1342" uniqueCount="550">
   <si>
     <t>[sku]</t>
   </si>
@@ -1551,6 +1551,129 @@
   </si>
   <si>
     <t>Archer01;Archer02;BakerWoman;Catapulter;BadFarmer;RichMan;ShieldMan;Soldier;Villager01;Villager02;Villager03;Villager04;BadWitch;Bomber;Driller;GoodWitch;GoodWitch02;Kamikaze;Miner;SnailUnka;Spartakus;Witch;Worker;WorkerSpace</t>
+  </si>
+  <si>
+    <t>baby_lower_damage_origin</t>
+  </si>
+  <si>
+    <t>baby_prey_hp_boost</t>
+  </si>
+  <si>
+    <t>baby_speed_increase</t>
+  </si>
+  <si>
+    <t>baby_food_increase</t>
+  </si>
+  <si>
+    <t>baby_boost_increase</t>
+  </si>
+  <si>
+    <t>baby_score_increase</t>
+  </si>
+  <si>
+    <t>baby_transform_ice_cream</t>
+  </si>
+  <si>
+    <t>baby_phoenix</t>
+  </si>
+  <si>
+    <t>baby_kill</t>
+  </si>
+  <si>
+    <t>baby_shoot_horns</t>
+  </si>
+  <si>
+    <t>TID_POWERUP_BABY_TRANSFORM_VEGETABLES_NAME</t>
+  </si>
+  <si>
+    <t>TID_POWERUP_BABY_TRANSFORM_VEGETABLES_DESC</t>
+  </si>
+  <si>
+    <t>TID_POWERUP_BABY_DROP_PIZZA_NAME</t>
+  </si>
+  <si>
+    <t>TID_POWERUP_BABY_DROP_PIZZA_DESC</t>
+  </si>
+  <si>
+    <t>TID_POWERUP_BABY_DROP_PIZZA_DESC_SHORT</t>
+  </si>
+  <si>
+    <t>TID_POWERUP_BABY_PHOENIX_NAME</t>
+  </si>
+  <si>
+    <t>TID_POWERUP_BABY_PHOENIX_DESC</t>
+  </si>
+  <si>
+    <t>TID_POWERUP_BABY_PHOENIX_DESC_SHORT</t>
+  </si>
+  <si>
+    <t>TID_POWERUP_BABY_SUN_NAME</t>
+  </si>
+  <si>
+    <t>TID_POWERUP_BABY_SUN_DESC</t>
+  </si>
+  <si>
+    <t>TID_POWERUP_BABY_SUN_DESC_SHORT</t>
+  </si>
+  <si>
+    <t>TID_POWERUP_BABY_UNLIMITED_BOOST_NAME</t>
+  </si>
+  <si>
+    <t>TID_POWERUP_BABY_UNLIMITED_BOOST_DESC</t>
+  </si>
+  <si>
+    <t>TID_POWERUP_BABY_UNLIMITED_BOOST_DESC_SHORT</t>
+  </si>
+  <si>
+    <t>TID_POWERUP_BABY_MAGNET_NAME</t>
+  </si>
+  <si>
+    <t>TID_POWERUP_BABY_MAGNET_DESC</t>
+  </si>
+  <si>
+    <t>TID_POWERUP_BABY_MAGNET_DESC_SHORT</t>
+  </si>
+  <si>
+    <t>TID_POWERUP_BABY_ACIDBALL_NAME</t>
+  </si>
+  <si>
+    <t>TID_POWERUP_BABY_ACIDBALL_DESC</t>
+  </si>
+  <si>
+    <t>TID_POWERUP_BABY_ACIDBALL_DESC_SHORT</t>
+  </si>
+  <si>
+    <t>TID_POWERUP_BABY_SHOOT_SPINE_NAME</t>
+  </si>
+  <si>
+    <t>TID_POWERUP_BABY_SHOOT_SPINE_DESC</t>
+  </si>
+  <si>
+    <t>TID_POWERUP_BABY_SHOOT_SPINE_SHORT</t>
+  </si>
+  <si>
+    <t>TID_POWERUP_BABY_STUN_NAME</t>
+  </si>
+  <si>
+    <t>TID_POWERUP_BABY_STUN_DESC</t>
+  </si>
+  <si>
+    <t>TID_POWERUP_BABY_STUN_DESC_SHORT</t>
+  </si>
+  <si>
+    <t>TID_POWERUP_BABY_KILL_HUMANOID_BURP_NAME</t>
+  </si>
+  <si>
+    <t>TID_POWERUP_BABY_KILL_HUMANOID_BURP_DESC</t>
+  </si>
+  <si>
+    <t>TID_POWERUP_BABY_KILL_HUMANOID_BURP_DESC_SHORT</t>
+  </si>
+  <si>
+    <t>icon_power_baby</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TID_POWERUP_BABY_TRANSFORM_VEGETABLES_DESC_SHORT </t>
   </si>
 </sst>
 </file>
@@ -2320,14 +2443,14 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3247,8 +3370,8 @@
   </sheetPr>
   <dimension ref="A1:L144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
-      <selection activeCell="E123" sqref="E123"/>
+    <sheetView tabSelected="1" topLeftCell="H103" workbookViewId="0">
+      <selection activeCell="K130" sqref="K130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7619,7 +7742,7 @@
         <v>489</v>
       </c>
       <c r="C121" s="121" t="s">
-        <v>14</v>
+        <v>489</v>
       </c>
       <c r="D121" s="121" t="s">
         <v>98</v>
@@ -7628,8 +7751,8 @@
         <v>10</v>
       </c>
       <c r="F121" s="122"/>
-      <c r="G121" s="123" t="s">
-        <v>138</v>
+      <c r="G121" s="139" t="s">
+        <v>548</v>
       </c>
       <c r="H121" s="123" t="s">
         <v>42</v>
@@ -7655,7 +7778,7 @@
         <v>490</v>
       </c>
       <c r="C122" s="107" t="s">
-        <v>80</v>
+        <v>509</v>
       </c>
       <c r="D122" s="107" t="s">
         <v>98</v>
@@ -7666,8 +7789,8 @@
       <c r="F122" s="108">
         <v>10</v>
       </c>
-      <c r="G122" s="128" t="s">
-        <v>140</v>
+      <c r="G122" s="46" t="s">
+        <v>548</v>
       </c>
       <c r="H122" s="128" t="s">
         <v>27</v>
@@ -7693,7 +7816,7 @@
         <v>491</v>
       </c>
       <c r="C123" s="107" t="s">
-        <v>63</v>
+        <v>510</v>
       </c>
       <c r="D123" s="107" t="s">
         <v>98</v>
@@ -7704,8 +7827,8 @@
       <c r="F123" s="108">
         <v>30</v>
       </c>
-      <c r="G123" s="128" t="s">
-        <v>137</v>
+      <c r="G123" s="46" t="s">
+        <v>548</v>
       </c>
       <c r="H123" s="128" t="s">
         <v>37</v>
@@ -7731,7 +7854,7 @@
         <v>495</v>
       </c>
       <c r="C124" s="22" t="s">
-        <v>56</v>
+        <v>511</v>
       </c>
       <c r="D124" s="22" t="s">
         <v>98</v>
@@ -7740,8 +7863,8 @@
         <v>10</v>
       </c>
       <c r="F124" s="23"/>
-      <c r="G124" s="133" t="s">
-        <v>135</v>
+      <c r="G124" s="18" t="s">
+        <v>548</v>
       </c>
       <c r="H124" s="133" t="s">
         <v>31</v>
@@ -7767,7 +7890,7 @@
         <v>497</v>
       </c>
       <c r="C125" s="136" t="s">
-        <v>63</v>
+        <v>510</v>
       </c>
       <c r="D125" s="6" t="s">
         <v>98</v>
@@ -7778,8 +7901,8 @@
       <c r="F125" s="137">
         <v>30</v>
       </c>
-      <c r="G125" s="138" t="s">
-        <v>137</v>
+      <c r="G125" s="140" t="s">
+        <v>548</v>
       </c>
       <c r="H125" s="133" t="s">
         <v>37</v>
@@ -7790,7 +7913,7 @@
       <c r="J125" s="135" t="s">
         <v>351</v>
       </c>
-      <c r="K125" s="139" t="s">
+      <c r="K125" s="138" t="s">
         <v>352</v>
       </c>
       <c r="L125" s="132">
@@ -7805,7 +7928,7 @@
         <v>499</v>
       </c>
       <c r="C126" s="6" t="s">
-        <v>43</v>
+        <v>512</v>
       </c>
       <c r="D126" s="6" t="s">
         <v>98</v>
@@ -7814,8 +7937,8 @@
         <v>10</v>
       </c>
       <c r="F126" s="17"/>
-      <c r="G126" s="133" t="s">
-        <v>137</v>
+      <c r="G126" s="18" t="s">
+        <v>548</v>
       </c>
       <c r="H126" s="133" t="s">
         <v>44</v>
@@ -7841,7 +7964,7 @@
         <v>502</v>
       </c>
       <c r="C127" s="26" t="s">
-        <v>10</v>
+        <v>502</v>
       </c>
       <c r="D127" s="26" t="s">
         <v>98</v>
@@ -7850,8 +7973,8 @@
         <v>5</v>
       </c>
       <c r="F127" s="27"/>
-      <c r="G127" s="140" t="s">
-        <v>136</v>
+      <c r="G127" s="28" t="s">
+        <v>548</v>
       </c>
       <c r="H127" s="133" t="s">
         <v>4</v>
@@ -7862,7 +7985,7 @@
       <c r="J127" s="135" t="s">
         <v>187</v>
       </c>
-      <c r="K127" s="139" t="s">
+      <c r="K127" s="138" t="s">
         <v>335</v>
       </c>
       <c r="L127" s="132">
@@ -7877,7 +8000,7 @@
         <v>504</v>
       </c>
       <c r="C128" s="6" t="s">
-        <v>30</v>
+        <v>513</v>
       </c>
       <c r="D128" s="6" t="s">
         <v>98</v>
@@ -7886,8 +8009,8 @@
         <v>10</v>
       </c>
       <c r="F128" s="17"/>
-      <c r="G128" s="133" t="s">
-        <v>135</v>
+      <c r="G128" s="18" t="s">
+        <v>548</v>
       </c>
       <c r="H128" s="133" t="s">
         <v>31</v>
@@ -7913,7 +8036,7 @@
         <v>506</v>
       </c>
       <c r="C129" s="6" t="s">
-        <v>55</v>
+        <v>514</v>
       </c>
       <c r="D129" s="6" t="s">
         <v>98</v>
@@ -7922,8 +8045,8 @@
         <v>20</v>
       </c>
       <c r="F129" s="17"/>
-      <c r="G129" s="133" t="s">
-        <v>136</v>
+      <c r="G129" s="18" t="s">
+        <v>548</v>
       </c>
       <c r="H129" s="133" t="s">
         <v>4</v>
@@ -7949,27 +8072,27 @@
         <v>492</v>
       </c>
       <c r="C130" s="22" t="s">
-        <v>102</v>
+        <v>515</v>
       </c>
       <c r="D130" s="107" t="s">
         <v>99</v>
       </c>
       <c r="E130" s="108"/>
       <c r="F130" s="108"/>
-      <c r="G130" s="128" t="s">
-        <v>141</v>
+      <c r="G130" s="46" t="s">
+        <v>548</v>
       </c>
       <c r="H130" s="128" t="s">
         <v>33</v>
       </c>
-      <c r="I130" s="129" t="s">
-        <v>109</v>
-      </c>
-      <c r="J130" s="130" t="s">
-        <v>110</v>
-      </c>
-      <c r="K130" s="131" t="s">
-        <v>111</v>
+      <c r="I130" s="47" t="s">
+        <v>519</v>
+      </c>
+      <c r="J130" s="48" t="s">
+        <v>520</v>
+      </c>
+      <c r="K130" s="49" t="s">
+        <v>549</v>
       </c>
       <c r="L130" s="132">
         <v>0</v>
@@ -7983,7 +8106,7 @@
         <v>493</v>
       </c>
       <c r="C131" s="107" t="s">
-        <v>54</v>
+        <v>516</v>
       </c>
       <c r="D131" s="107" t="s">
         <v>99</v>
@@ -7992,20 +8115,20 @@
         <v>1</v>
       </c>
       <c r="F131" s="108"/>
-      <c r="G131" s="128" t="s">
-        <v>141</v>
+      <c r="G131" s="46" t="s">
+        <v>548</v>
       </c>
       <c r="H131" s="128" t="s">
         <v>33</v>
       </c>
-      <c r="I131" s="129" t="s">
-        <v>412</v>
-      </c>
-      <c r="J131" s="130" t="s">
-        <v>413</v>
-      </c>
-      <c r="K131" s="131" t="s">
-        <v>414</v>
+      <c r="I131" s="47" t="s">
+        <v>524</v>
+      </c>
+      <c r="J131" s="48" t="s">
+        <v>525</v>
+      </c>
+      <c r="K131" s="49" t="s">
+        <v>526</v>
       </c>
       <c r="L131" s="132">
         <v>0</v>
@@ -8019,27 +8142,27 @@
         <v>494</v>
       </c>
       <c r="C132" s="107" t="s">
-        <v>119</v>
+        <v>517</v>
       </c>
       <c r="D132" s="107" t="s">
         <v>99</v>
       </c>
       <c r="E132" s="108"/>
       <c r="F132" s="108"/>
-      <c r="G132" s="128" t="s">
-        <v>141</v>
+      <c r="G132" s="46" t="s">
+        <v>548</v>
       </c>
       <c r="H132" s="128" t="s">
         <v>33</v>
       </c>
-      <c r="I132" s="129" t="s">
-        <v>123</v>
-      </c>
-      <c r="J132" s="130" t="s">
-        <v>124</v>
-      </c>
-      <c r="K132" s="131" t="s">
-        <v>125</v>
+      <c r="I132" s="47" t="s">
+        <v>545</v>
+      </c>
+      <c r="J132" s="48" t="s">
+        <v>546</v>
+      </c>
+      <c r="K132" s="49" t="s">
+        <v>547</v>
       </c>
       <c r="L132" s="132">
         <v>0</v>
@@ -8053,27 +8176,27 @@
         <v>498</v>
       </c>
       <c r="C133" s="22" t="s">
-        <v>74</v>
+        <v>498</v>
       </c>
       <c r="D133" s="6" t="s">
         <v>99</v>
       </c>
       <c r="E133" s="23"/>
       <c r="F133" s="23"/>
-      <c r="G133" s="128" t="s">
-        <v>135</v>
+      <c r="G133" s="46" t="s">
+        <v>548</v>
       </c>
       <c r="H133" s="128" t="s">
         <v>31</v>
       </c>
-      <c r="I133" s="129" t="s">
-        <v>436</v>
-      </c>
-      <c r="J133" s="130" t="s">
-        <v>437</v>
-      </c>
-      <c r="K133" s="131" t="s">
-        <v>438</v>
+      <c r="I133" s="47" t="s">
+        <v>530</v>
+      </c>
+      <c r="J133" s="48" t="s">
+        <v>531</v>
+      </c>
+      <c r="K133" s="49" t="s">
+        <v>532</v>
       </c>
       <c r="L133" s="132">
         <v>0</v>
@@ -8087,7 +8210,7 @@
         <v>496</v>
       </c>
       <c r="C134" s="22" t="s">
-        <v>53</v>
+        <v>496</v>
       </c>
       <c r="D134" s="22" t="s">
         <v>99</v>
@@ -8096,20 +8219,20 @@
         <v>1</v>
       </c>
       <c r="F134" s="23"/>
-      <c r="G134" s="128" t="s">
-        <v>141</v>
+      <c r="G134" s="46" t="s">
+        <v>548</v>
       </c>
       <c r="H134" s="128" t="s">
         <v>33</v>
       </c>
-      <c r="I134" s="129" t="s">
-        <v>409</v>
-      </c>
-      <c r="J134" s="130" t="s">
-        <v>410</v>
-      </c>
-      <c r="K134" s="131" t="s">
-        <v>411</v>
+      <c r="I134" s="47" t="s">
+        <v>533</v>
+      </c>
+      <c r="J134" s="48" t="s">
+        <v>534</v>
+      </c>
+      <c r="K134" s="49" t="s">
+        <v>535</v>
       </c>
       <c r="L134" s="132">
         <v>0</v>
@@ -8123,27 +8246,27 @@
         <v>500</v>
       </c>
       <c r="C135" s="22" t="s">
-        <v>72</v>
+        <v>500</v>
       </c>
       <c r="D135" s="22" t="s">
         <v>99</v>
       </c>
       <c r="E135" s="23"/>
       <c r="F135" s="23"/>
-      <c r="G135" s="128" t="s">
-        <v>141</v>
+      <c r="G135" s="46" t="s">
+        <v>548</v>
       </c>
       <c r="H135" s="128" t="s">
         <v>33</v>
       </c>
-      <c r="I135" s="129" t="s">
-        <v>433</v>
-      </c>
-      <c r="J135" s="130" t="s">
-        <v>434</v>
-      </c>
-      <c r="K135" s="131" t="s">
-        <v>435</v>
+      <c r="I135" s="47" t="s">
+        <v>542</v>
+      </c>
+      <c r="J135" s="48" t="s">
+        <v>543</v>
+      </c>
+      <c r="K135" s="49" t="s">
+        <v>544</v>
       </c>
       <c r="L135" s="132">
         <v>0</v>
@@ -8157,7 +8280,7 @@
         <v>501</v>
       </c>
       <c r="C136" s="22" t="s">
-        <v>41</v>
+        <v>501</v>
       </c>
       <c r="D136" s="22" t="s">
         <v>99</v>
@@ -8166,20 +8289,20 @@
         <v>1</v>
       </c>
       <c r="F136" s="23"/>
-      <c r="G136" s="128" t="s">
-        <v>138</v>
+      <c r="G136" s="46" t="s">
+        <v>548</v>
       </c>
       <c r="H136" s="128" t="s">
         <v>42</v>
       </c>
-      <c r="I136" s="129" t="s">
-        <v>400</v>
-      </c>
-      <c r="J136" s="130" t="s">
-        <v>401</v>
-      </c>
-      <c r="K136" s="131" t="s">
-        <v>402</v>
+      <c r="I136" s="47" t="s">
+        <v>536</v>
+      </c>
+      <c r="J136" s="48" t="s">
+        <v>537</v>
+      </c>
+      <c r="K136" s="49" t="s">
+        <v>538</v>
       </c>
       <c r="L136" s="132">
         <v>0</v>
@@ -8193,27 +8316,27 @@
         <v>503</v>
       </c>
       <c r="C137" s="107" t="s">
-        <v>100</v>
+        <v>503</v>
       </c>
       <c r="D137" s="107" t="s">
         <v>99</v>
       </c>
       <c r="E137" s="108"/>
       <c r="F137" s="108"/>
-      <c r="G137" s="128" t="s">
-        <v>141</v>
+      <c r="G137" s="46" t="s">
+        <v>548</v>
       </c>
       <c r="H137" s="128" t="s">
         <v>33</v>
       </c>
-      <c r="I137" s="129" t="s">
-        <v>103</v>
-      </c>
-      <c r="J137" s="130" t="s">
-        <v>104</v>
-      </c>
-      <c r="K137" s="131" t="s">
-        <v>105</v>
+      <c r="I137" s="47" t="s">
+        <v>527</v>
+      </c>
+      <c r="J137" s="48" t="s">
+        <v>528</v>
+      </c>
+      <c r="K137" s="49" t="s">
+        <v>529</v>
       </c>
       <c r="L137" s="132">
         <v>0</v>
@@ -8227,7 +8350,7 @@
         <v>505</v>
       </c>
       <c r="C138" s="107" t="s">
-        <v>85</v>
+        <v>505</v>
       </c>
       <c r="D138" s="107" t="s">
         <v>99</v>
@@ -8238,20 +8361,20 @@
       <c r="F138" s="108">
         <v>1</v>
       </c>
-      <c r="G138" s="128" t="s">
-        <v>137</v>
+      <c r="G138" s="46" t="s">
+        <v>548</v>
       </c>
       <c r="H138" s="128" t="s">
         <v>37</v>
       </c>
-      <c r="I138" s="129" t="s">
-        <v>451</v>
-      </c>
-      <c r="J138" s="130" t="s">
-        <v>452</v>
-      </c>
-      <c r="K138" s="131" t="s">
-        <v>453</v>
+      <c r="I138" s="47" t="s">
+        <v>521</v>
+      </c>
+      <c r="J138" s="48" t="s">
+        <v>522</v>
+      </c>
+      <c r="K138" s="49" t="s">
+        <v>523</v>
       </c>
       <c r="L138" s="132">
         <v>0</v>
@@ -8265,27 +8388,27 @@
         <v>507</v>
       </c>
       <c r="C139" s="107" t="s">
-        <v>112</v>
+        <v>518</v>
       </c>
       <c r="D139" s="107" t="s">
         <v>99</v>
       </c>
       <c r="E139" s="108"/>
       <c r="F139" s="108"/>
-      <c r="G139" s="128" t="s">
-        <v>141</v>
+      <c r="G139" s="46" t="s">
+        <v>548</v>
       </c>
       <c r="H139" s="128" t="s">
         <v>33</v>
       </c>
-      <c r="I139" s="129" t="s">
-        <v>113</v>
-      </c>
-      <c r="J139" s="130" t="s">
-        <v>114</v>
-      </c>
-      <c r="K139" s="131" t="s">
-        <v>115</v>
+      <c r="I139" s="47" t="s">
+        <v>539</v>
+      </c>
+      <c r="J139" s="48" t="s">
+        <v>540</v>
+      </c>
+      <c r="K139" s="49" t="s">
+        <v>541</v>
       </c>
       <c r="L139" s="132">
         <v>0</v>

</xml_diff>

<commit_message>
Fixing a tid name
Former-commit-id: 7ddd48ef89b6b3a80eb5b75ea3623ad503d1fb2b
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Powerups.xlsx
+++ b/Docs/Content/HungryDragonContent_Powerups.xlsx
@@ -1673,7 +1673,7 @@
     <t>icon_power_baby</t>
   </si>
   <si>
-    <t xml:space="preserve">TID_POWERUP_BABY_TRANSFORM_VEGETABLES_DESC_SHORT </t>
+    <t>TID_POWERUP_BABY_TRANSFORM_VEGETABLES_DESC_SHORT</t>
   </si>
 </sst>
 </file>
@@ -3370,8 +3370,8 @@
   </sheetPr>
   <dimension ref="A1:L144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H103" workbookViewId="0">
-      <selection activeCell="K130" sqref="K130"/>
+    <sheetView tabSelected="1" topLeftCell="H106" workbookViewId="0">
+      <selection activeCell="K132" sqref="K132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
added new power for community dragon
Former-commit-id: dbd8cdf0df493d66c2e100d566e749b3a2acca7e
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Powerups.xlsx
+++ b/Docs/Content/HungryDragonContent_Powerups.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ubi\HungryDragon\HD_Client\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\client\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A7CCF4F-E799-49F0-864D-9840A959F6A9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21840"/>
   </bookViews>
   <sheets>
     <sheet name="powerups" sheetId="6" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1342" uniqueCount="540">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1350" uniqueCount="541">
   <si>
     <t>[sku]</t>
   </si>
@@ -1645,12 +1644,15 @@
   </si>
   <si>
     <t>TID_POWERUP_BABY_TRANSFORM_VEGETABLES_DESC_SHORT</t>
+  </si>
+  <si>
+    <t>disguise_speed_boost_disguise_lower_damage_poison</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1804,7 +1806,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -2015,11 +2017,79 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="141">
+  <cellXfs count="162">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2423,6 +2493,67 @@
     <xf numFmtId="0" fontId="6" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3042,29 +3173,29 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="powerUpsDefinitions2" displayName="powerUpsDefinitions2" ref="A3:L139" totalsRowShown="0" headerRowDxfId="28" dataDxfId="26" headerRowBorderDxfId="27" tableBorderDxfId="25" totalsRowBorderDxfId="24">
-  <autoFilter ref="A3:L139" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="powerUpsDefinitions2" displayName="powerUpsDefinitions2" ref="A3:L140" totalsRowShown="0" headerRowDxfId="28" dataDxfId="26" headerRowBorderDxfId="27" tableBorderDxfId="25" totalsRowBorderDxfId="24">
+  <autoFilter ref="A3:L140"/>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="{powerUpsDefinitions}" dataDxfId="23" totalsRowDxfId="22"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="[sku]" dataDxfId="21" totalsRowDxfId="20"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="[type]" dataDxfId="19" totalsRowDxfId="18"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="[category]" dataDxfId="17" totalsRowDxfId="16"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="[param1]" dataDxfId="15" totalsRowDxfId="14"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="[param2]" dataDxfId="13" totalsRowDxfId="12"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="[icon]" dataDxfId="11" totalsRowDxfId="10">
+    <tableColumn id="1" name="{powerUpsDefinitions}" dataDxfId="23" totalsRowDxfId="22"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="21" totalsRowDxfId="20"/>
+    <tableColumn id="3" name="[type]" dataDxfId="19" totalsRowDxfId="18"/>
+    <tableColumn id="11" name="[category]" dataDxfId="17" totalsRowDxfId="16"/>
+    <tableColumn id="4" name="[param1]" dataDxfId="15" totalsRowDxfId="14"/>
+    <tableColumn id="5" name="[param2]" dataDxfId="13" totalsRowDxfId="12"/>
+    <tableColumn id="6" name="[icon]" dataDxfId="11" totalsRowDxfId="10">
       <calculatedColumnFormula>CONCATENATE("icon_",powerUpsDefinitions2[[#This Row],['[sku']]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="[miniIcon]" dataDxfId="9" totalsRowDxfId="8"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="[tidName]" dataDxfId="7" totalsRowDxfId="6">
+    <tableColumn id="10" name="[miniIcon]" dataDxfId="9" totalsRowDxfId="8"/>
+    <tableColumn id="7" name="[tidName]" dataDxfId="7" totalsRowDxfId="6">
       <calculatedColumnFormula>CONCATENATE("TID_POWERUP_",UPPER(powerUpsDefinitions2[[#This Row],['[sku']]]),"_NAME")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="[tidDesc]" dataDxfId="5" totalsRowDxfId="4">
+    <tableColumn id="8" name="[tidDesc]" dataDxfId="5" totalsRowDxfId="4">
       <calculatedColumnFormula>CONCATENATE("TID_POWERUP_",UPPER(powerUpsDefinitions2[[#This Row],['[sku']]]),"_DESC")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="[tidDescShort]" dataDxfId="3" totalsRowDxfId="2">
+    <tableColumn id="9" name="[tidDescShort]" dataDxfId="3" totalsRowDxfId="2">
       <calculatedColumnFormula>CONCATENATE(powerUpsDefinitions2[[#This Row],['[tidDesc']]],"_SHORT")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="[level]" dataDxfId="1" totalsRowDxfId="0"/>
+    <tableColumn id="12" name="[level]" dataDxfId="1" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3332,14 +3463,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="7"/>
   </sheetPr>
-  <dimension ref="A1:L144"/>
+  <dimension ref="A1:L145"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23:D24"/>
+    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="I140" sqref="I140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3352,7 +3483,7 @@
     <col min="6" max="6" width="45.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="52.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="54.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="53.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="60.7109375" customWidth="1"/>
     <col min="10" max="10" width="60.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="52.42578125" bestFit="1" customWidth="1"/>
   </cols>
@@ -8348,84 +8479,125 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A139" s="111" t="s">
-        <v>3</v>
-      </c>
-      <c r="B139" s="106" t="s">
+    <row r="139" spans="1:12" s="161" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A139" s="151" t="s">
+        <v>3</v>
+      </c>
+      <c r="B139" s="152" t="s">
         <v>507</v>
       </c>
-      <c r="C139" s="107" t="s">
+      <c r="C139" s="153" t="s">
         <v>112</v>
       </c>
-      <c r="D139" s="107" t="s">
+      <c r="D139" s="153" t="s">
         <v>99</v>
       </c>
-      <c r="E139" s="108"/>
-      <c r="F139" s="108"/>
-      <c r="G139" s="138" t="s">
+      <c r="E139" s="154"/>
+      <c r="F139" s="154"/>
+      <c r="G139" s="155" t="s">
         <v>538</v>
       </c>
-      <c r="H139" s="127" t="s">
+      <c r="H139" s="156" t="s">
         <v>33</v>
       </c>
-      <c r="I139" s="47" t="s">
+      <c r="I139" s="157" t="s">
         <v>529</v>
       </c>
-      <c r="J139" s="48" t="s">
+      <c r="J139" s="158" t="s">
         <v>530</v>
       </c>
-      <c r="K139" s="49" t="s">
+      <c r="K139" s="159" t="s">
         <v>531</v>
       </c>
-      <c r="L139" s="131">
+      <c r="L139" s="160">
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="141" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A141" s="1" t="s">
+    <row r="140" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A140" s="141" t="s">
+        <v>3</v>
+      </c>
+      <c r="B140" s="147" t="s">
+        <v>540</v>
+      </c>
+      <c r="C140" s="148" t="s">
+        <v>95</v>
+      </c>
+      <c r="D140" s="148" t="s">
+        <v>98</v>
+      </c>
+      <c r="E140" s="142" t="s">
+        <v>150</v>
+      </c>
+      <c r="F140" s="142" t="s">
+        <v>146</v>
+      </c>
+      <c r="G140" s="143" t="s">
+        <v>141</v>
+      </c>
+      <c r="H140" s="149" t="s">
+        <v>33</v>
+      </c>
+      <c r="I140" s="144" t="str">
+        <f>CONCATENATE("TID_POWERUP_",UPPER(powerUpsDefinitions2[[#This Row],['[sku']]]),"_NAME")</f>
+        <v>TID_POWERUP_DISGUISE_SPEED_BOOST_DISGUISE_LOWER_DAMAGE_POISON_NAME</v>
+      </c>
+      <c r="J140" s="145" t="str">
+        <f>CONCATENATE("TID_POWERUP_",UPPER(powerUpsDefinitions2[[#This Row],['[sku']]]),"_DESC")</f>
+        <v>TID_POWERUP_DISGUISE_SPEED_BOOST_DISGUISE_LOWER_DAMAGE_POISON_DESC</v>
+      </c>
+      <c r="K140" s="146" t="str">
+        <f>CONCATENATE(powerUpsDefinitions2[[#This Row],['[tidDesc']]],"_SHORT")</f>
+        <v>TID_POWERUP_DISGUISE_SPEED_BOOST_DISGUISE_LOWER_DAMAGE_POISON_DESC_SHORT</v>
+      </c>
+      <c r="L140" s="150">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="141" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="142" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A142" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B141" s="1"/>
-      <c r="C141" s="1"/>
-      <c r="D141" s="1"/>
-      <c r="E141" s="1"/>
-      <c r="F141" s="1"/>
-      <c r="G141" s="1"/>
-      <c r="H141" s="1"/>
-    </row>
-    <row r="143" spans="1:12" ht="136.5" x14ac:dyDescent="0.25">
-      <c r="A143" s="2" t="s">
+      <c r="B142" s="1"/>
+      <c r="C142" s="1"/>
+      <c r="D142" s="1"/>
+      <c r="E142" s="1"/>
+      <c r="F142" s="1"/>
+      <c r="G142" s="1"/>
+      <c r="H142" s="1"/>
+    </row>
+    <row r="144" spans="1:12" ht="136.5" x14ac:dyDescent="0.25">
+      <c r="A144" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="B143" s="2" t="s">
+      <c r="B144" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C143" s="50" t="s">
+      <c r="C144" s="50" t="s">
         <v>88</v>
       </c>
-      <c r="D143" s="51" t="s">
+      <c r="D144" s="51" t="s">
         <v>89</v>
       </c>
-      <c r="E143" s="51" t="s">
+      <c r="E144" s="51" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="144" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A144" s="52" t="s">
-        <v>3</v>
-      </c>
-      <c r="B144" s="4" t="s">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A145" s="52" t="s">
+        <v>3</v>
+      </c>
+      <c r="B145" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="C144" s="3">
+      <c r="C145" s="3">
         <v>11</v>
       </c>
-      <c r="D144" s="5">
+      <c r="D145" s="5">
         <v>2.2999999999999998</v>
       </c>
-      <c r="E144" s="5">
+      <c r="E145" s="5">
         <v>0.25</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixes on content Disable last power we are not using now
Former-commit-id: 3e6b0a8dcc817e2c557f9ce5aebbeef486972220
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Powerups.xlsx
+++ b/Docs/Content/HungryDragonContent_Powerups.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1456" uniqueCount="573">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1455" uniqueCount="573">
   <si>
     <t>[sku]</t>
   </si>
@@ -3280,33 +3280,7 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="powerUpsDefinitions2" displayName="powerUpsDefinitions2" ref="A3:L150" totalsRowShown="0" headerRowDxfId="28" dataDxfId="26" headerRowBorderDxfId="27" tableBorderDxfId="25" totalsRowBorderDxfId="24">
-  <autoFilter ref="A3:L150">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="baby_speed"/>
-        <filter val="disguise_furyDuration_lowerDamageMine_speed"/>
-        <filter val="disguise_furySize_boost_speed"/>
-        <filter val="disguise_speed"/>
-        <filter val="disguise_speed_boost"/>
-        <filter val="disguise_speed_boost_LOW"/>
-        <filter val="disguise_speed_fury_duration_LOW_lower_damage_poison"/>
-        <filter val="disguise_speed_fury_duration_lower_damage_poison"/>
-        <filter val="disguise_speed_furyDuration"/>
-        <filter val="disguise_speed_furyDuration_LOW"/>
-        <filter val="disguise_speed_hp"/>
-        <filter val="disguise_speed_hp_disguise_lower_damage_mine"/>
-        <filter val="disguise_speed_LOW"/>
-        <filter val="disguise_speed_LOW_boost_LOW"/>
-        <filter val="disguise_speed_LOW_boost_LOW_hp"/>
-        <filter val="disguise_speed_LOW_boost_LOW_lower_damage_poison"/>
-        <filter val="disguise_speed_LOW_hp"/>
-        <filter val="disguise_speed_LOW_hp_free_revive"/>
-        <filter val="disguise_speed_LOW_hp_LOW"/>
-        <filter val="disguise_speed_moreXp"/>
-        <filter val="speed"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A3:L150"/>
   <tableColumns count="12">
     <tableColumn id="1" name="{powerUpsDefinitions}" dataDxfId="23" totalsRowDxfId="22"/>
     <tableColumn id="2" name="[sku]" dataDxfId="21" totalsRowDxfId="20"/>
@@ -3601,8 +3575,8 @@
   </sheetPr>
   <dimension ref="A1:L155"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
-      <selection activeCell="B147" sqref="B147"/>
+    <sheetView tabSelected="1" topLeftCell="A103" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
+      <selection activeCell="A150" sqref="A150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3641,7 +3615,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="113.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="114" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>19</v>
       </c>
@@ -3679,7 +3653,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>3</v>
       </c>
@@ -3715,7 +3689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>3</v>
       </c>
@@ -3751,7 +3725,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
         <v>3</v>
       </c>
@@ -3787,7 +3761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
         <v>3</v>
       </c>
@@ -3823,7 +3797,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:12" s="61" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" s="61" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
         <v>3</v>
       </c>
@@ -3859,7 +3833,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
         <v>3</v>
       </c>
@@ -3895,7 +3869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
         <v>3</v>
       </c>
@@ -3931,7 +3905,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
         <v>3</v>
       </c>
@@ -3969,7 +3943,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
         <v>3</v>
       </c>
@@ -4007,7 +3981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
         <v>3</v>
       </c>
@@ -4045,7 +4019,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="24" t="s">
         <v>3</v>
       </c>
@@ -4081,7 +4055,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
         <v>3</v>
       </c>
@@ -4117,7 +4091,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
         <v>3</v>
       </c>
@@ -4153,7 +4127,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:12" s="61" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" s="61" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
         <v>3</v>
       </c>
@@ -4225,7 +4199,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="36" t="s">
         <v>3</v>
       </c>
@@ -4263,7 +4237,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
         <v>3</v>
       </c>
@@ -4301,7 +4275,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
         <v>3</v>
       </c>
@@ -4339,7 +4313,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="15" t="s">
         <v>3</v>
       </c>
@@ -4377,7 +4351,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="15" t="s">
         <v>3</v>
       </c>
@@ -4413,7 +4387,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="15" t="s">
         <v>3</v>
       </c>
@@ -4451,7 +4425,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="15" t="s">
         <v>3</v>
       </c>
@@ -4487,7 +4461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="15" t="s">
         <v>3</v>
       </c>
@@ -4523,7 +4497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="15" t="s">
         <v>3</v>
       </c>
@@ -4561,7 +4535,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:12" s="61" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" s="61" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="15" t="s">
         <v>3</v>
       </c>
@@ -4599,7 +4573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="15" t="s">
         <v>3</v>
       </c>
@@ -4637,7 +4611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="15" t="s">
         <v>3</v>
       </c>
@@ -4675,7 +4649,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="15" t="s">
         <v>3</v>
       </c>
@@ -4709,7 +4683,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="15" t="s">
         <v>3</v>
       </c>
@@ -4745,7 +4719,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="15" t="s">
         <v>3</v>
       </c>
@@ -4781,7 +4755,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="15" t="s">
         <v>3</v>
       </c>
@@ -4817,7 +4791,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="15" t="s">
         <v>3</v>
       </c>
@@ -4855,7 +4829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="15" t="s">
         <v>3</v>
       </c>
@@ -4891,7 +4865,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="15" t="s">
         <v>3</v>
       </c>
@@ -4927,7 +4901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="15" t="s">
         <v>3</v>
       </c>
@@ -4963,7 +4937,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="15" t="s">
         <v>3</v>
       </c>
@@ -4999,7 +4973,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="15" t="s">
         <v>3</v>
       </c>
@@ -5035,7 +5009,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="15" t="s">
         <v>3</v>
       </c>
@@ -5071,7 +5045,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="15" t="s">
         <v>3</v>
       </c>
@@ -5107,7 +5081,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="15" t="s">
         <v>3</v>
       </c>
@@ -5143,7 +5117,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="15" t="s">
         <v>3</v>
       </c>
@@ -5179,7 +5153,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="15" t="s">
         <v>3</v>
       </c>
@@ -5215,7 +5189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="15" t="s">
         <v>3</v>
       </c>
@@ -5249,7 +5223,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="15" t="s">
         <v>3</v>
       </c>
@@ -5283,7 +5257,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="15" t="s">
         <v>3</v>
       </c>
@@ -5317,7 +5291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="45" t="s">
         <v>3</v>
       </c>
@@ -5351,7 +5325,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" s="45" t="s">
         <v>3</v>
       </c>
@@ -5385,7 +5359,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" s="45" t="s">
         <v>3</v>
       </c>
@@ -5419,7 +5393,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" s="15" t="s">
         <v>3</v>
       </c>
@@ -5453,7 +5427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" s="15" t="s">
         <v>3</v>
       </c>
@@ -5487,7 +5461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" s="15" t="s">
         <v>3</v>
       </c>
@@ -5525,7 +5499,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" s="15" t="s">
         <v>3</v>
       </c>
@@ -5563,7 +5537,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" s="15" t="s">
         <v>3</v>
       </c>
@@ -5599,7 +5573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" s="15" t="s">
         <v>3</v>
       </c>
@@ -5633,7 +5607,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" s="15" t="s">
         <v>3</v>
       </c>
@@ -5667,7 +5641,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" s="45" t="s">
         <v>3</v>
       </c>
@@ -5701,7 +5675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:12" s="54" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" s="54" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="85" t="s">
         <v>3</v>
       </c>
@@ -5735,7 +5709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:12" s="55" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" s="55" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="56" t="s">
         <v>3</v>
       </c>
@@ -5769,7 +5743,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:12" s="55" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" s="55" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="56" t="s">
         <v>3</v>
       </c>
@@ -5803,7 +5777,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:12" s="55" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12" s="55" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="56" t="s">
         <v>3</v>
       </c>
@@ -5837,7 +5811,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:12" s="55" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" s="55" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="56" t="s">
         <v>3</v>
       </c>
@@ -5871,7 +5845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:12" s="55" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12" s="55" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="56" t="s">
         <v>3</v>
       </c>
@@ -5907,7 +5881,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:12" s="55" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12" s="55" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="56" t="s">
         <v>3</v>
       </c>
@@ -5943,7 +5917,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67" s="88" t="s">
         <v>3</v>
       </c>
@@ -5979,7 +5953,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68" s="88" t="s">
         <v>3</v>
       </c>
@@ -6015,7 +5989,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69" s="88" t="s">
         <v>3</v>
       </c>
@@ -6051,7 +6025,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A70" s="88" t="s">
         <v>3</v>
       </c>
@@ -6159,7 +6133,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A73" s="88" t="s">
         <v>3</v>
       </c>
@@ -6193,7 +6167,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A74" s="88" t="s">
         <v>3</v>
       </c>
@@ -6229,7 +6203,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A75" s="88" t="s">
         <v>3</v>
       </c>
@@ -6265,7 +6239,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A76" s="88" t="s">
         <v>3</v>
       </c>
@@ -6303,7 +6277,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A77" s="88" t="s">
         <v>3</v>
       </c>
@@ -6341,7 +6315,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A78" s="88" t="s">
         <v>3</v>
       </c>
@@ -6379,7 +6353,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A79" s="95" t="s">
         <v>3</v>
       </c>
@@ -6415,7 +6389,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A80" s="88" t="s">
         <v>3</v>
       </c>
@@ -6451,7 +6425,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A81" s="88" t="s">
         <v>3</v>
       </c>
@@ -6487,7 +6461,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A82" s="99" t="s">
         <v>3</v>
       </c>
@@ -6599,7 +6573,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="85" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A85" s="45" t="s">
         <v>3</v>
       </c>
@@ -6637,7 +6611,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="86" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A86" s="45" t="s">
         <v>3</v>
       </c>
@@ -6713,7 +6687,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="88" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A88" s="45" t="s">
         <v>3</v>
       </c>
@@ -6751,7 +6725,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="89" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A89" s="45" t="s">
         <v>3</v>
       </c>
@@ -6789,7 +6763,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="90" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A90" s="45" t="s">
         <v>3</v>
       </c>
@@ -6827,7 +6801,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="91" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A91" s="45" t="s">
         <v>3</v>
       </c>
@@ -6865,7 +6839,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="92" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A92" s="45" t="s">
         <v>3</v>
       </c>
@@ -6941,7 +6915,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="94" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A94" s="45" t="s">
         <v>3</v>
       </c>
@@ -6979,7 +6953,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="95" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A95" s="45" t="s">
         <v>3</v>
       </c>
@@ -7017,7 +6991,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="96" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A96" s="45" t="s">
         <v>3</v>
       </c>
@@ -7055,7 +7029,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="97" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A97" s="45" t="s">
         <v>3</v>
       </c>
@@ -7093,7 +7067,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="98" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A98" s="45" t="s">
         <v>3</v>
       </c>
@@ -7131,7 +7105,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="99" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A99" s="45" t="s">
         <v>3</v>
       </c>
@@ -7169,7 +7143,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="100" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A100" s="45" t="s">
         <v>3</v>
       </c>
@@ -7207,7 +7181,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="101" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A101" s="45" t="s">
         <v>3</v>
       </c>
@@ -7245,7 +7219,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="102" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A102" s="45" t="s">
         <v>3</v>
       </c>
@@ -7283,7 +7257,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="103" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A103" s="45" t="s">
         <v>3</v>
       </c>
@@ -7397,7 +7371,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="106" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A106" s="99" t="s">
         <v>3</v>
       </c>
@@ -7435,7 +7409,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="107" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A107" s="99" t="s">
         <v>3</v>
       </c>
@@ -7511,7 +7485,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="109" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A109" s="99" t="s">
         <v>3</v>
       </c>
@@ -7549,7 +7523,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="110" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A110" s="99" t="s">
         <v>3</v>
       </c>
@@ -7587,7 +7561,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="111" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A111" s="99" t="s">
         <v>3</v>
       </c>
@@ -7625,7 +7599,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="112" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A112" s="99" t="s">
         <v>3</v>
       </c>
@@ -7739,7 +7713,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="115" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A115" s="77" t="s">
         <v>3</v>
       </c>
@@ -7815,7 +7789,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="117" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A117" s="111" t="s">
         <v>3</v>
       </c>
@@ -7853,7 +7827,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="118" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A118" s="114" t="s">
         <v>3</v>
       </c>
@@ -7889,7 +7863,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="119" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A119" s="111" t="s">
         <v>3</v>
       </c>
@@ -7927,7 +7901,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="120" spans="1:12" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A120" s="111" t="s">
         <v>3</v>
       </c>
@@ -7965,7 +7939,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="121" spans="1:12" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A121" s="119" t="s">
         <v>3</v>
       </c>
@@ -8001,7 +7975,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A122" s="111" t="s">
         <v>3</v>
       </c>
@@ -8039,7 +8013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A123" s="111" t="s">
         <v>3</v>
       </c>
@@ -8113,7 +8087,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A125" s="15" t="s">
         <v>3</v>
       </c>
@@ -8151,7 +8125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A126" s="15" t="s">
         <v>3</v>
       </c>
@@ -8187,7 +8161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A127" s="24" t="s">
         <v>3</v>
       </c>
@@ -8223,7 +8197,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A128" s="15" t="s">
         <v>3</v>
       </c>
@@ -8259,7 +8233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A129" s="15" t="s">
         <v>3</v>
       </c>
@@ -8295,7 +8269,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A130" s="111" t="s">
         <v>3</v>
       </c>
@@ -8329,7 +8303,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A131" s="111" t="s">
         <v>3</v>
       </c>
@@ -8365,7 +8339,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A132" s="111" t="s">
         <v>3</v>
       </c>
@@ -8399,7 +8373,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A133" s="45" t="s">
         <v>3</v>
       </c>
@@ -8433,7 +8407,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A134" s="45" t="s">
         <v>3</v>
       </c>
@@ -8469,7 +8443,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A135" s="45" t="s">
         <v>3</v>
       </c>
@@ -8503,7 +8477,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A136" s="45" t="s">
         <v>3</v>
       </c>
@@ -8539,7 +8513,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A137" s="111" t="s">
         <v>3</v>
       </c>
@@ -8573,7 +8547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A138" s="111" t="s">
         <v>3</v>
       </c>
@@ -8611,7 +8585,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:12" s="156" customFormat="1" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:12" s="156" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A139" s="146" t="s">
         <v>3</v>
       </c>
@@ -8645,7 +8619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A140" s="141" t="s">
         <v>3</v>
       </c>
@@ -8681,7 +8655,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="141" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" s="141" t="s">
         <v>3</v>
       </c>
@@ -8757,7 +8731,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="143" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="45" t="s">
         <v>3</v>
       </c>
@@ -8833,7 +8807,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="145" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" s="45" t="s">
         <v>3</v>
       </c>
@@ -8981,8 +8955,8 @@
       <c r="K148" s="32" t="s">
         <v>225</v>
       </c>
-      <c r="L148" s="72">
-        <v>2</v>
+      <c r="L148" s="131">
+        <v>3</v>
       </c>
     </row>
     <row r="149" spans="1:12" x14ac:dyDescent="0.25">
@@ -9025,9 +8999,7 @@
       </c>
     </row>
     <row r="150" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A150" s="45" t="s">
-        <v>3</v>
-      </c>
+      <c r="A150" s="45"/>
       <c r="B150" s="115" t="s">
         <v>558</v>
       </c>
@@ -9056,7 +9028,7 @@
         <v>306</v>
       </c>
       <c r="K150" s="20" t="s">
-        <v>307</v>
+        <v>281</v>
       </c>
       <c r="L150" s="164">
         <v>3</v>

</xml_diff>

<commit_message>
BABY POWER UP GENEROUS HUMANOIDS
Former-commit-id: 9c6833b9d2750684ae2b63776490c481530542fd
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Powerups.xlsx
+++ b/Docs/Content/HungryDragonContent_Powerups.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1455" uniqueCount="573">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1455" uniqueCount="575">
   <si>
     <t>[sku]</t>
   </si>
@@ -1743,6 +1743,12 @@
   </si>
   <si>
     <t>disguise_boost_LOW_fury_duration_LOW_Steam</t>
+  </si>
+  <si>
+    <t>TID_POWERUP_PREY_HP_BOOST_HUMANOIDS_NAME</t>
+  </si>
+  <si>
+    <t>TID_POWERUP_PREY_HP_BOOST_HUMANOIDS_DESC_SHORT</t>
   </si>
 </sst>
 </file>
@@ -3575,8 +3581,8 @@
   </sheetPr>
   <dimension ref="A1:L155"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
-      <selection activeCell="A150" sqref="A150"/>
+    <sheetView tabSelected="1" topLeftCell="F109" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
+      <selection activeCell="J141" sqref="J141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8039,13 +8045,13 @@
         <v>37</v>
       </c>
       <c r="I123" s="128" t="s">
-        <v>346</v>
+        <v>573</v>
       </c>
       <c r="J123" s="129" t="s">
-        <v>347</v>
+        <v>573</v>
       </c>
       <c r="K123" s="130" t="s">
-        <v>348</v>
+        <v>574</v>
       </c>
       <c r="L123" s="131">
         <v>0</v>

</xml_diff>

<commit_message>
Jade Skins powers definition
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Powerups.xlsx
+++ b/Docs/Content/HungryDragonContent_Powerups.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\client\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\client_lfs\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1595" uniqueCount="600">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1628" uniqueCount="612">
   <si>
     <t>[sku]</t>
   </si>
@@ -1824,6 +1824,42 @@
   </si>
   <si>
     <t>disguise_transform_gold_LOWx2,5_boost_fury_duration_LOW</t>
+  </si>
+  <si>
+    <t>TID_POWERUP_DISGUISE_51_NAME</t>
+  </si>
+  <si>
+    <t>TID_POWERUP_DISGUISE_51_DESC</t>
+  </si>
+  <si>
+    <t>TID_POWERUP_DISGUISE_51_DESC_SHORT</t>
+  </si>
+  <si>
+    <t>TID_POWERUP_DISGUISE_52_NAME</t>
+  </si>
+  <si>
+    <t>TID_POWERUP_DISGUISE_53_NAME</t>
+  </si>
+  <si>
+    <t>TID_POWERUP_DISGUISE_52_DESC</t>
+  </si>
+  <si>
+    <t>TID_POWERUP_DISGUISE_53_DESC</t>
+  </si>
+  <si>
+    <t>TID_POWERUP_DISGUISE_52_DESC_SHORT</t>
+  </si>
+  <si>
+    <t>TID_POWERUP_DISGUISE_53_DESC_SHORT</t>
+  </si>
+  <si>
+    <t>disguise_boost_LOW_faster_boost</t>
+  </si>
+  <si>
+    <t>disguise_speed_LOW_boost_LOW_free_revive</t>
+  </si>
+  <si>
+    <t>disguise_speed_fury_duration_LOW</t>
   </si>
 </sst>
 </file>
@@ -2270,7 +2306,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="169">
+  <cellXfs count="170">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2756,6 +2792,7 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3375,8 +3412,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="powerUpsDefinitions2" displayName="powerUpsDefinitions2" ref="A3:L164" totalsRowShown="0" headerRowDxfId="28" dataDxfId="26" headerRowBorderDxfId="27" tableBorderDxfId="25" totalsRowBorderDxfId="24">
-  <autoFilter ref="A3:L164"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="powerUpsDefinitions2" displayName="powerUpsDefinitions2" ref="A3:L167" totalsRowShown="0" headerRowDxfId="28" dataDxfId="26" headerRowBorderDxfId="27" tableBorderDxfId="25" totalsRowBorderDxfId="24">
+  <autoFilter ref="A3:L167"/>
   <tableColumns count="12">
     <tableColumn id="1" name="{powerUpsDefinitions}" dataDxfId="23" totalsRowDxfId="22"/>
     <tableColumn id="2" name="[sku]" dataDxfId="21" totalsRowDxfId="20"/>
@@ -3669,10 +3706,10 @@
   <sheetPr>
     <tabColor theme="7"/>
   </sheetPr>
-  <dimension ref="A1:L169"/>
+  <dimension ref="A1:L173"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A119" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
-      <selection activeCell="B159" sqref="B159"/>
+    <sheetView tabSelected="1" topLeftCell="A136" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
+      <selection activeCell="B167" sqref="B167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6863,7 +6900,7 @@
       <c r="A90" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="B90" s="80" t="s">
+      <c r="B90" s="21" t="s">
         <v>153</v>
       </c>
       <c r="C90" s="70" t="s">
@@ -7997,7 +8034,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="120" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A120" s="111" t="s">
         <v>3</v>
       </c>
@@ -9646,50 +9683,164 @@
         <v>2</v>
       </c>
     </row>
-    <row r="165" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="166" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A166" s="1" t="s">
+    <row r="165" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A165" s="45" t="s">
+        <v>3</v>
+      </c>
+      <c r="B165" s="21" t="s">
+        <v>609</v>
+      </c>
+      <c r="C165" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="D165" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="E165" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="F165" s="23" t="s">
+        <v>578</v>
+      </c>
+      <c r="G165" s="46" t="s">
+        <v>141</v>
+      </c>
+      <c r="H165" s="46" t="s">
+        <v>33</v>
+      </c>
+      <c r="I165" s="47" t="s">
+        <v>600</v>
+      </c>
+      <c r="J165" s="48" t="s">
+        <v>601</v>
+      </c>
+      <c r="K165" s="49" t="s">
+        <v>602</v>
+      </c>
+      <c r="L165" s="66">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="166" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A166" s="45" t="s">
+        <v>3</v>
+      </c>
+      <c r="B166" s="21" t="s">
+        <v>611</v>
+      </c>
+      <c r="C166" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="D166" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="E166" s="23" t="s">
+        <v>149</v>
+      </c>
+      <c r="F166" s="23" t="s">
+        <v>169</v>
+      </c>
+      <c r="G166" s="46" t="s">
+        <v>141</v>
+      </c>
+      <c r="H166" s="46" t="s">
+        <v>33</v>
+      </c>
+      <c r="I166" s="47" t="s">
+        <v>603</v>
+      </c>
+      <c r="J166" s="48" t="s">
+        <v>605</v>
+      </c>
+      <c r="K166" s="49" t="s">
+        <v>607</v>
+      </c>
+      <c r="L166" s="66">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="167" spans="1:12" s="169" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A167" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="B167" s="25" t="s">
+        <v>610</v>
+      </c>
+      <c r="C167" s="26" t="s">
+        <v>95</v>
+      </c>
+      <c r="D167" s="26" t="s">
+        <v>98</v>
+      </c>
+      <c r="E167" s="27" t="s">
+        <v>539</v>
+      </c>
+      <c r="F167" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="G167" s="28" t="s">
+        <v>141</v>
+      </c>
+      <c r="H167" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="I167" s="19" t="s">
+        <v>604</v>
+      </c>
+      <c r="J167" s="20" t="s">
+        <v>606</v>
+      </c>
+      <c r="K167" s="29" t="s">
+        <v>608</v>
+      </c>
+      <c r="L167" s="64">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="169" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="170" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A170" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B166" s="1"/>
-      <c r="C166" s="1"/>
-      <c r="D166" s="1"/>
-      <c r="E166" s="1"/>
-      <c r="F166" s="1"/>
-      <c r="G166" s="1"/>
-      <c r="H166" s="1"/>
-    </row>
-    <row r="168" spans="1:12" ht="136.5" x14ac:dyDescent="0.25">
-      <c r="A168" s="2" t="s">
+      <c r="B170" s="1"/>
+      <c r="C170" s="1"/>
+      <c r="D170" s="1"/>
+      <c r="E170" s="1"/>
+      <c r="F170" s="1"/>
+      <c r="G170" s="1"/>
+      <c r="H170" s="1"/>
+    </row>
+    <row r="172" spans="1:12" ht="136.5" x14ac:dyDescent="0.25">
+      <c r="A172" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="B168" s="2" t="s">
+      <c r="B172" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C168" s="50" t="s">
+      <c r="C172" s="50" t="s">
         <v>88</v>
       </c>
-      <c r="D168" s="51" t="s">
+      <c r="D172" s="51" t="s">
         <v>89</v>
       </c>
-      <c r="E168" s="51" t="s">
+      <c r="E172" s="51" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="169" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A169" s="52" t="s">
-        <v>3</v>
-      </c>
-      <c r="B169" s="4" t="s">
+    <row r="173" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A173" s="52" t="s">
+        <v>3</v>
+      </c>
+      <c r="B173" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="C169" s="3">
+      <c r="C173" s="3">
         <v>11</v>
       </c>
-      <c r="D169" s="5">
+      <c r="D173" s="5">
         <v>2.2999999999999998</v>
       </c>
-      <c r="E169" s="5">
+      <c r="E173" s="5">
         <v>0.25</v>
       </c>
     </row>

</xml_diff>